<commit_message>
fuck I spend too much these days
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="221">
   <si>
     <t>Ημερομηνία</t>
   </si>
@@ -671,6 +671,15 @@
   </si>
   <si>
     <t>burger στο BurgerVill</t>
+  </si>
+  <si>
+    <t>moschato dusty (Χ2)</t>
+  </si>
+  <si>
+    <t>ταξί τα ξυμερώματα</t>
+  </si>
+  <si>
+    <t>πρωινό μετά από προπόνηση</t>
   </si>
 </sst>
 </file>
@@ -901,24 +910,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="154653440"/>
-        <c:axId val="154654976"/>
+        <c:axId val="146457728"/>
+        <c:axId val="146459264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154653440"/>
+        <c:axId val="146457728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154654976"/>
+        <c:crossAx val="146459264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154654976"/>
+        <c:axId val="146459264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -926,7 +935,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154653440"/>
+        <c:crossAx val="146457728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -988,7 +997,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1116,24 +1125,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="154596864"/>
-        <c:axId val="154598400"/>
+        <c:axId val="146397056"/>
+        <c:axId val="146398592"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154596864"/>
+        <c:axId val="146397056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154598400"/>
+        <c:crossAx val="146398592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154598400"/>
+        <c:axId val="146398592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1141,7 +1150,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154596864"/>
+        <c:crossAx val="146397056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1150,7 +1159,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1205,24 +1214,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="156588288"/>
-        <c:axId val="156590080"/>
+        <c:axId val="147413632"/>
+        <c:axId val="147419520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="156588288"/>
+        <c:axId val="147413632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156590080"/>
+        <c:crossAx val="147419520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="156590080"/>
+        <c:axId val="147419520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1230,7 +1239,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156588288"/>
+        <c:crossAx val="147413632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1239,7 +1248,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1697,8 +1706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="H192" sqref="H192"/>
+    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="H195" sqref="H195"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6034,6 +6043,75 @@
         <v>81</v>
       </c>
     </row>
+    <row r="192" spans="1:8">
+      <c r="A192" s="8">
+        <v>14</v>
+      </c>
+      <c r="B192" t="s">
+        <v>67</v>
+      </c>
+      <c r="C192" s="2">
+        <v>43240</v>
+      </c>
+      <c r="D192" t="s">
+        <v>218</v>
+      </c>
+      <c r="E192" t="s">
+        <v>78</v>
+      </c>
+      <c r="F192">
+        <v>5</v>
+      </c>
+      <c r="H192" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8">
+      <c r="A193" s="8">
+        <v>14</v>
+      </c>
+      <c r="B193" t="s">
+        <v>64</v>
+      </c>
+      <c r="C193" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D193" t="s">
+        <v>219</v>
+      </c>
+      <c r="E193" t="s">
+        <v>78</v>
+      </c>
+      <c r="F193">
+        <v>5</v>
+      </c>
+      <c r="H193" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8">
+      <c r="A194" s="9">
+        <v>4.7</v>
+      </c>
+      <c r="B194" t="s">
+        <v>67</v>
+      </c>
+      <c r="C194" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D194" t="s">
+        <v>220</v>
+      </c>
+      <c r="E194" t="s">
+        <v>78</v>
+      </c>
+      <c r="F194">
+        <v>5</v>
+      </c>
+      <c r="H194" t="s">
+        <v>164</v>
+      </c>
+    </row>
     <row r="366" spans="1:12">
       <c r="A366" s="1"/>
       <c r="B366" s="1"/>
@@ -6051,7 +6129,7 @@
     <row r="367" spans="1:12">
       <c r="A367" s="1">
         <f>SUBTOTAL(109,[Ποσό €])</f>
-        <v>2128.3799999999997</v>
+        <v>2161.0799999999995</v>
       </c>
       <c r="B367" s="1"/>
       <c r="C367" s="1"/>

</xml_diff>

<commit_message>
update cost, fuck my life
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="248">
   <si>
     <t>Ημερομηνία</t>
   </si>
@@ -746,6 +746,21 @@
   </si>
   <si>
     <t>burger cocacola</t>
+  </si>
+  <si>
+    <t>ταξί από την ανθούπολη</t>
+  </si>
+  <si>
+    <t>κοτόπουλο με λαχανικά</t>
+  </si>
+  <si>
+    <t>πρωινό, πίτσα και χυμός</t>
+  </si>
+  <si>
+    <t>1,5€</t>
+  </si>
+  <si>
+    <t>λεμονάδα από τα mikel</t>
   </si>
 </sst>
 </file>
@@ -976,24 +991,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="150328064"/>
-        <c:axId val="150329600"/>
+        <c:axId val="149607168"/>
+        <c:axId val="149608704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150328064"/>
+        <c:axId val="149607168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150329600"/>
+        <c:crossAx val="149608704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150329600"/>
+        <c:axId val="149608704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1001,7 +1016,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150328064"/>
+        <c:crossAx val="149607168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1063,7 +1078,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1191,24 +1206,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="150304256"/>
-        <c:axId val="150305792"/>
+        <c:axId val="149583360"/>
+        <c:axId val="149584896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="150304256"/>
+        <c:axId val="149583360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150305792"/>
+        <c:crossAx val="149584896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="150305792"/>
+        <c:axId val="149584896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1216,7 +1231,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="150304256"/>
+        <c:crossAx val="149583360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1225,7 +1240,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1280,24 +1295,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="151021824"/>
-        <c:axId val="151031808"/>
+        <c:axId val="150300928"/>
+        <c:axId val="150302720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151021824"/>
+        <c:axId val="150300928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151031808"/>
+        <c:crossAx val="150302720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151031808"/>
+        <c:axId val="150302720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1305,7 +1320,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151021824"/>
+        <c:crossAx val="150300928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1314,7 +1329,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1772,8 +1787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="D220" sqref="D220"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="D225" sqref="D225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6753,6 +6768,144 @@
         <v>81</v>
       </c>
     </row>
+    <row r="220" spans="1:8">
+      <c r="A220" s="8">
+        <v>5</v>
+      </c>
+      <c r="B220" t="s">
+        <v>64</v>
+      </c>
+      <c r="C220" s="2">
+        <v>43254</v>
+      </c>
+      <c r="D220" t="s">
+        <v>243</v>
+      </c>
+      <c r="E220" t="s">
+        <v>108</v>
+      </c>
+      <c r="F220">
+        <v>4</v>
+      </c>
+      <c r="H220" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8">
+      <c r="A221" s="8">
+        <v>5</v>
+      </c>
+      <c r="B221" t="s">
+        <v>67</v>
+      </c>
+      <c r="C221" s="2">
+        <v>43255</v>
+      </c>
+      <c r="D221" t="s">
+        <v>180</v>
+      </c>
+      <c r="E221" t="s">
+        <v>108</v>
+      </c>
+      <c r="F221">
+        <v>4</v>
+      </c>
+      <c r="H221" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8">
+      <c r="A222" s="9">
+        <v>4.7</v>
+      </c>
+      <c r="B222" t="s">
+        <v>67</v>
+      </c>
+      <c r="C222" s="2">
+        <v>43256</v>
+      </c>
+      <c r="D222" t="s">
+        <v>245</v>
+      </c>
+      <c r="E222" t="s">
+        <v>108</v>
+      </c>
+      <c r="F222">
+        <v>4</v>
+      </c>
+      <c r="H222" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8">
+      <c r="A223" s="8">
+        <v>5</v>
+      </c>
+      <c r="B223" t="s">
+        <v>67</v>
+      </c>
+      <c r="C223" s="2">
+        <v>43256</v>
+      </c>
+      <c r="D223" t="s">
+        <v>244</v>
+      </c>
+      <c r="E223" t="s">
+        <v>108</v>
+      </c>
+      <c r="F223">
+        <v>4</v>
+      </c>
+      <c r="H223" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8">
+      <c r="A224" s="8">
+        <v>10</v>
+      </c>
+      <c r="B224" t="s">
+        <v>65</v>
+      </c>
+      <c r="C224" s="2">
+        <v>43256</v>
+      </c>
+      <c r="D224" t="s">
+        <v>11</v>
+      </c>
+      <c r="E224" t="s">
+        <v>108</v>
+      </c>
+      <c r="F224">
+        <v>4</v>
+      </c>
+      <c r="H224" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8">
+      <c r="A225" t="s">
+        <v>246</v>
+      </c>
+      <c r="B225" t="s">
+        <v>67</v>
+      </c>
+      <c r="C225" s="2">
+        <v>43256</v>
+      </c>
+      <c r="D225" t="s">
+        <v>247</v>
+      </c>
+      <c r="E225" t="s">
+        <v>108</v>
+      </c>
+      <c r="F225">
+        <v>4</v>
+      </c>
+      <c r="H225" t="s">
+        <v>81</v>
+      </c>
+    </row>
     <row r="366" spans="1:12">
       <c r="A366" s="1"/>
       <c r="B366" s="1"/>
@@ -6770,7 +6923,7 @@
     <row r="367" spans="1:12">
       <c r="A367" s="1">
         <f>SUBTOTAL(109,[Ποσό €])</f>
-        <v>2441.09</v>
+        <v>2470.79</v>
       </c>
       <c r="B367" s="1"/>
       <c r="C367" s="1"/>

</xml_diff>

<commit_message>
added data to the database
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="266">
   <si>
     <t>Ημερομηνία</t>
   </si>
@@ -800,6 +800,21 @@
   </si>
   <si>
     <t>ταξί από τα village cinemas</t>
+  </si>
+  <si>
+    <t>σουβλάκια σκέτα (διατροφή)</t>
+  </si>
+  <si>
+    <t>παπούτσια addidas</t>
+  </si>
+  <si>
+    <t>writing tablet</t>
+  </si>
+  <si>
+    <t>δίπλωμα οδήγησης</t>
+  </si>
+  <si>
+    <t>πρωινό moccachino κουλούρι</t>
   </si>
 </sst>
 </file>
@@ -1030,24 +1045,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="153543808"/>
-        <c:axId val="153545344"/>
+        <c:axId val="126608128"/>
+        <c:axId val="126609664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153543808"/>
+        <c:axId val="126608128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153545344"/>
+        <c:crossAx val="126609664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153545344"/>
+        <c:axId val="126609664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1055,7 +1070,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153543808"/>
+        <c:crossAx val="126608128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1117,7 +1132,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1245,24 +1260,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="153507712"/>
-        <c:axId val="153509248"/>
+        <c:axId val="126592512"/>
+        <c:axId val="126594048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153507712"/>
+        <c:axId val="126592512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153509248"/>
+        <c:crossAx val="126594048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153509248"/>
+        <c:axId val="126594048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1270,7 +1285,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153507712"/>
+        <c:crossAx val="126592512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1279,7 +1294,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1334,24 +1349,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="154233472"/>
-        <c:axId val="154235264"/>
+        <c:axId val="157444352"/>
+        <c:axId val="157446144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154233472"/>
+        <c:axId val="157444352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154235264"/>
+        <c:crossAx val="157446144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154235264"/>
+        <c:axId val="157446144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1359,7 +1374,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154233472"/>
+        <c:crossAx val="157444352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1368,7 +1383,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1518,8 +1533,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A1:J367" totalsRowCount="1">
-  <autoFilter ref="A1:J366">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A1:J368" totalsRowCount="1">
+  <autoFilter ref="A1:J367">
     <filterColumn colId="1"/>
     <filterColumn colId="2"/>
   </autoFilter>
@@ -1824,10 +1839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L368"/>
+  <dimension ref="A1:L369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A218" workbookViewId="0">
-      <selection activeCell="C240" sqref="C240"/>
+    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="H151" sqref="H151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5199,7 +5214,7 @@
     </row>
     <row r="150" spans="1:8">
       <c r="A150" s="3">
-        <v>7</v>
+        <v>150</v>
       </c>
       <c r="B150" t="s">
         <v>68</v>
@@ -5208,7 +5223,7 @@
         <v>43211</v>
       </c>
       <c r="D150" t="s">
-        <v>174</v>
+        <v>264</v>
       </c>
       <c r="E150" t="s">
         <v>166</v>
@@ -5222,16 +5237,16 @@
     </row>
     <row r="151" spans="1:8">
       <c r="A151" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B151" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C151" s="2">
         <v>43211</v>
       </c>
       <c r="D151" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E151" t="s">
         <v>166</v>
@@ -5240,12 +5255,12 @@
         <v>5</v>
       </c>
       <c r="H151" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
     </row>
     <row r="152" spans="1:8">
       <c r="A152" s="3">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B152" t="s">
         <v>67</v>
@@ -5254,7 +5269,7 @@
         <v>43211</v>
       </c>
       <c r="D152" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E152" t="s">
         <v>166</v>
@@ -5267,17 +5282,17 @@
       </c>
     </row>
     <row r="153" spans="1:8">
-      <c r="A153" s="7">
-        <v>3.5</v>
+      <c r="A153" s="3">
+        <v>8</v>
       </c>
       <c r="B153" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C153" s="2">
         <v>43211</v>
       </c>
       <c r="D153" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E153" t="s">
         <v>166</v>
@@ -5286,21 +5301,21 @@
         <v>5</v>
       </c>
       <c r="H153" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
     </row>
     <row r="154" spans="1:8">
-      <c r="A154" s="8">
-        <v>55</v>
+      <c r="A154" s="7">
+        <v>3.5</v>
       </c>
       <c r="B154" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C154" s="2">
-        <v>43213</v>
+        <v>43211</v>
       </c>
       <c r="D154" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E154" t="s">
         <v>166</v>
@@ -5313,17 +5328,17 @@
       </c>
     </row>
     <row r="155" spans="1:8">
-      <c r="A155" s="9">
-        <v>0.6</v>
+      <c r="A155" s="8">
+        <v>55</v>
       </c>
       <c r="B155" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C155" s="2">
         <v>43213</v>
       </c>
       <c r="D155" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E155" t="s">
         <v>166</v>
@@ -5332,21 +5347,21 @@
         <v>5</v>
       </c>
       <c r="H155" t="s">
-        <v>164</v>
+        <v>81</v>
       </c>
     </row>
     <row r="156" spans="1:8">
-      <c r="A156" s="8">
-        <v>4</v>
+      <c r="A156" s="9">
+        <v>0.6</v>
       </c>
       <c r="B156" t="s">
         <v>67</v>
       </c>
       <c r="C156" s="2">
-        <v>43214</v>
+        <v>43213</v>
       </c>
       <c r="D156" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E156" t="s">
         <v>166</v>
@@ -5359,17 +5374,17 @@
       </c>
     </row>
     <row r="157" spans="1:8">
-      <c r="A157" s="9">
-        <v>39.9</v>
+      <c r="A157" s="8">
+        <v>4</v>
       </c>
       <c r="B157" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C157" s="2">
-        <v>43216</v>
+        <v>43214</v>
       </c>
       <c r="D157" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E157" t="s">
         <v>166</v>
@@ -5378,21 +5393,21 @@
         <v>5</v>
       </c>
       <c r="H157" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
     </row>
     <row r="158" spans="1:8">
       <c r="A158" s="9">
-        <v>1.6</v>
+        <v>39.9</v>
       </c>
       <c r="B158" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C158" s="2">
         <v>43216</v>
       </c>
       <c r="D158" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E158" t="s">
         <v>166</v>
@@ -5401,21 +5416,21 @@
         <v>5</v>
       </c>
       <c r="H158" t="s">
-        <v>164</v>
+        <v>81</v>
       </c>
     </row>
     <row r="159" spans="1:8">
-      <c r="A159" s="8">
-        <v>80</v>
+      <c r="A159" s="9">
+        <v>1.6</v>
       </c>
       <c r="B159" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C159" s="2">
-        <v>43217</v>
+        <v>43216</v>
       </c>
       <c r="D159" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E159" t="s">
         <v>166</v>
@@ -5424,21 +5439,21 @@
         <v>5</v>
       </c>
       <c r="H159" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
     </row>
     <row r="160" spans="1:8">
-      <c r="A160" s="9">
-        <v>6.2</v>
+      <c r="A160" s="8">
+        <v>80</v>
       </c>
       <c r="B160" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C160" s="2">
         <v>43217</v>
       </c>
       <c r="D160" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E160" t="s">
         <v>166</v>
@@ -5447,21 +5462,21 @@
         <v>5</v>
       </c>
       <c r="H160" t="s">
-        <v>164</v>
+        <v>81</v>
       </c>
     </row>
     <row r="161" spans="1:8">
-      <c r="A161" s="8">
-        <v>15</v>
+      <c r="A161" s="9">
+        <v>6.2</v>
       </c>
       <c r="B161" t="s">
         <v>67</v>
       </c>
       <c r="C161" s="2">
-        <v>43218</v>
+        <v>43217</v>
       </c>
       <c r="D161" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E161" t="s">
         <v>166</v>
@@ -5470,12 +5485,12 @@
         <v>5</v>
       </c>
       <c r="H161" t="s">
-        <v>86</v>
+        <v>164</v>
       </c>
     </row>
     <row r="162" spans="1:8">
-      <c r="A162" s="9">
-        <v>4.3</v>
+      <c r="A162" s="8">
+        <v>15</v>
       </c>
       <c r="B162" t="s">
         <v>67</v>
@@ -5484,7 +5499,7 @@
         <v>43218</v>
       </c>
       <c r="D162" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E162" t="s">
         <v>166</v>
@@ -5493,21 +5508,21 @@
         <v>5</v>
       </c>
       <c r="H162" t="s">
-        <v>164</v>
+        <v>86</v>
       </c>
     </row>
     <row r="163" spans="1:8">
       <c r="A163" s="9">
-        <v>9.6999999999999993</v>
+        <v>4.3</v>
       </c>
       <c r="B163" t="s">
         <v>67</v>
       </c>
       <c r="C163" s="2">
-        <v>43219</v>
+        <v>43218</v>
       </c>
       <c r="D163" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E163" t="s">
         <v>166</v>
@@ -5516,35 +5531,35 @@
         <v>5</v>
       </c>
       <c r="H163" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
     </row>
     <row r="164" spans="1:8">
       <c r="A164" s="9">
-        <v>2.4500000000000002</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="B164" t="s">
         <v>67</v>
       </c>
       <c r="C164" s="2">
-        <v>43220</v>
+        <v>43219</v>
       </c>
       <c r="D164" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E164" t="s">
         <v>166</v>
       </c>
       <c r="F164">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H164" t="s">
-        <v>147</v>
+        <v>81</v>
       </c>
     </row>
     <row r="165" spans="1:8">
       <c r="A165" s="9">
-        <v>1.96</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="B165" t="s">
         <v>67</v>
@@ -5553,7 +5568,7 @@
         <v>43220</v>
       </c>
       <c r="D165" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E165" t="s">
         <v>166</v>
@@ -5562,21 +5577,21 @@
         <v>4</v>
       </c>
       <c r="H165" t="s">
-        <v>187</v>
+        <v>147</v>
       </c>
     </row>
     <row r="166" spans="1:8">
       <c r="A166" s="9">
-        <v>11.5</v>
+        <v>1.96</v>
       </c>
       <c r="B166" t="s">
         <v>67</v>
       </c>
       <c r="C166" s="2">
-        <v>43221</v>
+        <v>43220</v>
       </c>
       <c r="D166" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E166" t="s">
         <v>166</v>
@@ -5585,21 +5600,21 @@
         <v>4</v>
       </c>
       <c r="H166" t="s">
-        <v>85</v>
+        <v>187</v>
       </c>
     </row>
     <row r="167" spans="1:8">
       <c r="A167" s="9">
-        <v>2.7</v>
+        <v>11.5</v>
       </c>
       <c r="B167" t="s">
         <v>67</v>
       </c>
       <c r="C167" s="2">
-        <v>43223</v>
+        <v>43221</v>
       </c>
       <c r="D167" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E167" t="s">
         <v>166</v>
@@ -5608,7 +5623,7 @@
         <v>4</v>
       </c>
       <c r="H167" t="s">
-        <v>187</v>
+        <v>85</v>
       </c>
     </row>
     <row r="168" spans="1:8">
@@ -5619,33 +5634,33 @@
         <v>67</v>
       </c>
       <c r="C168" s="2">
-        <v>43224</v>
+        <v>43223</v>
       </c>
       <c r="D168" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E168" t="s">
         <v>166</v>
       </c>
       <c r="F168">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H168" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
     </row>
     <row r="169" spans="1:8">
-      <c r="A169" s="8">
-        <v>7</v>
+      <c r="A169" s="9">
+        <v>2.7</v>
       </c>
       <c r="B169" t="s">
         <v>67</v>
       </c>
       <c r="C169" s="2">
-        <v>43225</v>
+        <v>43224</v>
       </c>
       <c r="D169" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E169" t="s">
         <v>166</v>
@@ -5654,21 +5669,21 @@
         <v>5</v>
       </c>
       <c r="H169" t="s">
-        <v>195</v>
+        <v>164</v>
       </c>
     </row>
     <row r="170" spans="1:8">
-      <c r="A170" s="9">
-        <v>4.8</v>
+      <c r="A170" s="8">
+        <v>7</v>
       </c>
       <c r="B170" t="s">
         <v>67</v>
       </c>
       <c r="C170" s="2">
-        <v>43227</v>
+        <v>43225</v>
       </c>
       <c r="D170" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E170" t="s">
         <v>166</v>
@@ -5677,12 +5692,12 @@
         <v>5</v>
       </c>
       <c r="H170" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="171" spans="1:8">
       <c r="A171" s="9">
-        <v>4.4000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="B171" t="s">
         <v>67</v>
@@ -5691,7 +5706,7 @@
         <v>43227</v>
       </c>
       <c r="D171" t="s">
-        <v>155</v>
+        <v>196</v>
       </c>
       <c r="E171" t="s">
         <v>166</v>
@@ -5700,21 +5715,21 @@
         <v>5</v>
       </c>
       <c r="H171" t="s">
-        <v>81</v>
+        <v>187</v>
       </c>
     </row>
     <row r="172" spans="1:8">
       <c r="A172" s="9">
-        <v>3.8</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B172" t="s">
         <v>67</v>
       </c>
       <c r="C172" s="2">
-        <v>43228</v>
+        <v>43227</v>
       </c>
       <c r="D172" t="s">
-        <v>197</v>
+        <v>155</v>
       </c>
       <c r="E172" t="s">
         <v>166</v>
@@ -5723,35 +5738,35 @@
         <v>5</v>
       </c>
       <c r="H172" t="s">
-        <v>187</v>
+        <v>81</v>
       </c>
     </row>
     <row r="173" spans="1:8">
       <c r="A173" s="9">
-        <v>1.5</v>
+        <v>3.8</v>
       </c>
       <c r="B173" t="s">
         <v>67</v>
       </c>
       <c r="C173" s="2">
-        <v>43229</v>
+        <v>43228</v>
       </c>
       <c r="D173" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E173" t="s">
-        <v>108</v>
+        <v>166</v>
       </c>
       <c r="F173">
         <v>5</v>
       </c>
       <c r="H173" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
     </row>
     <row r="174" spans="1:8">
       <c r="A174" s="9">
-        <v>11.5</v>
+        <v>1.5</v>
       </c>
       <c r="B174" t="s">
         <v>67</v>
@@ -5760,7 +5775,7 @@
         <v>43229</v>
       </c>
       <c r="D174" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E174" t="s">
         <v>108</v>
@@ -5769,21 +5784,21 @@
         <v>5</v>
       </c>
       <c r="H174" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
     </row>
     <row r="175" spans="1:8">
       <c r="A175" s="9">
-        <v>4.4000000000000004</v>
+        <v>11.5</v>
       </c>
       <c r="B175" t="s">
         <v>67</v>
       </c>
       <c r="C175" s="2">
-        <v>43230</v>
+        <v>43229</v>
       </c>
       <c r="D175" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E175" t="s">
         <v>108</v>
@@ -5797,16 +5812,16 @@
     </row>
     <row r="176" spans="1:8">
       <c r="A176" s="9">
-        <v>6.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="B176" t="s">
         <v>67</v>
       </c>
       <c r="C176" s="2">
-        <v>43233</v>
+        <v>43230</v>
       </c>
       <c r="D176" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E176" t="s">
         <v>108</v>
@@ -5815,7 +5830,7 @@
         <v>5</v>
       </c>
       <c r="H176" t="s">
-        <v>202</v>
+        <v>81</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -5829,76 +5844,76 @@
         <v>43233</v>
       </c>
       <c r="D177" t="s">
+        <v>201</v>
+      </c>
+      <c r="E177" t="s">
+        <v>108</v>
+      </c>
+      <c r="F177">
+        <v>5</v>
+      </c>
+      <c r="H177" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8">
+      <c r="A178" s="9">
+        <v>6.5</v>
+      </c>
+      <c r="B178" t="s">
+        <v>67</v>
+      </c>
+      <c r="C178" s="2">
+        <v>43233</v>
+      </c>
+      <c r="D178" t="s">
         <v>203</v>
       </c>
-      <c r="E177" t="s">
-        <v>108</v>
-      </c>
-      <c r="F177">
-        <v>5</v>
-      </c>
-      <c r="H177" t="s">
+      <c r="E178" t="s">
+        <v>108</v>
+      </c>
+      <c r="F178">
+        <v>5</v>
+      </c>
+      <c r="H178" t="s">
         <v>204</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8">
-      <c r="A178" s="8">
-        <v>5</v>
-      </c>
-      <c r="B178" t="s">
-        <v>67</v>
-      </c>
-      <c r="C178" s="2">
-        <v>43234</v>
-      </c>
-      <c r="D178" t="s">
-        <v>180</v>
-      </c>
-      <c r="E178" t="s">
-        <v>205</v>
-      </c>
-      <c r="F178">
-        <v>3</v>
-      </c>
-      <c r="H178" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="179" spans="1:8">
       <c r="A179" s="8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B179" t="s">
         <v>67</v>
       </c>
       <c r="C179" s="2">
-        <v>43236</v>
+        <v>43234</v>
       </c>
       <c r="D179" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="E179" t="s">
         <v>205</v>
       </c>
       <c r="F179">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H179" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
     </row>
     <row r="180" spans="1:8">
       <c r="A180" s="8">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B180" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C180" s="2">
         <v>43236</v>
       </c>
       <c r="D180" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E180" t="s">
         <v>205</v>
@@ -5907,21 +5922,21 @@
         <v>4</v>
       </c>
       <c r="H180" t="s">
-        <v>81</v>
+        <v>187</v>
       </c>
     </row>
     <row r="181" spans="1:8">
-      <c r="A181" s="9">
-        <v>3.2</v>
+      <c r="A181" s="8">
+        <v>8</v>
       </c>
       <c r="B181" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C181" s="2">
-        <v>43237</v>
+        <v>43236</v>
       </c>
       <c r="D181" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E181" t="s">
         <v>205</v>
@@ -5930,35 +5945,35 @@
         <v>4</v>
       </c>
       <c r="H181" t="s">
-        <v>147</v>
+        <v>81</v>
       </c>
     </row>
     <row r="182" spans="1:8">
-      <c r="A182" s="8">
-        <v>10</v>
+      <c r="A182" s="9">
+        <v>3.2</v>
       </c>
       <c r="B182" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C182" s="2">
         <v>43237</v>
       </c>
       <c r="D182" t="s">
-        <v>150</v>
+        <v>208</v>
       </c>
       <c r="E182" t="s">
         <v>205</v>
       </c>
       <c r="F182">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H182" t="s">
-        <v>187</v>
+        <v>147</v>
       </c>
     </row>
     <row r="183" spans="1:8">
       <c r="A183" s="8">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B183" t="s">
         <v>68</v>
@@ -5967,7 +5982,7 @@
         <v>43237</v>
       </c>
       <c r="D183" t="s">
-        <v>214</v>
+        <v>150</v>
       </c>
       <c r="E183" t="s">
         <v>205</v>
@@ -5976,12 +5991,12 @@
         <v>5</v>
       </c>
       <c r="H183" t="s">
-        <v>81</v>
+        <v>187</v>
       </c>
     </row>
     <row r="184" spans="1:8">
       <c r="A184" s="8">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B184" t="s">
         <v>68</v>
@@ -5990,7 +6005,7 @@
         <v>43237</v>
       </c>
       <c r="D184" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="E184" t="s">
         <v>205</v>
@@ -6003,17 +6018,17 @@
       </c>
     </row>
     <row r="185" spans="1:8">
-      <c r="A185" s="9">
-        <v>3.5</v>
+      <c r="A185" s="8">
+        <v>10</v>
       </c>
       <c r="B185" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C185" s="2">
         <v>43237</v>
       </c>
       <c r="D185" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E185" t="s">
         <v>205</v>
@@ -6022,21 +6037,21 @@
         <v>5</v>
       </c>
       <c r="H185" t="s">
-        <v>187</v>
+        <v>81</v>
       </c>
     </row>
     <row r="186" spans="1:8">
-      <c r="A186" s="8">
-        <v>10</v>
+      <c r="A186" s="9">
+        <v>3.5</v>
       </c>
       <c r="B186" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C186" s="2">
         <v>43237</v>
       </c>
       <c r="D186" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E186" t="s">
         <v>205</v>
@@ -6045,21 +6060,21 @@
         <v>5</v>
       </c>
       <c r="H186" t="s">
-        <v>81</v>
+        <v>187</v>
       </c>
     </row>
     <row r="187" spans="1:8">
       <c r="A187" s="8">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B187" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C187" s="2">
-        <v>43238</v>
+        <v>43237</v>
       </c>
       <c r="D187" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E187" t="s">
         <v>205</v>
@@ -6068,21 +6083,21 @@
         <v>5</v>
       </c>
       <c r="H187" t="s">
-        <v>187</v>
+        <v>81</v>
       </c>
     </row>
     <row r="188" spans="1:8">
-      <c r="A188" s="9">
-        <v>6.2</v>
+      <c r="A188" s="8">
+        <v>8</v>
       </c>
       <c r="B188" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C188" s="2">
         <v>43238</v>
       </c>
       <c r="D188" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E188" t="s">
         <v>205</v>
@@ -6091,21 +6106,21 @@
         <v>5</v>
       </c>
       <c r="H188" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
     </row>
     <row r="189" spans="1:8">
-      <c r="A189" s="8">
-        <v>2</v>
+      <c r="A189" s="9">
+        <v>6.2</v>
       </c>
       <c r="B189" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C189" s="2">
-        <v>43239</v>
+        <v>43238</v>
       </c>
       <c r="D189" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E189" t="s">
         <v>205</v>
@@ -6119,16 +6134,16 @@
     </row>
     <row r="190" spans="1:8">
       <c r="A190" s="8">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B190" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C190" s="2">
         <v>43239</v>
       </c>
       <c r="D190" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E190" t="s">
         <v>205</v>
@@ -6137,27 +6152,27 @@
         <v>5</v>
       </c>
       <c r="H190" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
     </row>
     <row r="191" spans="1:8">
       <c r="A191" s="8">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B191" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C191" s="2">
         <v>43239</v>
       </c>
       <c r="D191" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E191" t="s">
         <v>205</v>
       </c>
       <c r="F191">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H191" t="s">
         <v>81</v>
@@ -6165,25 +6180,25 @@
     </row>
     <row r="192" spans="1:8">
       <c r="A192" s="8">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B192" t="s">
         <v>67</v>
       </c>
       <c r="C192" s="2">
-        <v>43240</v>
+        <v>43239</v>
       </c>
       <c r="D192" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E192" t="s">
-        <v>78</v>
+        <v>205</v>
       </c>
       <c r="F192">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H192" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="193" spans="1:8">
@@ -6191,36 +6206,36 @@
         <v>14</v>
       </c>
       <c r="B193" t="s">
+        <v>67</v>
+      </c>
+      <c r="C193" s="2">
+        <v>43240</v>
+      </c>
+      <c r="D193" t="s">
+        <v>218</v>
+      </c>
+      <c r="E193" t="s">
+        <v>78</v>
+      </c>
+      <c r="F193">
+        <v>5</v>
+      </c>
+      <c r="H193" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8">
+      <c r="A194" s="8">
+        <v>14</v>
+      </c>
+      <c r="B194" t="s">
         <v>64</v>
-      </c>
-      <c r="C193" s="2">
-        <v>43241</v>
-      </c>
-      <c r="D193" t="s">
-        <v>219</v>
-      </c>
-      <c r="E193" t="s">
-        <v>78</v>
-      </c>
-      <c r="F193">
-        <v>5</v>
-      </c>
-      <c r="H193" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="194" spans="1:8">
-      <c r="A194" s="9">
-        <v>4.7</v>
-      </c>
-      <c r="B194" t="s">
-        <v>67</v>
       </c>
       <c r="C194" s="2">
         <v>43241</v>
       </c>
       <c r="D194" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E194" t="s">
         <v>78</v>
@@ -6229,21 +6244,21 @@
         <v>5</v>
       </c>
       <c r="H194" t="s">
-        <v>164</v>
+        <v>81</v>
       </c>
     </row>
     <row r="195" spans="1:8">
       <c r="A195" s="9">
-        <v>69.900000000000006</v>
+        <v>4.7</v>
       </c>
       <c r="B195" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C195" s="2">
         <v>43241</v>
       </c>
       <c r="D195" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E195" t="s">
         <v>78</v>
@@ -6252,81 +6267,81 @@
         <v>5</v>
       </c>
       <c r="H195" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
     </row>
     <row r="196" spans="1:8">
       <c r="A196" s="9">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="B196" t="s">
+        <v>72</v>
+      </c>
+      <c r="C196" s="2">
+        <v>43241</v>
+      </c>
+      <c r="D196" t="s">
+        <v>221</v>
+      </c>
+      <c r="E196" t="s">
+        <v>78</v>
+      </c>
+      <c r="F196">
+        <v>5</v>
+      </c>
+      <c r="H196" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8">
+      <c r="A197" s="9">
         <v>8.4</v>
       </c>
-      <c r="B196" t="s">
-        <v>67</v>
-      </c>
-      <c r="C196" s="2">
+      <c r="B197" t="s">
+        <v>67</v>
+      </c>
+      <c r="C197" s="2">
         <v>43242</v>
       </c>
-      <c r="D196" t="s">
+      <c r="D197" t="s">
         <v>222</v>
       </c>
-      <c r="E196" t="s">
-        <v>78</v>
-      </c>
-      <c r="F196">
-        <v>4</v>
-      </c>
-      <c r="H196" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="197" spans="1:8">
-      <c r="A197" s="8">
-        <v>5</v>
-      </c>
-      <c r="B197" t="s">
-        <v>67</v>
-      </c>
-      <c r="C197" s="2">
+      <c r="E197" t="s">
+        <v>78</v>
+      </c>
+      <c r="F197">
+        <v>4</v>
+      </c>
+      <c r="H197" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8">
+      <c r="A198" s="8">
+        <v>5</v>
+      </c>
+      <c r="B198" t="s">
+        <v>67</v>
+      </c>
+      <c r="C198" s="2">
         <v>43243</v>
       </c>
-      <c r="D197" t="s">
+      <c r="D198" t="s">
         <v>223</v>
       </c>
-      <c r="E197" t="s">
-        <v>78</v>
-      </c>
-      <c r="F197">
-        <v>4</v>
-      </c>
-      <c r="H197" t="s">
+      <c r="E198" t="s">
+        <v>78</v>
+      </c>
+      <c r="F198">
+        <v>4</v>
+      </c>
+      <c r="H198" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
-      <c r="A198" s="9">
+    <row r="199" spans="1:8">
+      <c r="A199" s="9">
         <v>4.5</v>
-      </c>
-      <c r="B198" t="s">
-        <v>67</v>
-      </c>
-      <c r="C198" s="2">
-        <v>43244</v>
-      </c>
-      <c r="D198" t="s">
-        <v>224</v>
-      </c>
-      <c r="E198" t="s">
-        <v>78</v>
-      </c>
-      <c r="F198">
-        <v>4</v>
-      </c>
-      <c r="H198" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="199" spans="1:8">
-      <c r="A199" s="8">
-        <v>6</v>
       </c>
       <c r="B199" t="s">
         <v>67</v>
@@ -6335,77 +6350,77 @@
         <v>43244</v>
       </c>
       <c r="D199" t="s">
+        <v>224</v>
+      </c>
+      <c r="E199" t="s">
+        <v>78</v>
+      </c>
+      <c r="F199">
+        <v>4</v>
+      </c>
+      <c r="H199" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8">
+      <c r="A200" s="8">
+        <v>6</v>
+      </c>
+      <c r="B200" t="s">
+        <v>67</v>
+      </c>
+      <c r="C200" s="2">
+        <v>43244</v>
+      </c>
+      <c r="D200" t="s">
         <v>225</v>
       </c>
-      <c r="E199" t="s">
-        <v>78</v>
-      </c>
-      <c r="F199">
-        <v>4</v>
-      </c>
-      <c r="H199" t="s">
+      <c r="E200" t="s">
+        <v>78</v>
+      </c>
+      <c r="F200">
+        <v>4</v>
+      </c>
+      <c r="H200" t="s">
         <v>187</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8">
-      <c r="A200" s="9">
-        <v>5.46</v>
-      </c>
-      <c r="B200" t="s">
-        <v>67</v>
-      </c>
-      <c r="C200" s="2">
-        <v>43245</v>
-      </c>
-      <c r="D200" t="s">
-        <v>226</v>
-      </c>
-      <c r="E200" t="s">
-        <v>78</v>
-      </c>
-      <c r="F200">
-        <v>4</v>
-      </c>
-      <c r="H200" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="201" spans="1:8">
       <c r="A201" s="9">
-        <v>78.849999999999994</v>
+        <v>5.46</v>
       </c>
       <c r="B201" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C201" s="2">
         <v>43245</v>
       </c>
       <c r="D201" t="s">
+        <v>226</v>
+      </c>
+      <c r="E201" t="s">
+        <v>78</v>
+      </c>
+      <c r="F201">
+        <v>4</v>
+      </c>
+      <c r="H201" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8">
+      <c r="A202" s="9">
+        <v>78.849999999999994</v>
+      </c>
+      <c r="B202" t="s">
+        <v>69</v>
+      </c>
+      <c r="C202" s="2">
+        <v>43245</v>
+      </c>
+      <c r="D202" t="s">
         <v>229</v>
       </c>
-      <c r="E201" t="s">
-        <v>78</v>
-      </c>
-      <c r="F201">
-        <v>5</v>
-      </c>
-      <c r="H201" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8">
-      <c r="A202" s="8">
-        <v>10</v>
-      </c>
-      <c r="B202" t="s">
-        <v>67</v>
-      </c>
-      <c r="C202" s="2">
-        <v>43246</v>
-      </c>
-      <c r="D202" t="s">
-        <v>227</v>
-      </c>
       <c r="E202" t="s">
         <v>78</v>
       </c>
@@ -6413,7 +6428,7 @@
         <v>5</v>
       </c>
       <c r="H202" t="s">
-        <v>228</v>
+        <v>81</v>
       </c>
     </row>
     <row r="203" spans="1:8">
@@ -6421,13 +6436,13 @@
         <v>10</v>
       </c>
       <c r="B203" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C203" s="2">
         <v>43246</v>
       </c>
       <c r="D203" t="s">
-        <v>105</v>
+        <v>227</v>
       </c>
       <c r="E203" t="s">
         <v>78</v>
@@ -6436,35 +6451,35 @@
         <v>5</v>
       </c>
       <c r="H203" t="s">
-        <v>81</v>
+        <v>228</v>
       </c>
     </row>
     <row r="204" spans="1:8">
       <c r="A204" s="8">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B204" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C204" s="2">
-        <v>43247</v>
+        <v>43246</v>
       </c>
       <c r="D204" t="s">
-        <v>230</v>
+        <v>105</v>
       </c>
       <c r="E204" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="F204">
         <v>5</v>
       </c>
       <c r="H204" t="s">
-        <v>152</v>
+        <v>81</v>
       </c>
     </row>
     <row r="205" spans="1:8">
       <c r="A205" s="8">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B205" t="s">
         <v>67</v>
@@ -6473,7 +6488,7 @@
         <v>43247</v>
       </c>
       <c r="D205" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E205" t="s">
         <v>108</v>
@@ -6486,8 +6501,8 @@
       </c>
     </row>
     <row r="206" spans="1:8">
-      <c r="A206" s="9">
-        <v>2.5</v>
+      <c r="A206" s="8">
+        <v>2</v>
       </c>
       <c r="B206" t="s">
         <v>67</v>
@@ -6496,7 +6511,7 @@
         <v>43247</v>
       </c>
       <c r="D206" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E206" t="s">
         <v>108</v>
@@ -6505,35 +6520,35 @@
         <v>5</v>
       </c>
       <c r="H206" t="s">
-        <v>81</v>
+        <v>152</v>
       </c>
     </row>
     <row r="207" spans="1:8">
       <c r="A207" s="9">
-        <v>5.9</v>
+        <v>2.5</v>
       </c>
       <c r="B207" t="s">
         <v>67</v>
       </c>
       <c r="C207" s="2">
-        <v>43248</v>
+        <v>43247</v>
       </c>
       <c r="D207" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E207" t="s">
         <v>108</v>
       </c>
       <c r="F207">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H207" t="s">
-        <v>164</v>
+        <v>81</v>
       </c>
     </row>
     <row r="208" spans="1:8">
       <c r="A208" s="9">
-        <v>8.6</v>
+        <v>5.9</v>
       </c>
       <c r="B208" t="s">
         <v>67</v>
@@ -6542,7 +6557,7 @@
         <v>43248</v>
       </c>
       <c r="D208" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E208" t="s">
         <v>108</v>
@@ -6551,21 +6566,21 @@
         <v>4</v>
       </c>
       <c r="H208" t="s">
-        <v>81</v>
+        <v>164</v>
       </c>
     </row>
     <row r="209" spans="1:8">
       <c r="A209" s="9">
-        <v>2.7</v>
+        <v>8.6</v>
       </c>
       <c r="B209" t="s">
         <v>67</v>
       </c>
       <c r="C209" s="2">
-        <v>43249</v>
+        <v>43248</v>
       </c>
       <c r="D209" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E209" t="s">
         <v>108</v>
@@ -6574,21 +6589,21 @@
         <v>4</v>
       </c>
       <c r="H209" t="s">
-        <v>187</v>
+        <v>81</v>
       </c>
     </row>
     <row r="210" spans="1:8">
       <c r="A210" s="9">
-        <v>4.8</v>
+        <v>2.7</v>
       </c>
       <c r="B210" t="s">
         <v>67</v>
       </c>
       <c r="C210" s="2">
-        <v>43250</v>
+        <v>43249</v>
       </c>
       <c r="D210" t="s">
-        <v>155</v>
+        <v>235</v>
       </c>
       <c r="E210" t="s">
         <v>108</v>
@@ -6597,12 +6612,12 @@
         <v>4</v>
       </c>
       <c r="H210" t="s">
-        <v>81</v>
+        <v>187</v>
       </c>
     </row>
     <row r="211" spans="1:8">
       <c r="A211" s="9">
-        <v>2.8</v>
+        <v>4.8</v>
       </c>
       <c r="B211" t="s">
         <v>67</v>
@@ -6611,7 +6626,7 @@
         <v>43250</v>
       </c>
       <c r="D211" t="s">
-        <v>224</v>
+        <v>155</v>
       </c>
       <c r="E211" t="s">
         <v>108</v>
@@ -6620,12 +6635,12 @@
         <v>4</v>
       </c>
       <c r="H211" t="s">
-        <v>147</v>
+        <v>81</v>
       </c>
     </row>
     <row r="212" spans="1:8">
-      <c r="A212" s="8">
-        <v>2</v>
+      <c r="A212" s="9">
+        <v>2.8</v>
       </c>
       <c r="B212" t="s">
         <v>67</v>
@@ -6634,7 +6649,7 @@
         <v>43250</v>
       </c>
       <c r="D212" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="E212" t="s">
         <v>108</v>
@@ -6643,12 +6658,12 @@
         <v>4</v>
       </c>
       <c r="H212" t="s">
-        <v>81</v>
+        <v>147</v>
       </c>
     </row>
     <row r="213" spans="1:8">
       <c r="A213" s="8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B213" t="s">
         <v>67</v>
@@ -6657,7 +6672,7 @@
         <v>43250</v>
       </c>
       <c r="D213" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E213" t="s">
         <v>108</v>
@@ -6666,12 +6681,12 @@
         <v>4</v>
       </c>
       <c r="H213" t="s">
-        <v>187</v>
+        <v>81</v>
       </c>
     </row>
     <row r="214" spans="1:8">
-      <c r="A214" s="9">
-        <v>2.5</v>
+      <c r="A214" s="8">
+        <v>5</v>
       </c>
       <c r="B214" t="s">
         <v>67</v>
@@ -6680,7 +6695,7 @@
         <v>43250</v>
       </c>
       <c r="D214" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E214" t="s">
         <v>108</v>
@@ -6689,21 +6704,21 @@
         <v>4</v>
       </c>
       <c r="H214" t="s">
-        <v>81</v>
+        <v>187</v>
       </c>
     </row>
     <row r="215" spans="1:8">
       <c r="A215" s="9">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="B215" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C215" s="2">
-        <v>43251</v>
+        <v>43250</v>
       </c>
       <c r="D215" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="E215" t="s">
         <v>108</v>
@@ -6717,30 +6732,30 @@
     </row>
     <row r="216" spans="1:8">
       <c r="A216" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="B216" t="s">
+        <v>64</v>
+      </c>
+      <c r="C216" s="2">
+        <v>43251</v>
+      </c>
+      <c r="D216" t="s">
+        <v>236</v>
+      </c>
+      <c r="E216" t="s">
+        <v>108</v>
+      </c>
+      <c r="F216">
+        <v>4</v>
+      </c>
+      <c r="H216" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8">
+      <c r="A217" s="9">
         <v>1.8</v>
-      </c>
-      <c r="B216" t="s">
-        <v>67</v>
-      </c>
-      <c r="C216" s="2">
-        <v>43252</v>
-      </c>
-      <c r="D216" t="s">
-        <v>240</v>
-      </c>
-      <c r="E216" t="s">
-        <v>108</v>
-      </c>
-      <c r="F216">
-        <v>4</v>
-      </c>
-      <c r="H216" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="217" spans="1:8">
-      <c r="A217" s="8">
-        <v>4</v>
       </c>
       <c r="B217" t="s">
         <v>67</v>
@@ -6749,7 +6764,7 @@
         <v>43252</v>
       </c>
       <c r="D217" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E217" t="s">
         <v>108</v>
@@ -6758,12 +6773,12 @@
         <v>4</v>
       </c>
       <c r="H217" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
     </row>
     <row r="218" spans="1:8">
       <c r="A218" s="8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B218" t="s">
         <v>67</v>
@@ -6772,7 +6787,7 @@
         <v>43252</v>
       </c>
       <c r="D218" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E218" t="s">
         <v>108</v>
@@ -6785,8 +6800,8 @@
       </c>
     </row>
     <row r="219" spans="1:8">
-      <c r="A219" s="9">
-        <v>1.8</v>
+      <c r="A219" s="8">
+        <v>6</v>
       </c>
       <c r="B219" t="s">
         <v>67</v>
@@ -6795,30 +6810,30 @@
         <v>43252</v>
       </c>
       <c r="D219" t="s">
+        <v>242</v>
+      </c>
+      <c r="E219" t="s">
+        <v>108</v>
+      </c>
+      <c r="F219">
+        <v>4</v>
+      </c>
+      <c r="H219" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8">
+      <c r="A220" s="9">
+        <v>1.8</v>
+      </c>
+      <c r="B220" t="s">
+        <v>67</v>
+      </c>
+      <c r="C220" s="2">
+        <v>43252</v>
+      </c>
+      <c r="D220" t="s">
         <v>33</v>
-      </c>
-      <c r="E219" t="s">
-        <v>108</v>
-      </c>
-      <c r="F219">
-        <v>4</v>
-      </c>
-      <c r="H219" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="220" spans="1:8">
-      <c r="A220" s="8">
-        <v>5</v>
-      </c>
-      <c r="B220" t="s">
-        <v>64</v>
-      </c>
-      <c r="C220" s="2">
-        <v>43254</v>
-      </c>
-      <c r="D220" t="s">
-        <v>243</v>
       </c>
       <c r="E220" t="s">
         <v>108</v>
@@ -6835,36 +6850,36 @@
         <v>5</v>
       </c>
       <c r="B221" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C221" s="2">
+        <v>43254</v>
+      </c>
+      <c r="D221" t="s">
+        <v>243</v>
+      </c>
+      <c r="E221" t="s">
+        <v>108</v>
+      </c>
+      <c r="F221">
+        <v>4</v>
+      </c>
+      <c r="H221" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8">
+      <c r="A222" s="8">
+        <v>5</v>
+      </c>
+      <c r="B222" t="s">
+        <v>67</v>
+      </c>
+      <c r="C222" s="2">
         <v>43255</v>
       </c>
-      <c r="D221" t="s">
+      <c r="D222" t="s">
         <v>180</v>
-      </c>
-      <c r="E221" t="s">
-        <v>108</v>
-      </c>
-      <c r="F221">
-        <v>4</v>
-      </c>
-      <c r="H221" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="222" spans="1:8">
-      <c r="A222" s="9">
-        <v>4.7</v>
-      </c>
-      <c r="B222" t="s">
-        <v>67</v>
-      </c>
-      <c r="C222" s="2">
-        <v>43256</v>
-      </c>
-      <c r="D222" t="s">
-        <v>245</v>
       </c>
       <c r="E222" t="s">
         <v>108</v>
@@ -6877,8 +6892,8 @@
       </c>
     </row>
     <row r="223" spans="1:8">
-      <c r="A223" s="8">
-        <v>5</v>
+      <c r="A223" s="9">
+        <v>4.7</v>
       </c>
       <c r="B223" t="s">
         <v>67</v>
@@ -6887,7 +6902,7 @@
         <v>43256</v>
       </c>
       <c r="D223" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E223" t="s">
         <v>108</v>
@@ -6901,16 +6916,16 @@
     </row>
     <row r="224" spans="1:8">
       <c r="A224" s="8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B224" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C224" s="2">
         <v>43256</v>
       </c>
       <c r="D224" t="s">
-        <v>11</v>
+        <v>244</v>
       </c>
       <c r="E224" t="s">
         <v>108</v>
@@ -6919,67 +6934,67 @@
         <v>4</v>
       </c>
       <c r="H224" t="s">
-        <v>81</v>
+        <v>187</v>
       </c>
     </row>
     <row r="225" spans="1:8">
-      <c r="A225" s="9">
-        <v>1.5</v>
+      <c r="A225" s="8">
+        <v>10</v>
       </c>
       <c r="B225" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C225" s="2">
         <v>43256</v>
       </c>
       <c r="D225" t="s">
+        <v>11</v>
+      </c>
+      <c r="E225" t="s">
+        <v>108</v>
+      </c>
+      <c r="F225">
+        <v>4</v>
+      </c>
+      <c r="H225" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8">
+      <c r="A226" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="B226" t="s">
+        <v>67</v>
+      </c>
+      <c r="C226" s="2">
+        <v>43256</v>
+      </c>
+      <c r="D226" t="s">
         <v>246</v>
       </c>
-      <c r="E225" t="s">
-        <v>108</v>
-      </c>
-      <c r="F225">
-        <v>4</v>
-      </c>
-      <c r="H225" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="226" spans="1:8">
-      <c r="A226" s="8">
-        <v>99</v>
-      </c>
-      <c r="B226" t="s">
-        <v>64</v>
-      </c>
-      <c r="C226" s="2">
-        <v>43257</v>
-      </c>
-      <c r="D226" t="s">
-        <v>247</v>
-      </c>
       <c r="E226" t="s">
         <v>108</v>
       </c>
       <c r="F226">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H226" t="s">
-        <v>187</v>
+        <v>81</v>
       </c>
     </row>
     <row r="227" spans="1:8">
       <c r="A227" s="8">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="B227" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C227" s="2">
         <v>43257</v>
       </c>
-      <c r="D227" s="2" t="s">
-        <v>248</v>
+      <c r="D227" t="s">
+        <v>247</v>
       </c>
       <c r="E227" t="s">
         <v>108</v>
@@ -6992,8 +7007,8 @@
       </c>
     </row>
     <row r="228" spans="1:8">
-      <c r="A228" s="9">
-        <v>2.8</v>
+      <c r="A228" s="8">
+        <v>7</v>
       </c>
       <c r="B228" t="s">
         <v>67</v>
@@ -7001,8 +7016,8 @@
       <c r="C228" s="2">
         <v>43257</v>
       </c>
-      <c r="D228" t="s">
-        <v>249</v>
+      <c r="D228" s="2" t="s">
+        <v>248</v>
       </c>
       <c r="E228" t="s">
         <v>108</v>
@@ -7011,27 +7026,27 @@
         <v>3</v>
       </c>
       <c r="H228" t="s">
-        <v>81</v>
+        <v>187</v>
       </c>
     </row>
     <row r="229" spans="1:8">
-      <c r="A229" s="8">
-        <v>1</v>
+      <c r="A229" s="9">
+        <v>2.8</v>
       </c>
       <c r="B229" t="s">
         <v>67</v>
       </c>
       <c r="C229" s="2">
-        <v>43260</v>
+        <v>43257</v>
       </c>
       <c r="D229" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E229" t="s">
         <v>108</v>
       </c>
       <c r="F229">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H229" t="s">
         <v>81</v>
@@ -7039,7 +7054,7 @@
     </row>
     <row r="230" spans="1:8">
       <c r="A230" s="8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B230" t="s">
         <v>67</v>
@@ -7048,7 +7063,7 @@
         <v>43260</v>
       </c>
       <c r="D230" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E230" t="s">
         <v>108</v>
@@ -7062,39 +7077,39 @@
     </row>
     <row r="231" spans="1:8">
       <c r="A231" s="8">
+        <v>4</v>
+      </c>
+      <c r="B231" t="s">
+        <v>67</v>
+      </c>
+      <c r="C231" s="2">
+        <v>43260</v>
+      </c>
+      <c r="D231" t="s">
+        <v>251</v>
+      </c>
+      <c r="E231" t="s">
+        <v>108</v>
+      </c>
+      <c r="F231">
+        <v>4</v>
+      </c>
+      <c r="H231" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8">
+      <c r="A232" s="8">
         <v>50</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B232" t="s">
         <v>68</v>
-      </c>
-      <c r="C231" s="2">
-        <v>43261</v>
-      </c>
-      <c r="D231" t="s">
-        <v>252</v>
-      </c>
-      <c r="E231" t="s">
-        <v>108</v>
-      </c>
-      <c r="F231">
-        <v>4</v>
-      </c>
-      <c r="H231" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="232" spans="1:8">
-      <c r="A232" s="9">
-        <v>7.2</v>
-      </c>
-      <c r="B232" t="s">
-        <v>67</v>
       </c>
       <c r="C232" s="2">
         <v>43261</v>
       </c>
       <c r="D232" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E232" t="s">
         <v>108</v>
@@ -7103,12 +7118,12 @@
         <v>4</v>
       </c>
       <c r="H232" t="s">
-        <v>164</v>
+        <v>81</v>
       </c>
     </row>
     <row r="233" spans="1:8">
-      <c r="A233" s="8">
-        <v>1</v>
+      <c r="A233" s="9">
+        <v>7.2</v>
       </c>
       <c r="B233" t="s">
         <v>67</v>
@@ -7117,7 +7132,7 @@
         <v>43261</v>
       </c>
       <c r="D233" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E233" t="s">
         <v>108</v>
@@ -7131,7 +7146,7 @@
     </row>
     <row r="234" spans="1:8">
       <c r="A234" s="8">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B234" t="s">
         <v>67</v>
@@ -7140,7 +7155,7 @@
         <v>43261</v>
       </c>
       <c r="D234" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E234" t="s">
         <v>108</v>
@@ -7149,12 +7164,12 @@
         <v>4</v>
       </c>
       <c r="H234" t="s">
-        <v>82</v>
+        <v>164</v>
       </c>
     </row>
     <row r="235" spans="1:8">
-      <c r="A235" s="9">
-        <v>1.1000000000000001</v>
+      <c r="A235" s="8">
+        <v>7</v>
       </c>
       <c r="B235" t="s">
         <v>67</v>
@@ -7163,31 +7178,31 @@
         <v>43261</v>
       </c>
       <c r="D235" t="s">
+        <v>255</v>
+      </c>
+      <c r="E235" t="s">
+        <v>108</v>
+      </c>
+      <c r="F235">
+        <v>4</v>
+      </c>
+      <c r="H235" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8">
+      <c r="A236" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B236" t="s">
+        <v>67</v>
+      </c>
+      <c r="C236" s="2">
+        <v>43261</v>
+      </c>
+      <c r="D236" t="s">
         <v>256</v>
       </c>
-      <c r="E235" t="s">
-        <v>108</v>
-      </c>
-      <c r="F235">
-        <v>4</v>
-      </c>
-      <c r="H235" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="236" spans="1:8">
-      <c r="A236" s="8">
-        <v>7</v>
-      </c>
-      <c r="B236" t="s">
-        <v>64</v>
-      </c>
-      <c r="C236" s="2">
-        <v>43262</v>
-      </c>
-      <c r="D236" t="s">
-        <v>257</v>
-      </c>
       <c r="E236" t="s">
         <v>108</v>
       </c>
@@ -7195,21 +7210,21 @@
         <v>4</v>
       </c>
       <c r="H236" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="237" spans="1:8">
       <c r="A237" s="8">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B237" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C237" s="2">
         <v>43262</v>
       </c>
       <c r="D237" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E237" t="s">
         <v>108</v>
@@ -7223,7 +7238,7 @@
     </row>
     <row r="238" spans="1:8">
       <c r="A238" s="8">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B238" t="s">
         <v>73</v>
@@ -7232,7 +7247,7 @@
         <v>43262</v>
       </c>
       <c r="D238" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E238" t="s">
         <v>108</v>
@@ -7245,47 +7260,168 @@
       </c>
     </row>
     <row r="239" spans="1:8">
-      <c r="A239" s="9">
+      <c r="A239" s="8">
+        <v>3</v>
+      </c>
+      <c r="B239" t="s">
+        <v>73</v>
+      </c>
+      <c r="C239" s="2">
+        <v>43262</v>
+      </c>
+      <c r="D239" t="s">
+        <v>259</v>
+      </c>
+      <c r="E239" t="s">
+        <v>108</v>
+      </c>
+      <c r="F239">
+        <v>4</v>
+      </c>
+      <c r="H239" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8">
+      <c r="A240" s="9">
         <v>11.2</v>
       </c>
-      <c r="B239" t="s">
+      <c r="B240" t="s">
         <v>64</v>
       </c>
-      <c r="C239" s="2">
+      <c r="C240" s="2">
         <v>43263</v>
       </c>
-      <c r="D239" t="s">
+      <c r="D240" t="s">
         <v>260</v>
       </c>
-      <c r="E239" t="s">
-        <v>108</v>
-      </c>
-      <c r="F239">
-        <v>4</v>
-      </c>
-      <c r="H239" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="366" spans="1:12">
-      <c r="A366" s="1"/>
-      <c r="B366" s="1"/>
-      <c r="C366" s="1"/>
-      <c r="D366" s="1"/>
-      <c r="E366" s="1"/>
-      <c r="F366" s="1"/>
-      <c r="G366" s="1"/>
-      <c r="H366" s="1"/>
-      <c r="I366" s="1"/>
-      <c r="J366" s="1"/>
-      <c r="K366" s="1"/>
-      <c r="L366" s="1"/>
+      <c r="E240" t="s">
+        <v>108</v>
+      </c>
+      <c r="F240">
+        <v>4</v>
+      </c>
+      <c r="H240" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8">
+      <c r="A241" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="B241" t="s">
+        <v>67</v>
+      </c>
+      <c r="C241" s="2">
+        <v>43263</v>
+      </c>
+      <c r="D241" t="s">
+        <v>265</v>
+      </c>
+      <c r="E241" t="s">
+        <v>108</v>
+      </c>
+      <c r="F241">
+        <v>5</v>
+      </c>
+      <c r="H241" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8">
+      <c r="A242" s="8">
+        <v>150</v>
+      </c>
+      <c r="B242" t="s">
+        <v>68</v>
+      </c>
+      <c r="C242" s="2">
+        <v>43263</v>
+      </c>
+      <c r="D242" t="s">
+        <v>264</v>
+      </c>
+      <c r="E242" t="s">
+        <v>108</v>
+      </c>
+      <c r="F242">
+        <v>5</v>
+      </c>
+      <c r="H242" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8">
+      <c r="A243" s="9">
+        <v>12.7</v>
+      </c>
+      <c r="B243" t="s">
+        <v>72</v>
+      </c>
+      <c r="C243" s="2">
+        <v>43264</v>
+      </c>
+      <c r="D243" t="s">
+        <v>263</v>
+      </c>
+      <c r="E243" t="s">
+        <v>108</v>
+      </c>
+      <c r="F243">
+        <v>4</v>
+      </c>
+      <c r="H243" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8">
+      <c r="A244" s="9">
+        <v>89.9</v>
+      </c>
+      <c r="B244" t="s">
+        <v>69</v>
+      </c>
+      <c r="C244" s="2">
+        <v>43264</v>
+      </c>
+      <c r="D244" t="s">
+        <v>262</v>
+      </c>
+      <c r="E244" t="s">
+        <v>108</v>
+      </c>
+      <c r="F244">
+        <v>4</v>
+      </c>
+      <c r="H244" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8">
+      <c r="A245" s="9">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B245" t="s">
+        <v>67</v>
+      </c>
+      <c r="C245" s="2">
+        <v>43264</v>
+      </c>
+      <c r="D245" t="s">
+        <v>261</v>
+      </c>
+      <c r="E245" t="s">
+        <v>108</v>
+      </c>
+      <c r="F245">
+        <v>4</v>
+      </c>
+      <c r="H245" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="367" spans="1:12">
-      <c r="A367" s="1">
-        <f>SUBTOTAL(109,[Ποσό €])</f>
-        <v>2688.5899999999997</v>
-      </c>
+      <c r="A367" s="1"/>
       <c r="B367" s="1"/>
       <c r="C367" s="1"/>
       <c r="D367" s="1"/>
@@ -7295,9 +7431,26 @@
       <c r="H367" s="1"/>
       <c r="I367" s="1"/>
       <c r="J367" s="1"/>
+      <c r="K367" s="1"/>
+      <c r="L367" s="1"/>
     </row>
     <row r="368" spans="1:12">
-      <c r="A368" s="4"/>
+      <c r="A368" s="1">
+        <f>SUBTOTAL(109,[Ποσό €])</f>
+        <v>3097.6899999999991</v>
+      </c>
+      <c r="B368" s="1"/>
+      <c r="C368" s="1"/>
+      <c r="D368" s="1"/>
+      <c r="E368" s="1"/>
+      <c r="F368" s="1"/>
+      <c r="G368" s="1"/>
+      <c r="H368" s="1"/>
+      <c r="I368" s="1"/>
+      <c r="J368" s="1"/>
+    </row>
+    <row r="369" spans="1:1">
+      <c r="A369" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
delete unecessary column from database
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -1045,24 +1045,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="126608128"/>
-        <c:axId val="126609664"/>
+        <c:axId val="113632000"/>
+        <c:axId val="113633536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="126608128"/>
+        <c:axId val="113632000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126609664"/>
+        <c:crossAx val="113633536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126609664"/>
+        <c:axId val="113633536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1070,7 +1070,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126608128"/>
+        <c:crossAx val="113632000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1132,7 +1132,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1260,24 +1260,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="126592512"/>
-        <c:axId val="126594048"/>
+        <c:axId val="113616384"/>
+        <c:axId val="113617920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="126592512"/>
+        <c:axId val="113616384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126594048"/>
+        <c:crossAx val="113617920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126594048"/>
+        <c:axId val="113617920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1285,7 +1285,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126592512"/>
+        <c:crossAx val="113616384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1294,7 +1294,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1349,24 +1349,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="157444352"/>
-        <c:axId val="157446144"/>
+        <c:axId val="115435776"/>
+        <c:axId val="115437568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="157444352"/>
+        <c:axId val="115435776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="157446144"/>
+        <c:crossAx val="115437568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="157446144"/>
+        <c:axId val="115437568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1374,7 +1374,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="157444352"/>
+        <c:crossAx val="115435776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1383,7 +1383,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1841,8 +1841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="H151" sqref="H151"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B368" sqref="B368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4458,7 +4458,7 @@
         <v>0.7</v>
       </c>
       <c r="B117" t="s">
-        <v>134</v>
+        <v>67</v>
       </c>
       <c r="C117" s="2">
         <v>43194</v>

</xml_diff>

<commit_message>
added some new columns in database
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="273">
   <si>
     <t>Ημερομηνία</t>
   </si>
@@ -830,6 +830,12 @@
   </si>
   <si>
     <t>Ναύπλιο</t>
+  </si>
+  <si>
+    <t>σαντουιτς με προσουτο</t>
+  </si>
+  <si>
+    <t>γκοφρέτα</t>
   </si>
 </sst>
 </file>
@@ -1060,24 +1066,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="126542592"/>
-        <c:axId val="126544128"/>
+        <c:axId val="113238784"/>
+        <c:axId val="113240320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="126542592"/>
+        <c:axId val="113238784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126544128"/>
+        <c:crossAx val="113240320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126544128"/>
+        <c:axId val="113240320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1085,7 +1091,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126542592"/>
+        <c:crossAx val="113238784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1147,7 +1153,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1275,24 +1281,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="126526976"/>
-        <c:axId val="126528512"/>
+        <c:axId val="113223168"/>
+        <c:axId val="113224704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="126526976"/>
+        <c:axId val="113223168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126528512"/>
+        <c:crossAx val="113224704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126528512"/>
+        <c:axId val="113224704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +1306,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126526976"/>
+        <c:crossAx val="113223168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1309,7 +1315,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1364,24 +1370,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="127232256"/>
-        <c:axId val="127234048"/>
+        <c:axId val="145783040"/>
+        <c:axId val="145784832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="127232256"/>
+        <c:axId val="145783040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127234048"/>
+        <c:crossAx val="145784832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127234048"/>
+        <c:axId val="145784832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1389,7 +1395,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127232256"/>
+        <c:crossAx val="145783040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1398,7 +1404,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1856,8 +1862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A242" workbookViewId="0">
-      <selection activeCell="H250" sqref="H250"/>
+    <sheetView tabSelected="1" topLeftCell="A243" workbookViewId="0">
+      <selection activeCell="D252" sqref="D252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7527,6 +7533,49 @@
         <v>270</v>
       </c>
     </row>
+    <row r="250" spans="1:8">
+      <c r="A250" s="9">
+        <v>3.9</v>
+      </c>
+      <c r="B250" t="s">
+        <v>67</v>
+      </c>
+      <c r="C250" s="2">
+        <v>43269</v>
+      </c>
+      <c r="D250" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="E250" t="s">
+        <v>108</v>
+      </c>
+      <c r="F250">
+        <v>5</v>
+      </c>
+      <c r="H250" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8">
+      <c r="B251" t="s">
+        <v>67</v>
+      </c>
+      <c r="C251" s="2">
+        <v>43269</v>
+      </c>
+      <c r="D251" t="s">
+        <v>272</v>
+      </c>
+      <c r="E251" t="s">
+        <v>108</v>
+      </c>
+      <c r="F251">
+        <v>5</v>
+      </c>
+      <c r="H251" t="s">
+        <v>164</v>
+      </c>
+    </row>
     <row r="367" spans="1:12">
       <c r="A367" s="1"/>
       <c r="B367" s="1"/>
@@ -7544,7 +7593,7 @@
     <row r="368" spans="1:12">
       <c r="A368" s="1">
         <f>SUBTOTAL(109,[Ποσό €])</f>
-        <v>3114.0899999999988</v>
+        <v>3117.9899999999989</v>
       </c>
       <c r="B368" s="1"/>
       <c r="C368" s="1"/>

</xml_diff>

<commit_message>
changes ready to step furder to the new UI
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="376">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1078,57 +1078,21 @@
     <t>Education</t>
   </si>
   <si>
-    <t>Food &amp; drink</t>
-  </si>
-  <si>
-    <t>Family &amp; friends</t>
-  </si>
-  <si>
-    <t>Health care &amp; Drug stores</t>
-  </si>
-  <si>
-    <t>household &amp; utilities</t>
-  </si>
-  <si>
-    <t>Insurance &amp; finances</t>
-  </si>
-  <si>
     <t>Entertainment</t>
   </si>
   <si>
-    <t>Media &amp; Electronics</t>
-  </si>
-  <si>
     <t>Shopping</t>
   </si>
   <si>
-    <t>Subscriptions &amp; donations</t>
-  </si>
-  <si>
-    <t>tax &amp; Fines</t>
-  </si>
-  <si>
     <t>Beaty</t>
   </si>
   <si>
-    <t>family &amp; friends</t>
-  </si>
-  <si>
     <t>transport</t>
   </si>
   <si>
     <t>shopping</t>
   </si>
   <si>
-    <t>travel &amp; holidays</t>
-  </si>
-  <si>
-    <t>tax &amp; fines</t>
-  </si>
-  <si>
-    <t>media &amp; electonics</t>
-  </si>
-  <si>
     <t>health care</t>
   </si>
   <si>
@@ -1139,6 +1103,45 @@
   </si>
   <si>
     <t>αεροπορικά για Κρήτη (+ Μιχάλη)</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>family-friends</t>
+  </si>
+  <si>
+    <t>Food-drink</t>
+  </si>
+  <si>
+    <t>Family-friends</t>
+  </si>
+  <si>
+    <t>Health care-Drug stores</t>
+  </si>
+  <si>
+    <t>household-utilities</t>
+  </si>
+  <si>
+    <t>Insurance-finances</t>
+  </si>
+  <si>
+    <t>Media-Electronics</t>
+  </si>
+  <si>
+    <t>Subscriptions-donations</t>
+  </si>
+  <si>
+    <t>tax-Fines</t>
+  </si>
+  <si>
+    <t>travel-holidays</t>
+  </si>
+  <si>
+    <t>media-electonics</t>
+  </si>
+  <si>
+    <t>tax-fines</t>
   </si>
 </sst>
 </file>
@@ -1575,8 +1578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" workbookViewId="0">
-      <selection activeCell="D227" sqref="D227"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,7 +1632,7 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C2" s="2">
         <v>43120</v>
@@ -1673,13 +1676,16 @@
       <c r="K3" t="s">
         <v>353</v>
       </c>
+      <c r="L3" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C4" s="2">
         <v>43120</v>
@@ -1697,7 +1703,10 @@
         <v>250</v>
       </c>
       <c r="K4" t="s">
-        <v>354</v>
+        <v>365</v>
+      </c>
+      <c r="L4" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1723,7 +1732,10 @@
         <v>253</v>
       </c>
       <c r="K5" t="s">
-        <v>355</v>
+        <v>366</v>
+      </c>
+      <c r="L5" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1731,7 +1743,7 @@
         <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C6" s="2">
         <v>43121</v>
@@ -1749,7 +1761,10 @@
         <v>250</v>
       </c>
       <c r="K6" t="s">
-        <v>356</v>
+        <v>367</v>
+      </c>
+      <c r="L6" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1775,7 +1790,10 @@
         <v>250</v>
       </c>
       <c r="K7" t="s">
-        <v>357</v>
+        <v>368</v>
+      </c>
+      <c r="L7" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1801,7 +1819,7 @@
         <v>254</v>
       </c>
       <c r="K8" t="s">
-        <v>358</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1827,7 +1845,10 @@
         <v>254</v>
       </c>
       <c r="K9" t="s">
-        <v>359</v>
+        <v>354</v>
+      </c>
+      <c r="L9" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1853,7 +1874,10 @@
         <v>257</v>
       </c>
       <c r="K10" t="s">
-        <v>360</v>
+        <v>370</v>
+      </c>
+      <c r="L10" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1879,7 +1903,10 @@
         <v>257</v>
       </c>
       <c r="K11" t="s">
-        <v>361</v>
+        <v>355</v>
+      </c>
+      <c r="L11" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -1905,7 +1932,7 @@
         <v>255</v>
       </c>
       <c r="K12" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1931,6 +1958,9 @@
         <v>257</v>
       </c>
       <c r="K13" t="s">
+        <v>372</v>
+      </c>
+      <c r="L13" t="s">
         <v>363</v>
       </c>
     </row>
@@ -1957,7 +1987,10 @@
         <v>257</v>
       </c>
       <c r="K14" t="s">
-        <v>366</v>
+        <v>357</v>
+      </c>
+      <c r="L14" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1965,7 +1998,7 @@
         <v>5.15</v>
       </c>
       <c r="B15" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C15" s="2">
         <v>43129</v>
@@ -1983,7 +2016,10 @@
         <v>256</v>
       </c>
       <c r="K15" t="s">
-        <v>368</v>
+        <v>373</v>
+      </c>
+      <c r="L15" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1991,7 +2027,7 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C16" s="2">
         <v>43129</v>
@@ -2009,7 +2045,10 @@
         <v>255</v>
       </c>
       <c r="K16" t="s">
-        <v>364</v>
+        <v>356</v>
+      </c>
+      <c r="L16" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2224,7 +2263,7 @@
         <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C26" s="2">
         <v>43139</v>
@@ -2408,7 +2447,7 @@
         <v>49.9</v>
       </c>
       <c r="B34" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C34" s="2">
         <v>43143</v>
@@ -2428,7 +2467,7 @@
         <v>140</v>
       </c>
       <c r="B35" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C35" s="2">
         <v>43143</v>
@@ -2520,7 +2559,7 @@
         <v>15.96</v>
       </c>
       <c r="B39" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C39" s="2">
         <v>43148</v>
@@ -2566,7 +2605,7 @@
         <v>79.8</v>
       </c>
       <c r="B41" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C41" s="2">
         <v>43148</v>
@@ -2612,7 +2651,7 @@
         <v>38.880000000000003</v>
       </c>
       <c r="B43" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C43" s="2">
         <v>43151</v>
@@ -2658,7 +2697,7 @@
         <v>0.79</v>
       </c>
       <c r="B45" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C45" s="2">
         <v>43152</v>
@@ -2681,7 +2720,7 @@
         <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C46" s="2">
         <v>43153</v>
@@ -2773,7 +2812,7 @@
         <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C50" s="2">
         <v>43155</v>
@@ -2819,7 +2858,7 @@
         <v>1.8</v>
       </c>
       <c r="B52" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C52" s="2">
         <v>43155</v>
@@ -2935,7 +2974,7 @@
         <v>5.4</v>
       </c>
       <c r="B57" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C57" s="2">
         <v>43156</v>
@@ -2981,7 +3020,7 @@
         <v>5.4</v>
       </c>
       <c r="B59" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C59" s="2">
         <v>43156</v>
@@ -3004,7 +3043,7 @@
         <v>0.6</v>
       </c>
       <c r="B60" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C60" s="2">
         <v>43157</v>
@@ -3096,7 +3135,7 @@
         <v>1.2</v>
       </c>
       <c r="B64" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C64" s="2">
         <v>43158</v>
@@ -3119,7 +3158,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="B65" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C65" s="2">
         <v>43158</v>
@@ -3142,7 +3181,7 @@
         <v>13.5</v>
       </c>
       <c r="B66" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C66" s="2">
         <v>43160</v>
@@ -3212,7 +3251,7 @@
         <v>90</v>
       </c>
       <c r="B69" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C69" s="2">
         <v>43161</v>
@@ -3235,7 +3274,7 @@
         <v>65.5</v>
       </c>
       <c r="B70" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C70" s="2">
         <v>43161</v>
@@ -3258,7 +3297,7 @@
         <v>4.5</v>
       </c>
       <c r="B71" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C71" s="2">
         <v>43162</v>
@@ -3281,7 +3320,7 @@
         <v>10</v>
       </c>
       <c r="B72" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C72" s="2">
         <v>43162</v>
@@ -3443,7 +3482,7 @@
         <v>9.9</v>
       </c>
       <c r="B79" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C79" s="2">
         <v>43169</v>
@@ -3489,7 +3528,7 @@
         <v>79.8</v>
       </c>
       <c r="B81" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C81" s="2">
         <v>43169</v>
@@ -3512,7 +3551,7 @@
         <v>10</v>
       </c>
       <c r="B82" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="C82" s="2">
         <v>43170</v>
@@ -3650,7 +3689,7 @@
         <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C88" s="2">
         <v>43171</v>
@@ -3673,7 +3712,7 @@
         <v>24.9</v>
       </c>
       <c r="B89" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C89" s="2">
         <v>43171</v>
@@ -3719,7 +3758,7 @@
         <v>44.99</v>
       </c>
       <c r="B91" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C91" s="2">
         <v>43174</v>
@@ -3742,7 +3781,7 @@
         <v>4</v>
       </c>
       <c r="B92" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C92" s="2">
         <v>43175</v>
@@ -3909,7 +3948,7 @@
         <v>34.9</v>
       </c>
       <c r="B101" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C101" s="2">
         <v>43183</v>
@@ -4192,7 +4231,7 @@
         <v>8</v>
       </c>
       <c r="B115" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C115" s="2">
         <v>43194</v>
@@ -4261,7 +4300,7 @@
         <v>6.3</v>
       </c>
       <c r="B118" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C118" s="2">
         <v>43194</v>
@@ -4399,7 +4438,7 @@
         <v>24.3</v>
       </c>
       <c r="B124" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C124" s="2">
         <v>43199</v>
@@ -4583,7 +4622,7 @@
         <v>5</v>
       </c>
       <c r="B132" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C132" s="2">
         <v>43202</v>
@@ -4606,7 +4645,7 @@
         <v>43</v>
       </c>
       <c r="B133" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C133" s="2">
         <v>43203</v>
@@ -4629,7 +4668,7 @@
         <v>10</v>
       </c>
       <c r="B134" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="C134" s="2">
         <v>43203</v>
@@ -4790,7 +4829,7 @@
         <v>4</v>
       </c>
       <c r="B141" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="C141" s="2">
         <v>43207</v>
@@ -4997,7 +5036,7 @@
         <v>150</v>
       </c>
       <c r="B150" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="C150" s="2">
         <v>43211</v>
@@ -5020,7 +5059,7 @@
         <v>7</v>
       </c>
       <c r="B151" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="C151" s="2">
         <v>43211</v>
@@ -5089,7 +5128,7 @@
         <v>3.5</v>
       </c>
       <c r="B154" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C154" s="2">
         <v>43211</v>
@@ -5112,7 +5151,7 @@
         <v>55</v>
       </c>
       <c r="B155" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C155" s="2">
         <v>43213</v>
@@ -5181,7 +5220,7 @@
         <v>39.9</v>
       </c>
       <c r="B158" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C158" s="2">
         <v>43216</v>
@@ -5710,7 +5749,7 @@
         <v>8</v>
       </c>
       <c r="B181" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C181" s="2">
         <v>43236</v>
@@ -5756,7 +5795,7 @@
         <v>10</v>
       </c>
       <c r="B183" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="C183" s="2">
         <v>43237</v>
@@ -5779,7 +5818,7 @@
         <v>3</v>
       </c>
       <c r="B184" t="s">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="C184" s="2">
         <v>43237</v>
@@ -5802,7 +5841,7 @@
         <v>10</v>
       </c>
       <c r="B185" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="C185" s="2">
         <v>43237</v>
@@ -5848,7 +5887,7 @@
         <v>10</v>
       </c>
       <c r="B187" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C187" s="2">
         <v>43237</v>
@@ -5894,7 +5933,7 @@
         <v>6.2</v>
       </c>
       <c r="B189" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C189" s="2">
         <v>43238</v>
@@ -5940,7 +5979,7 @@
         <v>10</v>
       </c>
       <c r="B191" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C191" s="2">
         <v>43239</v>
@@ -6009,7 +6048,7 @@
         <v>14</v>
       </c>
       <c r="B194" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C194" s="2">
         <v>43241</v>
@@ -6055,7 +6094,7 @@
         <v>69.900000000000006</v>
       </c>
       <c r="B196" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C196" s="2">
         <v>43241</v>
@@ -6193,7 +6232,7 @@
         <v>78.849999999999994</v>
       </c>
       <c r="B202" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C202" s="2">
         <v>43245</v>
@@ -6515,7 +6554,7 @@
         <v>3.5</v>
       </c>
       <c r="B216" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C216" s="2">
         <v>43251</v>
@@ -6630,7 +6669,7 @@
         <v>5</v>
       </c>
       <c r="B221" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C221" s="2">
         <v>43254</v>
@@ -6768,13 +6807,13 @@
         <v>129</v>
       </c>
       <c r="B227" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C227" s="2">
         <v>43257</v>
       </c>
       <c r="D227" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="E227" t="s">
         <v>247</v>
@@ -6883,7 +6922,7 @@
         <v>50</v>
       </c>
       <c r="B232" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C232" s="2">
         <v>43261</v>
@@ -6998,7 +7037,7 @@
         <v>7</v>
       </c>
       <c r="B237" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C237" s="2">
         <v>43262</v>
@@ -7021,7 +7060,7 @@
         <v>15</v>
       </c>
       <c r="B238" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="C238" s="2">
         <v>43262</v>
@@ -7044,7 +7083,7 @@
         <v>3</v>
       </c>
       <c r="B239" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="C239" s="2">
         <v>43262</v>
@@ -7067,7 +7106,7 @@
         <v>11.2</v>
       </c>
       <c r="B240" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C240" s="2">
         <v>43263</v>
@@ -7113,7 +7152,7 @@
         <v>150</v>
       </c>
       <c r="B242" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="C242" s="2">
         <v>43263</v>
@@ -7136,7 +7175,7 @@
         <v>12.7</v>
       </c>
       <c r="B243" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C243" s="2">
         <v>43264</v>
@@ -7159,7 +7198,7 @@
         <v>89.9</v>
       </c>
       <c r="B244" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C244" s="2">
         <v>43264</v>
@@ -7550,7 +7589,7 @@
         <v>4</v>
       </c>
       <c r="B261" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C261" s="2">
         <v>43274</v>
@@ -7688,7 +7727,7 @@
         <v>13.5</v>
       </c>
       <c r="B267" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C267" s="2">
         <v>43275</v>
@@ -7734,7 +7773,7 @@
         <v>20</v>
       </c>
       <c r="B269" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C269" s="2">
         <v>43277</v>
@@ -7895,7 +7934,7 @@
         <v>5</v>
       </c>
       <c r="B276" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C276" s="2">
         <v>43280</v>
@@ -7918,7 +7957,7 @@
         <v>10</v>
       </c>
       <c r="B277" t="s">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="C277" s="2">
         <v>43280</v>
@@ -7964,7 +8003,7 @@
         <v>10</v>
       </c>
       <c r="B279" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C279" s="2">
         <v>43281</v>
@@ -8079,7 +8118,7 @@
         <v>119.9</v>
       </c>
       <c r="B284" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C284" s="2">
         <v>43284</v>
@@ -8125,7 +8164,7 @@
         <v>3.5</v>
       </c>
       <c r="B286" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="C286" s="2">
         <v>43284</v>
@@ -8332,7 +8371,7 @@
         <v>25</v>
       </c>
       <c r="B295" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="C295" s="2">
         <v>43289</v>
@@ -8355,7 +8394,7 @@
         <v>3.5</v>
       </c>
       <c r="B296" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C296" s="2">
         <v>43289</v>
@@ -8493,7 +8532,7 @@
         <v>15</v>
       </c>
       <c r="B302" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C302" s="2">
         <v>43293</v>
@@ -8654,7 +8693,7 @@
         <v>7.5</v>
       </c>
       <c r="B309" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="C309" s="2">
         <v>43295</v>
@@ -8700,7 +8739,7 @@
         <v>5</v>
       </c>
       <c r="B311" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C311" s="2">
         <v>43295</v>
@@ -8723,7 +8762,7 @@
         <v>3</v>
       </c>
       <c r="B312" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C312" s="2">
         <v>43296</v>
@@ -9160,7 +9199,7 @@
         <v>3.85</v>
       </c>
       <c r="B331" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C331" s="2">
         <v>43306</v>
@@ -9252,7 +9291,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="B335" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C335" s="2">
         <v>43307</v>
@@ -9275,7 +9314,7 @@
         <v>10</v>
       </c>
       <c r="B336" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="C336" s="2">
         <v>43307</v>
@@ -9318,7 +9357,7 @@
         <v>350</v>
       </c>
       <c r="B338" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="C338" s="2">
         <v>43308</v>
@@ -9433,7 +9472,7 @@
         <v>6</v>
       </c>
       <c r="B343" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="C343" s="2">
         <v>43311</v>
@@ -9525,7 +9564,7 @@
         <v>43.22</v>
       </c>
       <c r="B347" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C347" s="2">
         <v>43312</v>
@@ -9617,7 +9656,7 @@
         <v>20</v>
       </c>
       <c r="B351" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="C351" s="2">
         <v>43314</v>
@@ -9640,7 +9679,7 @@
         <v>14.84</v>
       </c>
       <c r="B352" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="C352" s="2">
         <v>43314</v>
@@ -9732,7 +9771,7 @@
         <v>29.4</v>
       </c>
       <c r="B356" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="C356" s="2">
         <v>43317</v>

</xml_diff>

<commit_message>
is going craaazy.Locations, types and smart search is up and running
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="377">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1142,6 +1142,9 @@
   </si>
   <si>
     <t>tax-fines</t>
+  </si>
+  <si>
+    <t>Peri</t>
   </si>
 </sst>
 </file>
@@ -1578,8 +1581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L369"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,7 +1717,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>229</v>
+        <v>376</v>
       </c>
       <c r="C5" s="2">
         <v>43120</v>

</xml_diff>

<commit_message>
gamwwwwwwwwww to spiti moy
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="364">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1106,9 +1106,6 @@
   </si>
   <si>
     <t>tax-fines</t>
-  </si>
-  <si>
-    <t>Peri</t>
   </si>
 </sst>
 </file>
@@ -1546,7 +1543,7 @@
   <dimension ref="A1:L369"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D358" sqref="D358"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,7 +1666,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>364</v>
+        <v>229</v>
       </c>
       <c r="C5" s="2">
         <v>43120</v>

</xml_diff>

<commit_message>
Made Console project that fucks whatever it wants to the database
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="Έξοδα" sheetId="1" r:id="rId1"/>
+    <sheet name="costs" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -1210,12 +1210,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1256,7 +1256,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -1354,7 +1354,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1396,7 +1396,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1428,9 +1428,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1462,6 +1463,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1637,14 +1639,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L518"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A384" workbookViewId="0">
       <selection activeCell="D394" sqref="D394"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
@@ -1660,7 +1662,7 @@
     <col min="12" max="12" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>235</v>
       </c>
@@ -1689,7 +1691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>20</v>
       </c>
@@ -1713,7 +1715,7 @@
       </c>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>10</v>
       </c>
@@ -1736,7 +1738,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>100</v>
       </c>
@@ -1759,7 +1761,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>10</v>
       </c>
@@ -1782,7 +1784,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>50</v>
       </c>
@@ -1805,7 +1807,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>3.2</v>
       </c>
@@ -1828,7 +1830,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1.3</v>
       </c>
@@ -1851,7 +1853,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1.2</v>
       </c>
@@ -1874,7 +1876,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>5</v>
       </c>
@@ -1897,7 +1899,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>4.5</v>
       </c>
@@ -1920,7 +1922,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>4</v>
       </c>
@@ -1943,7 +1945,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>10.6</v>
       </c>
@@ -1966,7 +1968,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>1.8</v>
       </c>
@@ -1989,7 +1991,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>5.15</v>
       </c>
@@ -2012,7 +2014,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>18</v>
       </c>
@@ -2035,7 +2037,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>1.5</v>
       </c>
@@ -2058,7 +2060,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>7.8</v>
       </c>
@@ -2081,7 +2083,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>4.4400000000000004</v>
       </c>
@@ -2104,7 +2106,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>1.5</v>
       </c>
@@ -2127,7 +2129,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>8.84</v>
       </c>
@@ -2150,7 +2152,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>4</v>
       </c>
@@ -2173,7 +2175,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>10</v>
       </c>
@@ -2196,7 +2198,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>1.8</v>
       </c>
@@ -2219,7 +2221,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>11.8</v>
       </c>
@@ -2242,7 +2244,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>40</v>
       </c>
@@ -2265,7 +2267,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>2.9</v>
       </c>
@@ -2288,7 +2290,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>4.3</v>
       </c>
@@ -2311,7 +2313,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>3.35</v>
       </c>
@@ -2334,7 +2336,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>5.2</v>
       </c>
@@ -2357,7 +2359,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>15</v>
       </c>
@@ -2380,7 +2382,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>3.9</v>
       </c>
@@ -2403,7 +2405,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>63.45</v>
       </c>
@@ -2426,7 +2428,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>49.9</v>
       </c>
@@ -2446,7 +2448,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>140</v>
       </c>
@@ -2469,7 +2471,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>1.8</v>
       </c>
@@ -2492,7 +2494,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>13.02</v>
       </c>
@@ -2515,7 +2517,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>4.7</v>
       </c>
@@ -2538,7 +2540,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>15.96</v>
       </c>
@@ -2561,7 +2563,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>9.8000000000000007</v>
       </c>
@@ -2584,7 +2586,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>79.8</v>
       </c>
@@ -2607,7 +2609,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>11.9</v>
       </c>
@@ -2630,7 +2632,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>38.880000000000003</v>
       </c>
@@ -2653,7 +2655,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>7.75</v>
       </c>
@@ -2676,7 +2678,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>0.79</v>
       </c>
@@ -2699,7 +2701,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>10</v>
       </c>
@@ -2722,7 +2724,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -2745,7 +2747,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -2768,7 +2770,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>1.8</v>
       </c>
@@ -2791,7 +2793,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>24</v>
       </c>
@@ -2814,7 +2816,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>24</v>
       </c>
@@ -2837,7 +2839,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>1.8</v>
       </c>
@@ -2860,7 +2862,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>3.5</v>
       </c>
@@ -2883,7 +2885,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>5.6</v>
       </c>
@@ -2907,7 +2909,7 @@
       </c>
       <c r="K54" s="4"/>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>1.5</v>
       </c>
@@ -2930,7 +2932,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>3</v>
       </c>
@@ -2953,7 +2955,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>5.4</v>
       </c>
@@ -2976,7 +2978,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>8</v>
       </c>
@@ -2999,7 +3001,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>5.4</v>
       </c>
@@ -3022,7 +3024,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>0.6</v>
       </c>
@@ -3045,7 +3047,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3068,7 +3070,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>1.5</v>
       </c>
@@ -3091,7 +3093,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3114,7 +3116,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>1.2</v>
       </c>
@@ -3137,7 +3139,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -3160,7 +3162,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>13.5</v>
       </c>
@@ -3183,7 +3185,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>3.5</v>
       </c>
@@ -3207,7 +3209,7 @@
       </c>
       <c r="K67" s="4"/>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>4.0999999999999996</v>
       </c>
@@ -3230,7 +3232,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>90</v>
       </c>
@@ -3253,7 +3255,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>65.5</v>
       </c>
@@ -3276,7 +3278,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>4.5</v>
       </c>
@@ -3299,7 +3301,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>10</v>
       </c>
@@ -3322,7 +3324,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>18.8</v>
       </c>
@@ -3345,7 +3347,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>1.8</v>
       </c>
@@ -3369,7 +3371,7 @@
       </c>
       <c r="K74" s="4"/>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>5.5</v>
       </c>
@@ -3392,7 +3394,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3415,7 +3417,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>3</v>
       </c>
@@ -3438,7 +3440,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>2</v>
       </c>
@@ -3461,7 +3463,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>9.9</v>
       </c>
@@ -3484,7 +3486,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>6.5</v>
       </c>
@@ -3507,7 +3509,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>79.8</v>
       </c>
@@ -3530,7 +3532,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>10</v>
       </c>
@@ -3553,7 +3555,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>2.5</v>
       </c>
@@ -3576,7 +3578,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>5</v>
       </c>
@@ -3599,7 +3601,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>1.6</v>
       </c>
@@ -3622,7 +3624,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>5.5</v>
       </c>
@@ -3645,7 +3647,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>0.8</v>
       </c>
@@ -3668,7 +3670,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>17</v>
       </c>
@@ -3691,7 +3693,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>24.9</v>
       </c>
@@ -3714,7 +3716,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>1.8</v>
       </c>
@@ -3737,7 +3739,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>44.99</v>
       </c>
@@ -3760,7 +3762,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>4</v>
       </c>
@@ -3783,7 +3785,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>5</v>
       </c>
@@ -3806,7 +3808,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>5</v>
       </c>
@@ -3829,13 +3831,13 @@
         <v>268</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3858,7 +3860,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>3</v>
       </c>
@@ -3881,7 +3883,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>6</v>
       </c>
@@ -3904,7 +3906,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>3.5</v>
       </c>
@@ -3927,7 +3929,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>34.9</v>
       </c>
@@ -3950,7 +3952,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>12</v>
       </c>
@@ -3973,10 +3975,10 @@
         <v>242</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>5</v>
       </c>
@@ -3999,7 +4001,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>6.9</v>
       </c>
@@ -4022,7 +4024,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>6.04</v>
       </c>
@@ -4045,7 +4047,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>4.8</v>
       </c>
@@ -4068,7 +4070,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>9.6999999999999993</v>
       </c>
@@ -4091,7 +4093,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>5.5</v>
       </c>
@@ -4114,7 +4116,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>7</v>
       </c>
@@ -4137,7 +4139,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>1</v>
       </c>
@@ -4160,7 +4162,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>4</v>
       </c>
@@ -4183,7 +4185,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>4.0999999999999996</v>
       </c>
@@ -4206,7 +4208,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>2.3199999999999998</v>
       </c>
@@ -4229,7 +4231,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>8</v>
       </c>
@@ -4252,7 +4254,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>12.5</v>
       </c>
@@ -4275,7 +4277,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>0.7</v>
       </c>
@@ -4298,7 +4300,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>6.3</v>
       </c>
@@ -4321,7 +4323,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>8</v>
       </c>
@@ -4344,7 +4346,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -4367,7 +4369,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>8</v>
       </c>
@@ -4390,7 +4392,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>4.5</v>
       </c>
@@ -4413,7 +4415,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>2.5</v>
       </c>
@@ -4436,7 +4438,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>24.3</v>
       </c>
@@ -4459,7 +4461,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>2</v>
       </c>
@@ -4482,7 +4484,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>16</v>
       </c>
@@ -4505,7 +4507,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>6</v>
       </c>
@@ -4528,7 +4530,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>5</v>
       </c>
@@ -4551,7 +4553,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>6.52</v>
       </c>
@@ -4574,7 +4576,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>1.8</v>
       </c>
@@ -4597,7 +4599,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>1</v>
       </c>
@@ -4620,7 +4622,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>5</v>
       </c>
@@ -4643,7 +4645,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
         <v>43</v>
       </c>
@@ -4666,7 +4668,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>10</v>
       </c>
@@ -4689,7 +4691,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>2.97</v>
       </c>
@@ -4712,7 +4714,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>10</v>
       </c>
@@ -4735,7 +4737,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>1.6</v>
       </c>
@@ -4758,7 +4760,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>1.5</v>
       </c>
@@ -4781,7 +4783,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>1.8</v>
       </c>
@@ -4804,7 +4806,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>7.3</v>
       </c>
@@ -4827,7 +4829,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>4</v>
       </c>
@@ -4850,7 +4852,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <v>2.1</v>
       </c>
@@ -4873,7 +4875,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>4.2</v>
       </c>
@@ -4896,7 +4898,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>9</v>
       </c>
@@ -4919,7 +4921,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <v>1</v>
       </c>
@@ -4942,7 +4944,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>3.5</v>
       </c>
@@ -4965,7 +4967,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -4988,7 +4990,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>3</v>
       </c>
@@ -5011,7 +5013,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>2</v>
       </c>
@@ -5034,7 +5036,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>150</v>
       </c>
@@ -5057,7 +5059,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
         <v>7</v>
       </c>
@@ -5080,7 +5082,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>5</v>
       </c>
@@ -5103,7 +5105,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
         <v>8</v>
       </c>
@@ -5126,7 +5128,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="4">
         <v>3.5</v>
       </c>
@@ -5149,7 +5151,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="4">
         <v>55</v>
       </c>
@@ -5172,7 +5174,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="4">
         <v>0.6</v>
       </c>
@@ -5195,7 +5197,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="4">
         <v>4</v>
       </c>
@@ -5218,7 +5220,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="4">
         <v>39.9</v>
       </c>
@@ -5241,7 +5243,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="4">
         <v>1.6</v>
       </c>
@@ -5264,7 +5266,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="4">
         <v>80</v>
       </c>
@@ -5287,7 +5289,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>6.2</v>
       </c>
@@ -5310,7 +5312,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="4">
         <v>15</v>
       </c>
@@ -5333,7 +5335,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="4">
         <v>4.3</v>
       </c>
@@ -5356,7 +5358,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="4">
         <v>9.6999999999999993</v>
       </c>
@@ -5379,7 +5381,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="4">
         <v>2.4500000000000002</v>
       </c>
@@ -5402,7 +5404,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="4">
         <v>1.96</v>
       </c>
@@ -5425,7 +5427,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="4">
         <v>11.5</v>
       </c>
@@ -5448,7 +5450,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="4">
         <v>2.7</v>
       </c>
@@ -5471,7 +5473,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="4">
         <v>2.7</v>
       </c>
@@ -5494,7 +5496,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="4">
         <v>7</v>
       </c>
@@ -5517,7 +5519,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="4">
         <v>4.8</v>
       </c>
@@ -5540,7 +5542,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
         <v>4.4000000000000004</v>
       </c>
@@ -5563,7 +5565,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="4">
         <v>3.8</v>
       </c>
@@ -5586,7 +5588,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
         <v>1.5</v>
       </c>
@@ -5609,7 +5611,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="4">
         <v>11.5</v>
       </c>
@@ -5632,7 +5634,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
         <v>4.4000000000000004</v>
       </c>
@@ -5655,7 +5657,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
         <v>6.5</v>
       </c>
@@ -5678,7 +5680,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
         <v>6.5</v>
       </c>
@@ -5701,7 +5703,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
         <v>5</v>
       </c>
@@ -5724,7 +5726,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="4">
         <v>6</v>
       </c>
@@ -5747,7 +5749,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="4">
         <v>8</v>
       </c>
@@ -5770,7 +5772,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="4">
         <v>3.2</v>
       </c>
@@ -5793,7 +5795,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="4">
         <v>10</v>
       </c>
@@ -5816,7 +5818,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="4">
         <v>3</v>
       </c>
@@ -5839,7 +5841,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="4">
         <v>10</v>
       </c>
@@ -5862,7 +5864,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="4">
         <v>3.5</v>
       </c>
@@ -5885,7 +5887,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="4">
         <v>10</v>
       </c>
@@ -5908,7 +5910,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="4">
         <v>8</v>
       </c>
@@ -5931,7 +5933,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="4">
         <v>6.2</v>
       </c>
@@ -5954,7 +5956,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="4">
         <v>2</v>
       </c>
@@ -5977,7 +5979,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="4">
         <v>10</v>
       </c>
@@ -6000,7 +6002,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="4">
         <v>22</v>
       </c>
@@ -6023,7 +6025,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="4">
         <v>14</v>
       </c>
@@ -6046,7 +6048,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="194" spans="1:8">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="4">
         <v>14</v>
       </c>
@@ -6069,7 +6071,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="195" spans="1:8">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="4">
         <v>4.7</v>
       </c>
@@ -6092,7 +6094,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="196" spans="1:8">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="4">
         <v>69.900000000000006</v>
       </c>
@@ -6115,7 +6117,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="197" spans="1:8">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="4">
         <v>8.4</v>
       </c>
@@ -6138,7 +6140,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="4">
         <v>5</v>
       </c>
@@ -6161,7 +6163,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="4">
         <v>4.5</v>
       </c>
@@ -6184,7 +6186,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="200" spans="1:8">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="4">
         <v>6</v>
       </c>
@@ -6207,7 +6209,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
         <v>5.46</v>
       </c>
@@ -6230,7 +6232,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="4">
         <v>78.849999999999994</v>
       </c>
@@ -6253,7 +6255,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="203" spans="1:8">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="4">
         <v>10</v>
       </c>
@@ -6276,7 +6278,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="204" spans="1:8">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="4">
         <v>10</v>
       </c>
@@ -6299,7 +6301,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="205" spans="1:8">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="4">
         <v>26</v>
       </c>
@@ -6322,7 +6324,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="206" spans="1:8">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="4">
         <v>2</v>
       </c>
@@ -6345,7 +6347,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="207" spans="1:8">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="4">
         <v>2.5</v>
       </c>
@@ -6368,7 +6370,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="4">
         <v>5.9</v>
       </c>
@@ -6391,7 +6393,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="209" spans="1:8">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="4">
         <v>8.6</v>
       </c>
@@ -6414,7 +6416,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="210" spans="1:8">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="4">
         <v>2.7</v>
       </c>
@@ -6437,7 +6439,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="211" spans="1:8">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="4">
         <v>4.8</v>
       </c>
@@ -6460,7 +6462,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="212" spans="1:8">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="4">
         <v>2.8</v>
       </c>
@@ -6483,7 +6485,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="213" spans="1:8">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="4">
         <v>2</v>
       </c>
@@ -6506,7 +6508,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="214" spans="1:8">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="4">
         <v>5</v>
       </c>
@@ -6529,7 +6531,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="215" spans="1:8">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="4">
         <v>2.5</v>
       </c>
@@ -6552,7 +6554,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="216" spans="1:8">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="4">
         <v>3.5</v>
       </c>
@@ -6575,7 +6577,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="217" spans="1:8">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="4">
         <v>1.8</v>
       </c>
@@ -6598,7 +6600,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="218" spans="1:8">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="4">
         <v>4</v>
       </c>
@@ -6621,7 +6623,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="219" spans="1:8">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="4">
         <v>6</v>
       </c>
@@ -6644,7 +6646,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="220" spans="1:8">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="4">
         <v>1.8</v>
       </c>
@@ -6667,7 +6669,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="221" spans="1:8">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="4">
         <v>5</v>
       </c>
@@ -6690,7 +6692,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="222" spans="1:8">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="4">
         <v>5</v>
       </c>
@@ -6713,7 +6715,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="223" spans="1:8">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="4">
         <v>4.7</v>
       </c>
@@ -6736,7 +6738,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="224" spans="1:8">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="4">
         <v>5</v>
       </c>
@@ -6759,7 +6761,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="225" spans="1:8">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="4">
         <v>10</v>
       </c>
@@ -6782,7 +6784,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="226" spans="1:8">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="4">
         <v>1.5</v>
       </c>
@@ -6805,7 +6807,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="227" spans="1:8">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="4">
         <v>129</v>
       </c>
@@ -6828,7 +6830,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="228" spans="1:8">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="4">
         <v>7</v>
       </c>
@@ -6851,7 +6853,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="229" spans="1:8">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="4">
         <v>2.8</v>
       </c>
@@ -6874,7 +6876,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="230" spans="1:8">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="4">
         <v>1</v>
       </c>
@@ -6897,7 +6899,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="231" spans="1:8">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" s="4">
         <v>4</v>
       </c>
@@ -6920,7 +6922,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="232" spans="1:8">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="4">
         <v>50</v>
       </c>
@@ -6943,7 +6945,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="233" spans="1:8">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="4">
         <v>7.2</v>
       </c>
@@ -6966,7 +6968,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="234" spans="1:8">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" s="4">
         <v>1</v>
       </c>
@@ -6989,7 +6991,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="235" spans="1:8">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" s="4">
         <v>7</v>
       </c>
@@ -7012,7 +7014,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="236" spans="1:8">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -7035,7 +7037,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="237" spans="1:8">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="4">
         <v>7</v>
       </c>
@@ -7058,7 +7060,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="238" spans="1:8">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" s="4">
         <v>15</v>
       </c>
@@ -7081,7 +7083,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="239" spans="1:8">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" s="4">
         <v>3</v>
       </c>
@@ -7104,7 +7106,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="240" spans="1:8">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="4">
         <v>11.2</v>
       </c>
@@ -7127,7 +7129,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="241" spans="1:8">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="4">
         <v>2.1</v>
       </c>
@@ -7150,7 +7152,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="242" spans="1:8">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="4">
         <v>150</v>
       </c>
@@ -7173,7 +7175,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="243" spans="1:8">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="4">
         <v>12.7</v>
       </c>
@@ -7196,7 +7198,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="244" spans="1:8">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" s="4">
         <v>89.9</v>
       </c>
@@ -7219,7 +7221,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="245" spans="1:8">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="4">
         <v>4.4000000000000004</v>
       </c>
@@ -7242,7 +7244,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="246" spans="1:8">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="4">
         <v>4.2</v>
       </c>
@@ -7265,7 +7267,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="247" spans="1:8">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -7288,7 +7290,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="248" spans="1:8">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="4">
         <v>5</v>
       </c>
@@ -7311,7 +7313,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="249" spans="1:8">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="4">
         <v>5</v>
       </c>
@@ -7334,7 +7336,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="250" spans="1:8">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="4">
         <v>3.9</v>
       </c>
@@ -7357,7 +7359,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="251" spans="1:8">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="4">
         <v>0.5</v>
       </c>
@@ -7380,7 +7382,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="252" spans="1:8">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="4">
         <v>2.4</v>
       </c>
@@ -7403,7 +7405,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:8">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" s="4">
         <v>2</v>
       </c>
@@ -7426,7 +7428,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="254" spans="1:8">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" s="4">
         <v>4.7</v>
       </c>
@@ -7449,7 +7451,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="255" spans="1:8">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="4">
         <v>5.3</v>
       </c>
@@ -7472,7 +7474,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="256" spans="1:8">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="4">
         <v>4.2</v>
       </c>
@@ -7495,7 +7497,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="257" spans="1:8">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" s="4">
         <v>5</v>
       </c>
@@ -7518,7 +7520,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="258" spans="1:8">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" s="4">
         <v>2.5</v>
       </c>
@@ -7541,7 +7543,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:8">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" s="4">
         <v>3.3</v>
       </c>
@@ -7564,7 +7566,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="260" spans="1:8">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" s="4">
         <v>5.6</v>
       </c>
@@ -7587,7 +7589,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="261" spans="1:8">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" s="4">
         <v>4</v>
       </c>
@@ -7610,7 +7612,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="262" spans="1:8">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262" s="4">
         <v>10.199999999999999</v>
       </c>
@@ -7633,7 +7635,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="263" spans="1:8">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" s="4">
         <v>8</v>
       </c>
@@ -7656,7 +7658,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="264" spans="1:8">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264" s="4">
         <v>2.1</v>
       </c>
@@ -7679,7 +7681,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="265" spans="1:8">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265" s="4">
         <v>3.7</v>
       </c>
@@ -7702,7 +7704,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="266" spans="1:8">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266" s="4">
         <v>7</v>
       </c>
@@ -7725,7 +7727,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="267" spans="1:8">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267" s="4">
         <v>13.5</v>
       </c>
@@ -7748,7 +7750,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="268" spans="1:8">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268" s="4">
         <v>5</v>
       </c>
@@ -7771,7 +7773,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="269" spans="1:8">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269" s="4">
         <v>20</v>
       </c>
@@ -7794,7 +7796,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="270" spans="1:8">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270" s="4">
         <v>6</v>
       </c>
@@ -7817,7 +7819,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="271" spans="1:8">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271" s="4">
         <v>0.5</v>
       </c>
@@ -7840,7 +7842,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="272" spans="1:8">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272" s="4">
         <v>5</v>
       </c>
@@ -7863,7 +7865,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="273" spans="1:8">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" s="4">
         <v>11</v>
       </c>
@@ -7886,7 +7888,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="274" spans="1:8">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" s="4">
         <v>8.8000000000000007</v>
       </c>
@@ -7909,7 +7911,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="275" spans="1:8">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="4">
         <v>0.5</v>
       </c>
@@ -7932,7 +7934,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="276" spans="1:8">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="4">
         <v>5</v>
       </c>
@@ -7955,7 +7957,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="277" spans="1:8">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="4">
         <v>10</v>
       </c>
@@ -7978,7 +7980,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="278" spans="1:8">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="4">
         <v>15</v>
       </c>
@@ -8001,7 +8003,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="279" spans="1:8">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" s="4">
         <v>10</v>
       </c>
@@ -8024,7 +8026,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="280" spans="1:8">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280" s="4">
         <v>11.9</v>
       </c>
@@ -8047,7 +8049,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="281" spans="1:8">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281" s="4">
         <v>7</v>
       </c>
@@ -8070,7 +8072,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="282" spans="1:8">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -8093,7 +8095,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="283" spans="1:8">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>1.9</v>
       </c>
@@ -8116,7 +8118,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="284" spans="1:8">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>119.9</v>
       </c>
@@ -8139,7 +8141,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="285" spans="1:8">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>6.3</v>
       </c>
@@ -8162,7 +8164,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="286" spans="1:8">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>3.5</v>
       </c>
@@ -8185,7 +8187,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="287" spans="1:8">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>1.5</v>
       </c>
@@ -8208,7 +8210,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="288" spans="1:8">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>1.9</v>
       </c>
@@ -8231,7 +8233,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="289" spans="1:8">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>4.5</v>
       </c>
@@ -8254,7 +8256,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="290" spans="1:8">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>6.4</v>
       </c>
@@ -8277,7 +8279,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="291" spans="1:8">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>1.9</v>
       </c>
@@ -8300,7 +8302,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="292" spans="1:8">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>10.6</v>
       </c>
@@ -8323,7 +8325,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="293" spans="1:8">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>4.5</v>
       </c>
@@ -8346,7 +8348,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="294" spans="1:8">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>22.2</v>
       </c>
@@ -8369,7 +8371,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="295" spans="1:8">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295" s="6">
         <v>25</v>
       </c>
@@ -8392,7 +8394,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="296" spans="1:8">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A296" s="6">
         <v>3.5</v>
       </c>
@@ -8415,7 +8417,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="297" spans="1:8">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>4</v>
       </c>
@@ -8438,7 +8440,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="298" spans="1:8">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>2.2000000000000002</v>
       </c>
@@ -8461,7 +8463,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="299" spans="1:8">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>11.5</v>
       </c>
@@ -8484,7 +8486,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="300" spans="1:8">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>6.3</v>
       </c>
@@ -8507,7 +8509,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="301" spans="1:8">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>3.6</v>
       </c>
@@ -8530,7 +8532,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="302" spans="1:8">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>15</v>
       </c>
@@ -8553,7 +8555,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="303" spans="1:8">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>2</v>
       </c>
@@ -8576,7 +8578,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="304" spans="1:8">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>4.5</v>
       </c>
@@ -8599,7 +8601,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="305" spans="1:8">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>2.9</v>
       </c>
@@ -8622,7 +8624,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="306" spans="1:8">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>3.9</v>
       </c>
@@ -8645,7 +8647,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="307" spans="1:8">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>1.7</v>
       </c>
@@ -8668,7 +8670,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="308" spans="1:8">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>10</v>
       </c>
@@ -8691,7 +8693,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="309" spans="1:8">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>7.5</v>
       </c>
@@ -8714,7 +8716,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="310" spans="1:8">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>10.050000000000001</v>
       </c>
@@ -8737,7 +8739,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="311" spans="1:8">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>5</v>
       </c>
@@ -8760,7 +8762,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="312" spans="1:8">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>3</v>
       </c>
@@ -8783,7 +8785,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="313" spans="1:8">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>2</v>
       </c>
@@ -8806,7 +8808,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="314" spans="1:8">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>10.6</v>
       </c>
@@ -8829,7 +8831,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="315" spans="1:8">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>4</v>
       </c>
@@ -8852,7 +8854,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="316" spans="1:8">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>2</v>
       </c>
@@ -8875,7 +8877,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="317" spans="1:8">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>5.8</v>
       </c>
@@ -8898,7 +8900,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="318" spans="1:8">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>5</v>
       </c>
@@ -8921,7 +8923,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="319" spans="1:8">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>6.55</v>
       </c>
@@ -8944,7 +8946,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="320" spans="1:8">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>2.8</v>
       </c>
@@ -8967,7 +8969,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="321" spans="1:8">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>3.8</v>
       </c>
@@ -8990,7 +8992,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="322" spans="1:8">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>9</v>
       </c>
@@ -9013,7 +9015,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="323" spans="1:8">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>8</v>
       </c>
@@ -9036,7 +9038,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="324" spans="1:8">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>1.5</v>
       </c>
@@ -9059,7 +9061,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="325" spans="1:8">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>5</v>
       </c>
@@ -9082,7 +9084,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="326" spans="1:8">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>4.5999999999999996</v>
       </c>
@@ -9105,7 +9107,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="327" spans="1:8">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>0.5</v>
       </c>
@@ -9128,7 +9130,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="328" spans="1:8">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>2.95</v>
       </c>
@@ -9151,7 +9153,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="329" spans="1:8">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>3.8</v>
       </c>
@@ -9174,7 +9176,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="330" spans="1:8">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>10</v>
       </c>
@@ -9197,7 +9199,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="331" spans="1:8">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>3.85</v>
       </c>
@@ -9220,7 +9222,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="332" spans="1:8">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>1.2</v>
       </c>
@@ -9243,7 +9245,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="333" spans="1:8">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>2</v>
       </c>
@@ -9266,7 +9268,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="334" spans="1:8">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>8.5</v>
       </c>
@@ -9289,7 +9291,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="335" spans="1:8">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>4.9000000000000004</v>
       </c>
@@ -9312,7 +9314,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="336" spans="1:8">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>10</v>
       </c>
@@ -9335,7 +9337,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="337" spans="1:8">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>1.5</v>
       </c>
@@ -9355,7 +9357,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="338" spans="1:8">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>350</v>
       </c>
@@ -9378,7 +9380,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="339" spans="1:8">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>4.4000000000000004</v>
       </c>
@@ -9401,7 +9403,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="340" spans="1:8">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>3.2</v>
       </c>
@@ -9424,7 +9426,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="341" spans="1:8">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>3.8</v>
       </c>
@@ -9447,7 +9449,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="342" spans="1:8">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>0.9</v>
       </c>
@@ -9470,7 +9472,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="343" spans="1:8">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>6</v>
       </c>
@@ -9493,7 +9495,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="344" spans="1:8">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>3.8</v>
       </c>
@@ -9516,7 +9518,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="345" spans="1:8">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>2</v>
       </c>
@@ -9539,7 +9541,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="346" spans="1:8">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>5.5</v>
       </c>
@@ -9562,7 +9564,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="347" spans="1:8">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>43.22</v>
       </c>
@@ -9585,7 +9587,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="348" spans="1:8">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>2</v>
       </c>
@@ -9608,7 +9610,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="349" spans="1:8">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>7</v>
       </c>
@@ -9631,7 +9633,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="350" spans="1:8">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>1.61</v>
       </c>
@@ -9654,7 +9656,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="351" spans="1:8">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>20</v>
       </c>
@@ -9677,7 +9679,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="352" spans="1:8">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>14.84</v>
       </c>
@@ -9700,7 +9702,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="353" spans="1:12">
+    <row r="353" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>5.6</v>
       </c>
@@ -9723,7 +9725,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="354" spans="1:12">
+    <row r="354" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>6.8</v>
       </c>
@@ -9746,7 +9748,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="355" spans="1:12">
+    <row r="355" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>7.7</v>
       </c>
@@ -9769,7 +9771,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="356" spans="1:12">
+    <row r="356" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>29.4</v>
       </c>
@@ -9792,7 +9794,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="357" spans="1:12">
+    <row r="357" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>0.5</v>
       </c>
@@ -9815,7 +9817,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="358" spans="1:12">
+    <row r="358" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>2.2000000000000002</v>
       </c>
@@ -9838,7 +9840,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="359" spans="1:12">
+    <row r="359" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>3.5</v>
       </c>
@@ -9861,7 +9863,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="360" spans="1:12">
+    <row r="360" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>4.4000000000000004</v>
       </c>
@@ -9884,7 +9886,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="361" spans="1:12">
+    <row r="361" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>5.7</v>
       </c>
@@ -9907,7 +9909,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="362" spans="1:12">
+    <row r="362" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>7.74</v>
       </c>
@@ -9930,7 +9932,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="363" spans="1:12">
+    <row r="363" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>7</v>
       </c>
@@ -9953,7 +9955,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="364" spans="1:12">
+    <row r="364" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>3.8</v>
       </c>
@@ -9976,7 +9978,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="365" spans="1:12">
+    <row r="365" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>100</v>
       </c>
@@ -9999,7 +10001,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="366" spans="1:12">
+    <row r="366" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>5</v>
       </c>
@@ -10023,7 +10025,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="367" spans="1:12">
+    <row r="367" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A367" s="6">
         <v>2</v>
       </c>
@@ -10050,7 +10052,7 @@
       <c r="K367" s="1"/>
       <c r="L367" s="1"/>
     </row>
-    <row r="368" spans="1:12">
+    <row r="368" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>7</v>
       </c>
@@ -10073,7 +10075,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="369" spans="1:8">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>10</v>
       </c>
@@ -10096,7 +10098,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="370" spans="1:8">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>10.8</v>
       </c>
@@ -10119,7 +10121,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="371" spans="1:8">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>10.5</v>
       </c>
@@ -10142,7 +10144,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="372" spans="1:8">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>5.5</v>
       </c>
@@ -10165,7 +10167,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="373" spans="1:8">
+    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>5</v>
       </c>
@@ -10188,7 +10190,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="374" spans="1:8">
+    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>0.5</v>
       </c>
@@ -10211,7 +10213,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="375" spans="1:8">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>10.5</v>
       </c>
@@ -10234,7 +10236,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="376" spans="1:8">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>14</v>
       </c>
@@ -10257,7 +10259,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="377" spans="1:8">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>2</v>
       </c>
@@ -10280,7 +10282,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="378" spans="1:8">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>3.5</v>
       </c>
@@ -10303,7 +10305,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="379" spans="1:8">
+    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>3.5</v>
       </c>
@@ -10326,7 +10328,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="380" spans="1:8">
+    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>3.5</v>
       </c>
@@ -10349,7 +10351,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="381" spans="1:8">
+    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>2</v>
       </c>
@@ -10372,7 +10374,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="382" spans="1:8">
+    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>2</v>
       </c>
@@ -10395,7 +10397,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="383" spans="1:8">
+    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>2.5</v>
       </c>
@@ -10418,7 +10420,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="384" spans="1:8">
+    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>6.5</v>
       </c>
@@ -10441,7 +10443,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="385" spans="1:8">
+    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>3.78</v>
       </c>
@@ -10464,7 +10466,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="386" spans="1:8">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>7</v>
       </c>
@@ -10487,7 +10489,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="387" spans="1:8">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>2.5</v>
       </c>
@@ -10510,7 +10512,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="388" spans="1:8">
+    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>2</v>
       </c>
@@ -10533,7 +10535,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="389" spans="1:8">
+    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>1</v>
       </c>
@@ -10556,7 +10558,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="390" spans="1:8">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>10.5</v>
       </c>
@@ -10579,7 +10581,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="391" spans="1:8">
+    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>1.5</v>
       </c>
@@ -10602,7 +10604,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="392" spans="1:8">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>2.7</v>
       </c>
@@ -10625,7 +10627,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="393" spans="1:8">
+    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>2</v>
       </c>
@@ -10648,7 +10650,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="394" spans="1:8">
+    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>17.5</v>
       </c>
@@ -10671,7 +10673,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="518" spans="1:8">
+    <row r="518" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A518" s="1"/>
       <c r="B518" s="1"/>
       <c r="C518" s="1"/>

</xml_diff>

<commit_message>
Starting the same project in C#
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1575" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="398">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1205,6 +1205,9 @@
   </si>
   <si>
     <t>μπύρα (+ Ανέστη, + Ηλία, +Βαγγέλη, + Σταύρου)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ακουστικά </t>
   </si>
 </sst>
 </file>
@@ -1641,7 +1644,7 @@
   <dimension ref="A1:L518"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A387" workbookViewId="0">
-      <selection activeCell="C399" sqref="C399"/>
+      <selection activeCell="D396" sqref="D396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10704,6 +10707,9 @@
       <c r="C396" s="2">
         <v>43332</v>
       </c>
+      <c r="D396" t="s">
+        <v>397</v>
+      </c>
       <c r="E396" t="s">
         <v>238</v>
       </c>

</xml_diff>

<commit_message>
Create functionality to add values to the database
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11760"/>
@@ -1213,12 +1213,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1259,7 +1259,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -1340,8 +1340,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A1:H518" totalsRowShown="0">
-  <autoFilter ref="A1:H518"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A1:H396" totalsRowShown="0">
+  <autoFilter ref="A1:H396"/>
   <tableColumns count="8">
     <tableColumn id="1" name="amount" totalsRowDxfId="7"/>
     <tableColumn id="11" name="type" totalsRowDxfId="6"/>
@@ -1357,7 +1357,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1399,7 +1399,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1431,9 +1431,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1465,6 +1466,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1640,14 +1642,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L518"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L396"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A387" workbookViewId="0">
-      <selection activeCell="D396" sqref="D396"/>
+    <sheetView tabSelected="1" topLeftCell="A370" workbookViewId="0">
+      <selection activeCell="J394" sqref="J394"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
@@ -1663,7 +1665,7 @@
     <col min="12" max="12" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>235</v>
       </c>
@@ -1692,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>20</v>
       </c>
@@ -1716,7 +1718,7 @@
       </c>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>10</v>
       </c>
@@ -1739,7 +1741,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>100</v>
       </c>
@@ -1762,7 +1764,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>10</v>
       </c>
@@ -1785,7 +1787,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>50</v>
       </c>
@@ -1808,7 +1810,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>3.2</v>
       </c>
@@ -1831,7 +1833,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>1.3</v>
       </c>
@@ -1854,7 +1856,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1.2</v>
       </c>
@@ -1877,7 +1879,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>5</v>
       </c>
@@ -1900,7 +1902,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>4.5</v>
       </c>
@@ -1923,7 +1925,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>4</v>
       </c>
@@ -1946,7 +1948,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>10.6</v>
       </c>
@@ -1969,7 +1971,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>1.8</v>
       </c>
@@ -1992,7 +1994,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>5.15</v>
       </c>
@@ -2015,7 +2017,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>18</v>
       </c>
@@ -2038,7 +2040,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>1.5</v>
       </c>
@@ -2061,7 +2063,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>7.8</v>
       </c>
@@ -2084,7 +2086,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>4.4400000000000004</v>
       </c>
@@ -2107,7 +2109,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>1.5</v>
       </c>
@@ -2130,7 +2132,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>8.84</v>
       </c>
@@ -2153,7 +2155,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>4</v>
       </c>
@@ -2176,7 +2178,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>10</v>
       </c>
@@ -2199,7 +2201,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>1.8</v>
       </c>
@@ -2222,7 +2224,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>11.8</v>
       </c>
@@ -2245,7 +2247,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>40</v>
       </c>
@@ -2268,7 +2270,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>2.9</v>
       </c>
@@ -2291,7 +2293,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>4.3</v>
       </c>
@@ -2314,7 +2316,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>3.35</v>
       </c>
@@ -2337,7 +2339,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>5.2</v>
       </c>
@@ -2360,7 +2362,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>15</v>
       </c>
@@ -2383,7 +2385,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>3.9</v>
       </c>
@@ -2406,7 +2408,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>63.45</v>
       </c>
@@ -2429,7 +2431,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>49.9</v>
       </c>
@@ -2449,7 +2451,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>140</v>
       </c>
@@ -2472,7 +2474,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>1.8</v>
       </c>
@@ -2495,7 +2497,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>13.02</v>
       </c>
@@ -2518,7 +2520,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>4.7</v>
       </c>
@@ -2541,7 +2543,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>15.96</v>
       </c>
@@ -2564,7 +2566,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>9.8000000000000007</v>
       </c>
@@ -2587,7 +2589,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>79.8</v>
       </c>
@@ -2610,7 +2612,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>11.9</v>
       </c>
@@ -2633,7 +2635,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>38.880000000000003</v>
       </c>
@@ -2656,7 +2658,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>7.75</v>
       </c>
@@ -2679,7 +2681,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>0.79</v>
       </c>
@@ -2702,7 +2704,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>10</v>
       </c>
@@ -2725,7 +2727,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -2748,7 +2750,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -2771,7 +2773,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>1.8</v>
       </c>
@@ -2794,7 +2796,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>24</v>
       </c>
@@ -2817,7 +2819,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>24</v>
       </c>
@@ -2840,7 +2842,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>1.8</v>
       </c>
@@ -2863,7 +2865,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>3.5</v>
       </c>
@@ -2886,7 +2888,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>5.6</v>
       </c>
@@ -2910,7 +2912,7 @@
       </c>
       <c r="K54" s="4"/>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>1.5</v>
       </c>
@@ -2933,7 +2935,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>3</v>
       </c>
@@ -2956,7 +2958,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>5.4</v>
       </c>
@@ -2979,7 +2981,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>8</v>
       </c>
@@ -3002,7 +3004,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>5.4</v>
       </c>
@@ -3025,7 +3027,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>0.6</v>
       </c>
@@ -3048,7 +3050,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3071,7 +3073,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>1.5</v>
       </c>
@@ -3094,7 +3096,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3117,7 +3119,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>1.2</v>
       </c>
@@ -3140,7 +3142,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -3163,7 +3165,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>13.5</v>
       </c>
@@ -3186,7 +3188,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>3.5</v>
       </c>
@@ -3210,7 +3212,7 @@
       </c>
       <c r="K67" s="4"/>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>4.0999999999999996</v>
       </c>
@@ -3233,7 +3235,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>90</v>
       </c>
@@ -3256,7 +3258,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>65.5</v>
       </c>
@@ -3279,7 +3281,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>4.5</v>
       </c>
@@ -3302,7 +3304,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>10</v>
       </c>
@@ -3325,7 +3327,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>18.8</v>
       </c>
@@ -3348,7 +3350,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>1.8</v>
       </c>
@@ -3372,7 +3374,7 @@
       </c>
       <c r="K74" s="4"/>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>5.5</v>
       </c>
@@ -3395,7 +3397,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3418,7 +3420,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>3</v>
       </c>
@@ -3441,7 +3443,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>2</v>
       </c>
@@ -3464,7 +3466,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>9.9</v>
       </c>
@@ -3487,7 +3489,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>6.5</v>
       </c>
@@ -3510,7 +3512,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>79.8</v>
       </c>
@@ -3533,7 +3535,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>10</v>
       </c>
@@ -3556,7 +3558,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>2.5</v>
       </c>
@@ -3579,7 +3581,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>5</v>
       </c>
@@ -3602,7 +3604,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>1.6</v>
       </c>
@@ -3625,7 +3627,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>5.5</v>
       </c>
@@ -3648,7 +3650,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>0.8</v>
       </c>
@@ -3671,7 +3673,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>17</v>
       </c>
@@ -3694,7 +3696,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>24.9</v>
       </c>
@@ -3717,7 +3719,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>1.8</v>
       </c>
@@ -3740,7 +3742,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>44.99</v>
       </c>
@@ -3763,7 +3765,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>4</v>
       </c>
@@ -3786,7 +3788,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>5</v>
       </c>
@@ -3809,7 +3811,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>5</v>
       </c>
@@ -3832,13 +3834,13 @@
         <v>268</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3861,7 +3863,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>3</v>
       </c>
@@ -3884,7 +3886,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>6</v>
       </c>
@@ -3907,7 +3909,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>3.5</v>
       </c>
@@ -3930,7 +3932,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>34.9</v>
       </c>
@@ -3953,7 +3955,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>12</v>
       </c>
@@ -3976,10 +3978,10 @@
         <v>242</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>5</v>
       </c>
@@ -4002,7 +4004,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>6.9</v>
       </c>
@@ -4025,7 +4027,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>6.04</v>
       </c>
@@ -4048,7 +4050,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>4.8</v>
       </c>
@@ -4071,7 +4073,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>9.6999999999999993</v>
       </c>
@@ -4094,7 +4096,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>5.5</v>
       </c>
@@ -4117,7 +4119,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>7</v>
       </c>
@@ -4140,7 +4142,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>1</v>
       </c>
@@ -4163,7 +4165,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>4</v>
       </c>
@@ -4186,7 +4188,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>4.0999999999999996</v>
       </c>
@@ -4209,7 +4211,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>2.3199999999999998</v>
       </c>
@@ -4232,7 +4234,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>8</v>
       </c>
@@ -4255,7 +4257,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>12.5</v>
       </c>
@@ -4278,7 +4280,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>0.7</v>
       </c>
@@ -4301,7 +4303,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>6.3</v>
       </c>
@@ -4324,7 +4326,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>8</v>
       </c>
@@ -4347,7 +4349,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -4370,7 +4372,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>8</v>
       </c>
@@ -4393,7 +4395,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>4.5</v>
       </c>
@@ -4416,7 +4418,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>2.5</v>
       </c>
@@ -4439,7 +4441,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>24.3</v>
       </c>
@@ -4462,7 +4464,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>2</v>
       </c>
@@ -4485,7 +4487,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>16</v>
       </c>
@@ -4508,7 +4510,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>6</v>
       </c>
@@ -4531,7 +4533,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>5</v>
       </c>
@@ -4554,7 +4556,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>6.52</v>
       </c>
@@ -4577,7 +4579,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>1.8</v>
       </c>
@@ -4600,7 +4602,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>1</v>
       </c>
@@ -4623,7 +4625,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>5</v>
       </c>
@@ -4646,7 +4648,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
         <v>43</v>
       </c>
@@ -4669,7 +4671,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>10</v>
       </c>
@@ -4692,7 +4694,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>2.97</v>
       </c>
@@ -4715,7 +4717,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>10</v>
       </c>
@@ -4738,7 +4740,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>1.6</v>
       </c>
@@ -4761,7 +4763,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>1.5</v>
       </c>
@@ -4784,7 +4786,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>1.8</v>
       </c>
@@ -4807,7 +4809,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>7.3</v>
       </c>
@@ -4830,7 +4832,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>4</v>
       </c>
@@ -4853,7 +4855,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <v>2.1</v>
       </c>
@@ -4876,7 +4878,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>4.2</v>
       </c>
@@ -4899,7 +4901,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>9</v>
       </c>
@@ -4922,7 +4924,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <v>1</v>
       </c>
@@ -4945,7 +4947,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>3.5</v>
       </c>
@@ -4968,7 +4970,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -4991,7 +4993,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>3</v>
       </c>
@@ -5014,7 +5016,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>2</v>
       </c>
@@ -5037,7 +5039,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>150</v>
       </c>
@@ -5060,7 +5062,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
         <v>7</v>
       </c>
@@ -5083,7 +5085,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>5</v>
       </c>
@@ -5106,7 +5108,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
         <v>8</v>
       </c>
@@ -5129,7 +5131,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="4">
         <v>3.5</v>
       </c>
@@ -5152,7 +5154,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="4">
         <v>55</v>
       </c>
@@ -5175,7 +5177,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="4">
         <v>0.6</v>
       </c>
@@ -5198,7 +5200,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="4">
         <v>4</v>
       </c>
@@ -5221,7 +5223,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="4">
         <v>39.9</v>
       </c>
@@ -5244,7 +5246,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="4">
         <v>1.6</v>
       </c>
@@ -5267,7 +5269,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="4">
         <v>80</v>
       </c>
@@ -5290,7 +5292,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>6.2</v>
       </c>
@@ -5313,7 +5315,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="4">
         <v>15</v>
       </c>
@@ -5336,7 +5338,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="4">
         <v>4.3</v>
       </c>
@@ -5359,7 +5361,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="4">
         <v>9.6999999999999993</v>
       </c>
@@ -5382,7 +5384,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="4">
         <v>2.4500000000000002</v>
       </c>
@@ -5405,7 +5407,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="4">
         <v>1.96</v>
       </c>
@@ -5428,7 +5430,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="4">
         <v>11.5</v>
       </c>
@@ -5451,7 +5453,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="4">
         <v>2.7</v>
       </c>
@@ -5474,7 +5476,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="4">
         <v>2.7</v>
       </c>
@@ -5497,7 +5499,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="4">
         <v>7</v>
       </c>
@@ -5520,7 +5522,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="4">
         <v>4.8</v>
       </c>
@@ -5543,7 +5545,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
         <v>4.4000000000000004</v>
       </c>
@@ -5566,7 +5568,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="4">
         <v>3.8</v>
       </c>
@@ -5589,7 +5591,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
         <v>1.5</v>
       </c>
@@ -5612,7 +5614,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="4">
         <v>11.5</v>
       </c>
@@ -5635,7 +5637,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
         <v>4.4000000000000004</v>
       </c>
@@ -5658,7 +5660,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
         <v>6.5</v>
       </c>
@@ -5681,7 +5683,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
         <v>6.5</v>
       </c>
@@ -5704,7 +5706,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
         <v>5</v>
       </c>
@@ -5727,7 +5729,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="4">
         <v>6</v>
       </c>
@@ -5750,7 +5752,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="4">
         <v>8</v>
       </c>
@@ -5773,7 +5775,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="4">
         <v>3.2</v>
       </c>
@@ -5796,7 +5798,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="4">
         <v>10</v>
       </c>
@@ -5819,7 +5821,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="4">
         <v>3</v>
       </c>
@@ -5842,7 +5844,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="4">
         <v>10</v>
       </c>
@@ -5865,7 +5867,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="4">
         <v>3.5</v>
       </c>
@@ -5888,7 +5890,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="4">
         <v>10</v>
       </c>
@@ -5911,7 +5913,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="4">
         <v>8</v>
       </c>
@@ -5934,7 +5936,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="4">
         <v>6.2</v>
       </c>
@@ -5957,7 +5959,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="4">
         <v>2</v>
       </c>
@@ -5980,7 +5982,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="4">
         <v>10</v>
       </c>
@@ -6003,7 +6005,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="4">
         <v>22</v>
       </c>
@@ -6026,7 +6028,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="4">
         <v>14</v>
       </c>
@@ -6049,7 +6051,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="194" spans="1:8">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="4">
         <v>14</v>
       </c>
@@ -6072,7 +6074,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="195" spans="1:8">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="4">
         <v>4.7</v>
       </c>
@@ -6095,7 +6097,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="196" spans="1:8">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="4">
         <v>69.900000000000006</v>
       </c>
@@ -6118,7 +6120,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="197" spans="1:8">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="4">
         <v>8.4</v>
       </c>
@@ -6141,7 +6143,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="4">
         <v>5</v>
       </c>
@@ -6164,7 +6166,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="4">
         <v>4.5</v>
       </c>
@@ -6187,7 +6189,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="200" spans="1:8">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="4">
         <v>6</v>
       </c>
@@ -6210,7 +6212,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
         <v>5.46</v>
       </c>
@@ -6233,7 +6235,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="4">
         <v>78.849999999999994</v>
       </c>
@@ -6256,7 +6258,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="203" spans="1:8">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="4">
         <v>10</v>
       </c>
@@ -6279,7 +6281,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="204" spans="1:8">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="4">
         <v>10</v>
       </c>
@@ -6302,7 +6304,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="205" spans="1:8">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="4">
         <v>26</v>
       </c>
@@ -6325,7 +6327,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="206" spans="1:8">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="4">
         <v>2</v>
       </c>
@@ -6348,7 +6350,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="207" spans="1:8">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="4">
         <v>2.5</v>
       </c>
@@ -6371,7 +6373,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="4">
         <v>5.9</v>
       </c>
@@ -6394,7 +6396,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="209" spans="1:8">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="4">
         <v>8.6</v>
       </c>
@@ -6417,7 +6419,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="210" spans="1:8">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="4">
         <v>2.7</v>
       </c>
@@ -6440,7 +6442,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="211" spans="1:8">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="4">
         <v>4.8</v>
       </c>
@@ -6463,7 +6465,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="212" spans="1:8">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="4">
         <v>2.8</v>
       </c>
@@ -6486,7 +6488,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="213" spans="1:8">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="4">
         <v>2</v>
       </c>
@@ -6509,7 +6511,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="214" spans="1:8">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="4">
         <v>5</v>
       </c>
@@ -6532,7 +6534,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="215" spans="1:8">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="4">
         <v>2.5</v>
       </c>
@@ -6555,7 +6557,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="216" spans="1:8">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="4">
         <v>3.5</v>
       </c>
@@ -6578,7 +6580,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="217" spans="1:8">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="4">
         <v>1.8</v>
       </c>
@@ -6601,7 +6603,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="218" spans="1:8">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="4">
         <v>4</v>
       </c>
@@ -6624,7 +6626,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="219" spans="1:8">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="4">
         <v>6</v>
       </c>
@@ -6647,7 +6649,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="220" spans="1:8">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="4">
         <v>1.8</v>
       </c>
@@ -6670,7 +6672,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="221" spans="1:8">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="4">
         <v>5</v>
       </c>
@@ -6693,7 +6695,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="222" spans="1:8">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="4">
         <v>5</v>
       </c>
@@ -6716,7 +6718,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="223" spans="1:8">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="4">
         <v>4.7</v>
       </c>
@@ -6739,7 +6741,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="224" spans="1:8">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="4">
         <v>5</v>
       </c>
@@ -6762,7 +6764,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="225" spans="1:8">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="4">
         <v>10</v>
       </c>
@@ -6785,7 +6787,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="226" spans="1:8">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="4">
         <v>1.5</v>
       </c>
@@ -6808,7 +6810,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="227" spans="1:8">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="4">
         <v>129</v>
       </c>
@@ -6831,7 +6833,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="228" spans="1:8">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="4">
         <v>7</v>
       </c>
@@ -6854,7 +6856,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="229" spans="1:8">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="4">
         <v>2.8</v>
       </c>
@@ -6877,7 +6879,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="230" spans="1:8">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="4">
         <v>1</v>
       </c>
@@ -6900,7 +6902,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="231" spans="1:8">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" s="4">
         <v>4</v>
       </c>
@@ -6923,7 +6925,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="232" spans="1:8">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="4">
         <v>50</v>
       </c>
@@ -6946,7 +6948,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="233" spans="1:8">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="4">
         <v>7.2</v>
       </c>
@@ -6969,7 +6971,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="234" spans="1:8">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" s="4">
         <v>1</v>
       </c>
@@ -6992,7 +6994,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="235" spans="1:8">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" s="4">
         <v>7</v>
       </c>
@@ -7015,7 +7017,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="236" spans="1:8">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -7038,7 +7040,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="237" spans="1:8">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="4">
         <v>7</v>
       </c>
@@ -7061,7 +7063,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="238" spans="1:8">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" s="4">
         <v>15</v>
       </c>
@@ -7084,7 +7086,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="239" spans="1:8">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" s="4">
         <v>3</v>
       </c>
@@ -7107,7 +7109,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="240" spans="1:8">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="4">
         <v>11.2</v>
       </c>
@@ -7130,7 +7132,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="241" spans="1:8">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="4">
         <v>2.1</v>
       </c>
@@ -7153,7 +7155,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="242" spans="1:8">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="4">
         <v>150</v>
       </c>
@@ -7176,7 +7178,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="243" spans="1:8">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="4">
         <v>12.7</v>
       </c>
@@ -7199,7 +7201,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="244" spans="1:8">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" s="4">
         <v>89.9</v>
       </c>
@@ -7222,7 +7224,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="245" spans="1:8">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="4">
         <v>4.4000000000000004</v>
       </c>
@@ -7245,7 +7247,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="246" spans="1:8">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="4">
         <v>4.2</v>
       </c>
@@ -7268,7 +7270,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="247" spans="1:8">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -7291,7 +7293,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="248" spans="1:8">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="4">
         <v>5</v>
       </c>
@@ -7314,7 +7316,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="249" spans="1:8">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="4">
         <v>5</v>
       </c>
@@ -7337,7 +7339,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="250" spans="1:8">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="4">
         <v>3.9</v>
       </c>
@@ -7360,7 +7362,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="251" spans="1:8">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="4">
         <v>0.5</v>
       </c>
@@ -7383,7 +7385,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="252" spans="1:8">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="4">
         <v>2.4</v>
       </c>
@@ -7406,7 +7408,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:8">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" s="4">
         <v>2</v>
       </c>
@@ -7429,7 +7431,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="254" spans="1:8">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" s="4">
         <v>4.7</v>
       </c>
@@ -7452,7 +7454,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="255" spans="1:8">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="4">
         <v>5.3</v>
       </c>
@@ -7475,7 +7477,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="256" spans="1:8">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="4">
         <v>4.2</v>
       </c>
@@ -7498,7 +7500,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="257" spans="1:8">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" s="4">
         <v>5</v>
       </c>
@@ -7521,7 +7523,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="258" spans="1:8">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" s="4">
         <v>2.5</v>
       </c>
@@ -7544,7 +7546,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:8">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" s="4">
         <v>3.3</v>
       </c>
@@ -7567,7 +7569,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="260" spans="1:8">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" s="4">
         <v>5.6</v>
       </c>
@@ -7590,7 +7592,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="261" spans="1:8">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" s="4">
         <v>4</v>
       </c>
@@ -7613,7 +7615,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="262" spans="1:8">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262" s="4">
         <v>10.199999999999999</v>
       </c>
@@ -7636,7 +7638,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="263" spans="1:8">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" s="4">
         <v>8</v>
       </c>
@@ -7659,7 +7661,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="264" spans="1:8">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264" s="4">
         <v>2.1</v>
       </c>
@@ -7682,7 +7684,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="265" spans="1:8">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265" s="4">
         <v>3.7</v>
       </c>
@@ -7705,7 +7707,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="266" spans="1:8">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266" s="4">
         <v>7</v>
       </c>
@@ -7728,7 +7730,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="267" spans="1:8">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267" s="4">
         <v>13.5</v>
       </c>
@@ -7751,7 +7753,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="268" spans="1:8">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268" s="4">
         <v>5</v>
       </c>
@@ -7774,7 +7776,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="269" spans="1:8">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269" s="4">
         <v>20</v>
       </c>
@@ -7797,7 +7799,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="270" spans="1:8">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A270" s="4">
         <v>6</v>
       </c>
@@ -7820,7 +7822,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="271" spans="1:8">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271" s="4">
         <v>0.5</v>
       </c>
@@ -7843,7 +7845,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="272" spans="1:8">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272" s="4">
         <v>5</v>
       </c>
@@ -7866,7 +7868,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="273" spans="1:8">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" s="4">
         <v>11</v>
       </c>
@@ -7889,7 +7891,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="274" spans="1:8">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" s="4">
         <v>8.8000000000000007</v>
       </c>
@@ -7912,7 +7914,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="275" spans="1:8">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="4">
         <v>0.5</v>
       </c>
@@ -7935,7 +7937,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="276" spans="1:8">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="4">
         <v>5</v>
       </c>
@@ -7958,7 +7960,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="277" spans="1:8">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="4">
         <v>10</v>
       </c>
@@ -7981,7 +7983,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="278" spans="1:8">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="4">
         <v>15</v>
       </c>
@@ -8004,7 +8006,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="279" spans="1:8">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" s="4">
         <v>10</v>
       </c>
@@ -8027,7 +8029,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="280" spans="1:8">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280" s="4">
         <v>11.9</v>
       </c>
@@ -8050,7 +8052,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="281" spans="1:8">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281" s="4">
         <v>7</v>
       </c>
@@ -8073,7 +8075,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="282" spans="1:8">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -8096,7 +8098,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="283" spans="1:8">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>1.9</v>
       </c>
@@ -8119,7 +8121,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="284" spans="1:8">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>119.9</v>
       </c>
@@ -8142,7 +8144,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="285" spans="1:8">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>6.3</v>
       </c>
@@ -8165,7 +8167,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="286" spans="1:8">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>3.5</v>
       </c>
@@ -8188,7 +8190,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="287" spans="1:8">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>1.5</v>
       </c>
@@ -8211,7 +8213,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="288" spans="1:8">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>1.9</v>
       </c>
@@ -8234,7 +8236,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="289" spans="1:8">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>4.5</v>
       </c>
@@ -8257,7 +8259,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="290" spans="1:8">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>6.4</v>
       </c>
@@ -8280,7 +8282,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="291" spans="1:8">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>1.9</v>
       </c>
@@ -8303,7 +8305,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="292" spans="1:8">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>10.6</v>
       </c>
@@ -8326,7 +8328,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="293" spans="1:8">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>4.5</v>
       </c>
@@ -8349,7 +8351,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="294" spans="1:8">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>22.2</v>
       </c>
@@ -8372,7 +8374,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="295" spans="1:8">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295" s="6">
         <v>25</v>
       </c>
@@ -8395,7 +8397,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="296" spans="1:8">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A296" s="6">
         <v>3.5</v>
       </c>
@@ -8418,7 +8420,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="297" spans="1:8">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>4</v>
       </c>
@@ -8441,7 +8443,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="298" spans="1:8">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>2.2000000000000002</v>
       </c>
@@ -8464,7 +8466,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="299" spans="1:8">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>11.5</v>
       </c>
@@ -8487,7 +8489,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="300" spans="1:8">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>6.3</v>
       </c>
@@ -8510,7 +8512,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="301" spans="1:8">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>3.6</v>
       </c>
@@ -8533,7 +8535,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="302" spans="1:8">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>15</v>
       </c>
@@ -8556,7 +8558,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="303" spans="1:8">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>2</v>
       </c>
@@ -8579,7 +8581,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="304" spans="1:8">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>4.5</v>
       </c>
@@ -8602,7 +8604,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="305" spans="1:8">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>2.9</v>
       </c>
@@ -8625,7 +8627,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="306" spans="1:8">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>3.9</v>
       </c>
@@ -8648,7 +8650,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="307" spans="1:8">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>1.7</v>
       </c>
@@ -8671,7 +8673,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="308" spans="1:8">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>10</v>
       </c>
@@ -8694,7 +8696,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="309" spans="1:8">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>7.5</v>
       </c>
@@ -8717,7 +8719,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="310" spans="1:8">
+    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>10.050000000000001</v>
       </c>
@@ -8740,7 +8742,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="311" spans="1:8">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>5</v>
       </c>
@@ -8763,7 +8765,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="312" spans="1:8">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>3</v>
       </c>
@@ -8786,7 +8788,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="313" spans="1:8">
+    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>2</v>
       </c>
@@ -8809,7 +8811,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="314" spans="1:8">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>10.6</v>
       </c>
@@ -8832,7 +8834,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="315" spans="1:8">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>4</v>
       </c>
@@ -8855,7 +8857,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="316" spans="1:8">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>2</v>
       </c>
@@ -8878,7 +8880,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="317" spans="1:8">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>5.8</v>
       </c>
@@ -8901,7 +8903,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="318" spans="1:8">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>5</v>
       </c>
@@ -8924,7 +8926,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="319" spans="1:8">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>6.55</v>
       </c>
@@ -8947,7 +8949,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="320" spans="1:8">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>2.8</v>
       </c>
@@ -8970,7 +8972,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="321" spans="1:8">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>3.8</v>
       </c>
@@ -8993,7 +8995,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="322" spans="1:8">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>9</v>
       </c>
@@ -9016,7 +9018,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="323" spans="1:8">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>8</v>
       </c>
@@ -9039,7 +9041,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="324" spans="1:8">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>1.5</v>
       </c>
@@ -9062,7 +9064,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="325" spans="1:8">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>5</v>
       </c>
@@ -9085,7 +9087,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="326" spans="1:8">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>4.5999999999999996</v>
       </c>
@@ -9108,7 +9110,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="327" spans="1:8">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>0.5</v>
       </c>
@@ -9131,7 +9133,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="328" spans="1:8">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>2.95</v>
       </c>
@@ -9154,7 +9156,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="329" spans="1:8">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>3.8</v>
       </c>
@@ -9177,7 +9179,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="330" spans="1:8">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>10</v>
       </c>
@@ -9200,7 +9202,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="331" spans="1:8">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>3.85</v>
       </c>
@@ -9223,7 +9225,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="332" spans="1:8">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>1.2</v>
       </c>
@@ -9246,7 +9248,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="333" spans="1:8">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>2</v>
       </c>
@@ -9269,7 +9271,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="334" spans="1:8">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>8.5</v>
       </c>
@@ -9292,7 +9294,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="335" spans="1:8">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>4.9000000000000004</v>
       </c>
@@ -9315,7 +9317,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="336" spans="1:8">
+    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>10</v>
       </c>
@@ -9338,7 +9340,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="337" spans="1:8">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>1.5</v>
       </c>
@@ -9358,7 +9360,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="338" spans="1:8">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>350</v>
       </c>
@@ -9381,7 +9383,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="339" spans="1:8">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>4.4000000000000004</v>
       </c>
@@ -9404,7 +9406,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="340" spans="1:8">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>3.2</v>
       </c>
@@ -9427,7 +9429,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="341" spans="1:8">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>3.8</v>
       </c>
@@ -9450,7 +9452,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="342" spans="1:8">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>0.9</v>
       </c>
@@ -9473,7 +9475,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="343" spans="1:8">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>6</v>
       </c>
@@ -9496,7 +9498,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="344" spans="1:8">
+    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>3.8</v>
       </c>
@@ -9519,7 +9521,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="345" spans="1:8">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>2</v>
       </c>
@@ -9542,7 +9544,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="346" spans="1:8">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>5.5</v>
       </c>
@@ -9565,7 +9567,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="347" spans="1:8">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>43.22</v>
       </c>
@@ -9588,7 +9590,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="348" spans="1:8">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>2</v>
       </c>
@@ -9611,7 +9613,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="349" spans="1:8">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>7</v>
       </c>
@@ -9634,7 +9636,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="350" spans="1:8">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>1.61</v>
       </c>
@@ -9657,7 +9659,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="351" spans="1:8">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>20</v>
       </c>
@@ -9680,7 +9682,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="352" spans="1:8">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>14.84</v>
       </c>
@@ -9703,7 +9705,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="353" spans="1:12">
+    <row r="353" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>5.6</v>
       </c>
@@ -9726,7 +9728,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="354" spans="1:12">
+    <row r="354" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>6.8</v>
       </c>
@@ -9749,7 +9751,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="355" spans="1:12">
+    <row r="355" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>7.7</v>
       </c>
@@ -9772,7 +9774,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="356" spans="1:12">
+    <row r="356" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>29.4</v>
       </c>
@@ -9795,7 +9797,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="357" spans="1:12">
+    <row r="357" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>0.5</v>
       </c>
@@ -9818,7 +9820,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="358" spans="1:12">
+    <row r="358" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>2.2000000000000002</v>
       </c>
@@ -9841,7 +9843,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="359" spans="1:12">
+    <row r="359" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>3.5</v>
       </c>
@@ -9864,7 +9866,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="360" spans="1:12">
+    <row r="360" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>4.4000000000000004</v>
       </c>
@@ -9887,7 +9889,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="361" spans="1:12">
+    <row r="361" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>5.7</v>
       </c>
@@ -9910,7 +9912,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="362" spans="1:12">
+    <row r="362" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>7.74</v>
       </c>
@@ -9933,7 +9935,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="363" spans="1:12">
+    <row r="363" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>7</v>
       </c>
@@ -9956,7 +9958,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="364" spans="1:12">
+    <row r="364" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>3.8</v>
       </c>
@@ -9979,7 +9981,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="365" spans="1:12">
+    <row r="365" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>100</v>
       </c>
@@ -10002,7 +10004,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="366" spans="1:12">
+    <row r="366" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A366" s="1">
         <v>5</v>
       </c>
@@ -10026,7 +10028,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="367" spans="1:12">
+    <row r="367" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A367" s="6">
         <v>2</v>
       </c>
@@ -10053,7 +10055,7 @@
       <c r="K367" s="1"/>
       <c r="L367" s="1"/>
     </row>
-    <row r="368" spans="1:12">
+    <row r="368" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>7</v>
       </c>
@@ -10076,7 +10078,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="369" spans="1:8">
+    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>10</v>
       </c>
@@ -10099,7 +10101,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="370" spans="1:8">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>10.8</v>
       </c>
@@ -10122,7 +10124,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="371" spans="1:8">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>10.5</v>
       </c>
@@ -10145,7 +10147,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="372" spans="1:8">
+    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>5.5</v>
       </c>
@@ -10168,7 +10170,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="373" spans="1:8">
+    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>5</v>
       </c>
@@ -10191,7 +10193,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="374" spans="1:8">
+    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>0.5</v>
       </c>
@@ -10214,7 +10216,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="375" spans="1:8">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>10.5</v>
       </c>
@@ -10237,7 +10239,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="376" spans="1:8">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>14</v>
       </c>
@@ -10260,7 +10262,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="377" spans="1:8">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>2</v>
       </c>
@@ -10283,7 +10285,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="378" spans="1:8">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>3.5</v>
       </c>
@@ -10306,7 +10308,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="379" spans="1:8">
+    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>3.5</v>
       </c>
@@ -10329,7 +10331,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="380" spans="1:8">
+    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>3.5</v>
       </c>
@@ -10352,7 +10354,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="381" spans="1:8">
+    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>2</v>
       </c>
@@ -10375,7 +10377,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="382" spans="1:8">
+    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>2</v>
       </c>
@@ -10398,7 +10400,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="383" spans="1:8">
+    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>2.5</v>
       </c>
@@ -10421,7 +10423,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="384" spans="1:8">
+    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>6.5</v>
       </c>
@@ -10444,7 +10446,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="385" spans="1:8">
+    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>3.78</v>
       </c>
@@ -10467,7 +10469,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="386" spans="1:8">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>7</v>
       </c>
@@ -10490,7 +10492,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="387" spans="1:8">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>2.5</v>
       </c>
@@ -10513,7 +10515,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="388" spans="1:8">
+    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>2</v>
       </c>
@@ -10536,7 +10538,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="389" spans="1:8">
+    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>1</v>
       </c>
@@ -10559,7 +10561,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="390" spans="1:8">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>10.5</v>
       </c>
@@ -10582,7 +10584,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="391" spans="1:8">
+    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>1.5</v>
       </c>
@@ -10605,7 +10607,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="392" spans="1:8">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>2.7</v>
       </c>
@@ -10628,7 +10630,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="393" spans="1:8">
+    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>2</v>
       </c>
@@ -10651,7 +10653,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="394" spans="1:8">
+    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>17.5</v>
       </c>
@@ -10674,7 +10676,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="395" spans="1:8">
+    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>43</v>
       </c>
@@ -10697,7 +10699,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="396" spans="1:8">
+    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>69.900000000000006</v>
       </c>
@@ -10719,16 +10721,6 @@
       <c r="H396" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="518" spans="1:8">
-      <c r="A518" s="1"/>
-      <c r="B518" s="1"/>
-      <c r="C518" s="1"/>
-      <c r="D518" s="1"/>
-      <c r="E518" s="1"/>
-      <c r="F518" s="1"/>
-      <c r="G518" s="1"/>
-      <c r="H518" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add today costs in database
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1812" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1816" uniqueCount="453">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1370,6 +1370,9 @@
   </si>
   <si>
     <t>ταξί απο ανθούπολη για σπίτι</t>
+  </si>
+  <si>
+    <t>καυτερά noodles με λαχανικά</t>
   </si>
 </sst>
 </file>
@@ -1805,10 +1808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L455"/>
+  <dimension ref="A1:L456"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A433" workbookViewId="0">
-      <selection activeCell="E456" sqref="E456"/>
+      <selection activeCell="D457" sqref="D457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12244,6 +12247,29 @@
         <v>241</v>
       </c>
     </row>
+    <row r="456" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A456">
+        <v>4.2</v>
+      </c>
+      <c r="B456" t="s">
+        <v>223</v>
+      </c>
+      <c r="C456" s="2">
+        <v>43364</v>
+      </c>
+      <c r="D456" t="s">
+        <v>452</v>
+      </c>
+      <c r="E456" t="s">
+        <v>238</v>
+      </c>
+      <c r="F456">
+        <v>5</v>
+      </c>
+      <c r="H456" t="s">
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
delete Json Version and uptade costs
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11760"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2004" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2008" uniqueCount="496">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1499,17 +1499,20 @@
   </si>
   <si>
     <t xml:space="preserve">σπανακόπιτα </t>
+  </si>
+  <si>
+    <t>μπρελόκ για κλειδιά</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0\ &quot;€&quot;;[Red]\-#,##0\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1550,7 +1553,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -1631,8 +1634,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A1:H510" totalsRowShown="0">
-  <autoFilter ref="A1:H510">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A1:H514" totalsRowShown="0">
+  <autoFilter ref="A1:H514">
     <filterColumn colId="1">
       <filters>
         <filter val="transport"/>
@@ -1655,7 +1658,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Θέμα του Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1697,7 +1700,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1729,10 +1732,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1764,7 +1766,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1940,14 +1941,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L510"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L514"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A372" workbookViewId="0">
-      <selection activeCell="A511" sqref="A511"/>
+    <sheetView tabSelected="1" topLeftCell="A369" workbookViewId="0">
+      <selection activeCell="B513" sqref="B513"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
@@ -1963,7 +1964,7 @@
     <col min="12" max="12" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="5" t="s">
         <v>234</v>
       </c>
@@ -1992,7 +1993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" hidden="1">
       <c r="A2" s="5" t="s">
         <v>489</v>
       </c>
@@ -2018,7 +2019,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1">
       <c r="A3" s="4">
         <v>20</v>
       </c>
@@ -2042,7 +2043,7 @@
       </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1">
       <c r="A4" s="4">
         <v>10</v>
       </c>
@@ -2065,7 +2066,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1">
       <c r="A5" s="4">
         <v>100</v>
       </c>
@@ -2088,7 +2089,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1">
       <c r="A6" s="4">
         <v>10</v>
       </c>
@@ -2111,7 +2112,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1">
       <c r="A7" s="4">
         <v>50</v>
       </c>
@@ -2134,7 +2135,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1">
       <c r="A8" s="4">
         <v>3.2</v>
       </c>
@@ -2157,7 +2158,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1">
       <c r="A9" s="4">
         <v>1.3</v>
       </c>
@@ -2180,7 +2181,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1">
       <c r="A10" s="4">
         <v>1.2</v>
       </c>
@@ -2203,7 +2204,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1">
       <c r="A11" s="4">
         <v>5</v>
       </c>
@@ -2226,7 +2227,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1">
       <c r="A12" s="4">
         <v>4.5</v>
       </c>
@@ -2249,7 +2250,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1">
       <c r="A13" s="4">
         <v>4</v>
       </c>
@@ -2272,7 +2273,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1">
       <c r="A14" s="4">
         <v>10.6</v>
       </c>
@@ -2295,7 +2296,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" hidden="1">
       <c r="A15" s="4">
         <v>1.8</v>
       </c>
@@ -2318,7 +2319,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="4">
         <v>5.15</v>
       </c>
@@ -2341,7 +2342,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" hidden="1">
       <c r="A17" s="4">
         <v>18</v>
       </c>
@@ -2364,7 +2365,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1">
       <c r="A18" s="4">
         <v>1.5</v>
       </c>
@@ -2387,7 +2388,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" hidden="1">
       <c r="A19" s="4">
         <v>7.8</v>
       </c>
@@ -2410,7 +2411,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" hidden="1">
       <c r="A20" s="4">
         <v>4.4400000000000004</v>
       </c>
@@ -2433,7 +2434,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" hidden="1">
       <c r="A21" s="4">
         <v>1.5</v>
       </c>
@@ -2456,7 +2457,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" hidden="1">
       <c r="A22" s="4">
         <v>8.84</v>
       </c>
@@ -2479,7 +2480,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1">
       <c r="A23" s="4">
         <v>4</v>
       </c>
@@ -2502,7 +2503,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1">
       <c r="A24" s="4">
         <v>10</v>
       </c>
@@ -2525,7 +2526,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1">
       <c r="A25" s="4">
         <v>1.8</v>
       </c>
@@ -2548,7 +2549,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" hidden="1">
       <c r="A26" s="4">
         <v>11.8</v>
       </c>
@@ -2571,7 +2572,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" hidden="1">
       <c r="A27" s="4">
         <v>40</v>
       </c>
@@ -2594,7 +2595,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1">
       <c r="A28" s="4">
         <v>2.9</v>
       </c>
@@ -2617,7 +2618,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" hidden="1">
       <c r="A29" s="4">
         <v>4.3</v>
       </c>
@@ -2640,7 +2641,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1">
       <c r="A30" s="4">
         <v>3.35</v>
       </c>
@@ -2663,7 +2664,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" hidden="1">
       <c r="A31" s="4">
         <v>5.2</v>
       </c>
@@ -2686,7 +2687,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" hidden="1">
       <c r="A32" s="4">
         <v>15</v>
       </c>
@@ -2709,7 +2710,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" hidden="1">
       <c r="A33" s="4">
         <v>3.9</v>
       </c>
@@ -2732,7 +2733,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" hidden="1">
       <c r="A34" s="4">
         <v>63.45</v>
       </c>
@@ -2755,7 +2756,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" hidden="1">
       <c r="A35" s="4">
         <v>49.9</v>
       </c>
@@ -2775,7 +2776,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" hidden="1">
       <c r="A36" s="4">
         <v>140</v>
       </c>
@@ -2798,7 +2799,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" hidden="1">
       <c r="A37" s="4">
         <v>1.8</v>
       </c>
@@ -2821,7 +2822,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" hidden="1">
       <c r="A38" s="4">
         <v>13.02</v>
       </c>
@@ -2844,7 +2845,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" hidden="1">
       <c r="A39" s="4">
         <v>4.7</v>
       </c>
@@ -2867,7 +2868,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" hidden="1">
       <c r="A40" s="4">
         <v>15.96</v>
       </c>
@@ -2890,7 +2891,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" hidden="1">
       <c r="A41" s="4">
         <v>9.8000000000000007</v>
       </c>
@@ -2913,7 +2914,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" hidden="1">
       <c r="A42" s="4">
         <v>79.8</v>
       </c>
@@ -2936,7 +2937,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" hidden="1">
       <c r="A43" s="4">
         <v>11.9</v>
       </c>
@@ -2959,7 +2960,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" hidden="1">
       <c r="A44" s="4">
         <v>38.880000000000003</v>
       </c>
@@ -2982,7 +2983,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" hidden="1">
       <c r="A45" s="4">
         <v>7.75</v>
       </c>
@@ -3005,7 +3006,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" hidden="1">
       <c r="A46" s="4">
         <v>0.79</v>
       </c>
@@ -3028,7 +3029,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" s="4">
         <v>10</v>
       </c>
@@ -3051,7 +3052,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" hidden="1">
       <c r="A48" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3074,7 +3075,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" hidden="1">
       <c r="A49" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3097,7 +3098,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" hidden="1">
       <c r="A50" s="4">
         <v>1.8</v>
       </c>
@@ -3120,7 +3121,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11">
       <c r="A51" s="4">
         <v>24</v>
       </c>
@@ -3143,7 +3144,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" hidden="1">
       <c r="A52" s="4">
         <v>24</v>
       </c>
@@ -3166,7 +3167,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11">
       <c r="A53" s="4">
         <v>1.8</v>
       </c>
@@ -3189,7 +3190,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" hidden="1">
       <c r="A54" s="4">
         <v>3.5</v>
       </c>
@@ -3212,7 +3213,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" hidden="1">
       <c r="A55" s="4">
         <v>5.6</v>
       </c>
@@ -3236,7 +3237,7 @@
       </c>
       <c r="K55" s="4"/>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" hidden="1">
       <c r="A56" s="4">
         <v>1.5</v>
       </c>
@@ -3259,7 +3260,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" hidden="1">
       <c r="A57" s="4">
         <v>3</v>
       </c>
@@ -3282,7 +3283,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11">
       <c r="A58" s="4">
         <v>5.4</v>
       </c>
@@ -3305,7 +3306,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" hidden="1">
       <c r="A59" s="4">
         <v>8</v>
       </c>
@@ -3328,7 +3329,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11">
       <c r="A60" s="4">
         <v>5.4</v>
       </c>
@@ -3351,7 +3352,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11">
       <c r="A61" s="4">
         <v>0.6</v>
       </c>
@@ -3374,7 +3375,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" hidden="1">
       <c r="A62" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3397,7 +3398,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" hidden="1">
       <c r="A63" s="4">
         <v>1.5</v>
       </c>
@@ -3420,7 +3421,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" hidden="1">
       <c r="A64" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3443,7 +3444,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11">
       <c r="A65" s="4">
         <v>1.2</v>
       </c>
@@ -3466,7 +3467,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11">
       <c r="A66" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -3489,7 +3490,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11">
       <c r="A67" s="4">
         <v>13.5</v>
       </c>
@@ -3512,7 +3513,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" hidden="1">
       <c r="A68" s="4">
         <v>3.5</v>
       </c>
@@ -3536,7 +3537,7 @@
       </c>
       <c r="K68" s="4"/>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" hidden="1">
       <c r="A69" s="4">
         <v>4.0999999999999996</v>
       </c>
@@ -3559,7 +3560,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11">
       <c r="A70" s="4">
         <v>90</v>
       </c>
@@ -3582,7 +3583,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11">
       <c r="A71" s="4">
         <v>65.5</v>
       </c>
@@ -3605,7 +3606,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" hidden="1">
       <c r="A72" s="4">
         <v>4.5</v>
       </c>
@@ -3628,7 +3629,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" hidden="1">
       <c r="A73" s="4">
         <v>10</v>
       </c>
@@ -3651,7 +3652,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" hidden="1">
       <c r="A74" s="4">
         <v>18.8</v>
       </c>
@@ -3674,7 +3675,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" hidden="1">
       <c r="A75" s="4">
         <v>1.8</v>
       </c>
@@ -3698,7 +3699,7 @@
       </c>
       <c r="K75" s="4"/>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" hidden="1">
       <c r="A76" s="4">
         <v>5.5</v>
       </c>
@@ -3721,7 +3722,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" hidden="1">
       <c r="A77" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3744,7 +3745,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" hidden="1">
       <c r="A78" s="4">
         <v>3</v>
       </c>
@@ -3767,7 +3768,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" hidden="1">
       <c r="A79" s="4">
         <v>2</v>
       </c>
@@ -3790,7 +3791,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" hidden="1">
       <c r="A80" s="4">
         <v>9.9</v>
       </c>
@@ -3813,7 +3814,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" hidden="1">
       <c r="A81" s="4">
         <v>6.5</v>
       </c>
@@ -3836,7 +3837,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" hidden="1">
       <c r="A82" s="4">
         <v>79.8</v>
       </c>
@@ -3859,7 +3860,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" hidden="1">
       <c r="A83" s="4">
         <v>10</v>
       </c>
@@ -3882,7 +3883,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" hidden="1">
       <c r="A84" s="4">
         <v>2.5</v>
       </c>
@@ -3905,7 +3906,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" hidden="1">
       <c r="A85" s="4">
         <v>5</v>
       </c>
@@ -3928,7 +3929,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" hidden="1">
       <c r="A86" s="4">
         <v>1.6</v>
       </c>
@@ -3951,7 +3952,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" hidden="1">
       <c r="A87" s="4">
         <v>5.5</v>
       </c>
@@ -3974,7 +3975,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" hidden="1">
       <c r="A88" s="4">
         <v>0.8</v>
       </c>
@@ -3997,7 +3998,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" hidden="1">
       <c r="A89" s="4">
         <v>17</v>
       </c>
@@ -4020,7 +4021,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" hidden="1">
       <c r="A90" s="4">
         <v>24.9</v>
       </c>
@@ -4043,7 +4044,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" hidden="1">
       <c r="A91" s="4">
         <v>1.8</v>
       </c>
@@ -4066,7 +4067,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" hidden="1">
       <c r="A92" s="4">
         <v>44.99</v>
       </c>
@@ -4089,7 +4090,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8">
       <c r="A93" s="4">
         <v>4</v>
       </c>
@@ -4112,7 +4113,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" hidden="1">
       <c r="A94" s="4">
         <v>5</v>
       </c>
@@ -4135,7 +4136,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" hidden="1">
       <c r="A95" s="4">
         <v>5</v>
       </c>
@@ -4158,13 +4159,13 @@
         <v>267</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" hidden="1">
       <c r="A96" s="4"/>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" hidden="1">
       <c r="A97" s="4"/>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" hidden="1">
       <c r="A98" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -4187,7 +4188,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" hidden="1">
       <c r="A99" s="4">
         <v>3</v>
       </c>
@@ -4210,7 +4211,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" hidden="1">
       <c r="A100" s="4">
         <v>6</v>
       </c>
@@ -4233,7 +4234,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" hidden="1">
       <c r="A101" s="4">
         <v>3.5</v>
       </c>
@@ -4256,7 +4257,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" hidden="1">
       <c r="A102" s="4">
         <v>34.9</v>
       </c>
@@ -4279,7 +4280,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" hidden="1">
       <c r="A103" s="4">
         <v>12</v>
       </c>
@@ -4302,10 +4303,10 @@
         <v>241</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" hidden="1">
       <c r="A104" s="4"/>
     </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" hidden="1">
       <c r="A105" s="4">
         <v>5</v>
       </c>
@@ -4328,7 +4329,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" hidden="1">
       <c r="A106" s="4">
         <v>6.9</v>
       </c>
@@ -4351,7 +4352,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" hidden="1">
       <c r="A107" s="4">
         <v>6.04</v>
       </c>
@@ -4374,7 +4375,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" hidden="1">
       <c r="A108" s="4">
         <v>4.8</v>
       </c>
@@ -4397,7 +4398,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" hidden="1">
       <c r="A109" s="4">
         <v>9.6999999999999993</v>
       </c>
@@ -4420,7 +4421,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" hidden="1">
       <c r="A110" s="4">
         <v>5.5</v>
       </c>
@@ -4443,7 +4444,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" hidden="1">
       <c r="A111" s="4">
         <v>7</v>
       </c>
@@ -4466,7 +4467,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" hidden="1">
       <c r="A112" s="4">
         <v>1</v>
       </c>
@@ -4489,7 +4490,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" hidden="1">
       <c r="A113" s="4">
         <v>4</v>
       </c>
@@ -4512,7 +4513,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" hidden="1">
       <c r="A114" s="4">
         <v>4.0999999999999996</v>
       </c>
@@ -4535,7 +4536,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" hidden="1">
       <c r="A115" s="4">
         <v>2.3199999999999998</v>
       </c>
@@ -4558,7 +4559,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" hidden="1">
       <c r="A116" s="4">
         <v>8</v>
       </c>
@@ -4581,7 +4582,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" hidden="1">
       <c r="A117" s="4">
         <v>12.5</v>
       </c>
@@ -4604,7 +4605,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" hidden="1">
       <c r="A118" s="4">
         <v>0.7</v>
       </c>
@@ -4627,7 +4628,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8">
       <c r="A119" s="4">
         <v>6.3</v>
       </c>
@@ -4650,7 +4651,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" hidden="1">
       <c r="A120" s="4">
         <v>8</v>
       </c>
@@ -4673,7 +4674,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" hidden="1">
       <c r="A121" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -4696,7 +4697,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" hidden="1">
       <c r="A122" s="4">
         <v>8</v>
       </c>
@@ -4719,7 +4720,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" hidden="1">
       <c r="A123" s="4">
         <v>4.5</v>
       </c>
@@ -4742,7 +4743,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" hidden="1">
       <c r="A124" s="4">
         <v>2.5</v>
       </c>
@@ -4765,7 +4766,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8">
       <c r="A125" s="4">
         <v>24.3</v>
       </c>
@@ -4788,7 +4789,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" hidden="1">
       <c r="A126" s="4">
         <v>2</v>
       </c>
@@ -4811,7 +4812,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" hidden="1">
       <c r="A127" s="4">
         <v>16</v>
       </c>
@@ -4834,7 +4835,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" hidden="1">
       <c r="A128" s="4">
         <v>6</v>
       </c>
@@ -4857,7 +4858,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" hidden="1">
       <c r="A129" s="4">
         <v>5</v>
       </c>
@@ -4880,7 +4881,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" hidden="1">
       <c r="A130" s="4">
         <v>6.52</v>
       </c>
@@ -4903,7 +4904,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" hidden="1">
       <c r="A131" s="4">
         <v>1.8</v>
       </c>
@@ -4926,7 +4927,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" hidden="1">
       <c r="A132" s="4">
         <v>1</v>
       </c>
@@ -4949,7 +4950,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8">
       <c r="A133" s="4">
         <v>5</v>
       </c>
@@ -4972,7 +4973,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8">
       <c r="A134" s="4">
         <v>43</v>
       </c>
@@ -4995,7 +4996,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" hidden="1">
       <c r="A135" s="4">
         <v>10</v>
       </c>
@@ -5018,7 +5019,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" hidden="1">
       <c r="A136" s="4">
         <v>2.97</v>
       </c>
@@ -5041,7 +5042,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" hidden="1">
       <c r="A137" s="4">
         <v>10</v>
       </c>
@@ -5064,7 +5065,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" hidden="1">
       <c r="A138" s="4">
         <v>1.6</v>
       </c>
@@ -5087,7 +5088,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" hidden="1">
       <c r="A139" s="4">
         <v>1.5</v>
       </c>
@@ -5110,7 +5111,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" hidden="1">
       <c r="A140" s="4">
         <v>1.8</v>
       </c>
@@ -5133,7 +5134,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" hidden="1">
       <c r="A141" s="4">
         <v>7.3</v>
       </c>
@@ -5156,7 +5157,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" hidden="1">
       <c r="A142" s="4">
         <v>4</v>
       </c>
@@ -5179,7 +5180,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" hidden="1">
       <c r="A143" s="4">
         <v>2.1</v>
       </c>
@@ -5202,7 +5203,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" hidden="1">
       <c r="A144" s="4">
         <v>4.2</v>
       </c>
@@ -5225,7 +5226,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" hidden="1">
       <c r="A145" s="4">
         <v>9</v>
       </c>
@@ -5248,7 +5249,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" hidden="1">
       <c r="A146" s="4">
         <v>1</v>
       </c>
@@ -5271,7 +5272,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" hidden="1">
       <c r="A147" s="4">
         <v>3.5</v>
       </c>
@@ -5294,7 +5295,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" hidden="1">
       <c r="A148" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -5317,7 +5318,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" hidden="1">
       <c r="A149" s="4">
         <v>3</v>
       </c>
@@ -5340,7 +5341,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" hidden="1">
       <c r="A150" s="4">
         <v>2</v>
       </c>
@@ -5363,7 +5364,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" hidden="1">
       <c r="A151" s="4">
         <v>150</v>
       </c>
@@ -5386,7 +5387,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" hidden="1">
       <c r="A152" s="4">
         <v>7</v>
       </c>
@@ -5409,7 +5410,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" hidden="1">
       <c r="A153" s="4">
         <v>5</v>
       </c>
@@ -5432,7 +5433,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" hidden="1">
       <c r="A154" s="4">
         <v>8</v>
       </c>
@@ -5455,7 +5456,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8">
       <c r="A155" s="4">
         <v>3.5</v>
       </c>
@@ -5478,7 +5479,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" hidden="1">
       <c r="A156" s="4">
         <v>55</v>
       </c>
@@ -5501,7 +5502,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" hidden="1">
       <c r="A157" s="4">
         <v>0.6</v>
       </c>
@@ -5524,7 +5525,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" hidden="1">
       <c r="A158" s="4">
         <v>4</v>
       </c>
@@ -5547,7 +5548,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" hidden="1">
       <c r="A159" s="4">
         <v>39.9</v>
       </c>
@@ -5570,7 +5571,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" hidden="1">
       <c r="A160" s="4">
         <v>1.6</v>
       </c>
@@ -5593,7 +5594,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" hidden="1">
       <c r="A161" s="4">
         <v>80</v>
       </c>
@@ -5616,7 +5617,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" hidden="1">
       <c r="A162" s="4">
         <v>6.2</v>
       </c>
@@ -5639,7 +5640,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" hidden="1">
       <c r="A163" s="4">
         <v>15</v>
       </c>
@@ -5662,7 +5663,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" hidden="1">
       <c r="A164" s="4">
         <v>4.3</v>
       </c>
@@ -5685,7 +5686,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" hidden="1">
       <c r="A165" s="4">
         <v>9.6999999999999993</v>
       </c>
@@ -5708,7 +5709,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" hidden="1">
       <c r="A166" s="4">
         <v>2.4500000000000002</v>
       </c>
@@ -5731,7 +5732,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" hidden="1">
       <c r="A167" s="4">
         <v>1.96</v>
       </c>
@@ -5754,7 +5755,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" hidden="1">
       <c r="A168" s="4">
         <v>11.5</v>
       </c>
@@ -5777,7 +5778,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" hidden="1">
       <c r="A169" s="4">
         <v>2.7</v>
       </c>
@@ -5800,7 +5801,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" hidden="1">
       <c r="A170" s="4">
         <v>2.7</v>
       </c>
@@ -5823,7 +5824,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" hidden="1">
       <c r="A171" s="4">
         <v>7</v>
       </c>
@@ -5846,7 +5847,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" hidden="1">
       <c r="A172" s="4">
         <v>4.8</v>
       </c>
@@ -5869,7 +5870,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" hidden="1">
       <c r="A173" s="4">
         <v>4.4000000000000004</v>
       </c>
@@ -5892,7 +5893,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" hidden="1">
       <c r="A174" s="4">
         <v>3.8</v>
       </c>
@@ -5915,7 +5916,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" hidden="1">
       <c r="A175" s="4">
         <v>1.5</v>
       </c>
@@ -5938,7 +5939,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" hidden="1">
       <c r="A176" s="4">
         <v>11.5</v>
       </c>
@@ -5961,7 +5962,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" hidden="1">
       <c r="A177" s="4">
         <v>4.4000000000000004</v>
       </c>
@@ -5984,7 +5985,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" hidden="1">
       <c r="A178" s="4">
         <v>6.5</v>
       </c>
@@ -6007,7 +6008,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" hidden="1">
       <c r="A179" s="4">
         <v>6.5</v>
       </c>
@@ -6030,7 +6031,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" hidden="1">
       <c r="A180" s="4">
         <v>5</v>
       </c>
@@ -6053,7 +6054,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" hidden="1">
       <c r="A181" s="4">
         <v>6</v>
       </c>
@@ -6076,7 +6077,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8">
       <c r="A182" s="4">
         <v>8</v>
       </c>
@@ -6099,7 +6100,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" hidden="1">
       <c r="A183" s="4">
         <v>3.2</v>
       </c>
@@ -6122,7 +6123,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" hidden="1">
       <c r="A184" s="4">
         <v>10</v>
       </c>
@@ -6145,7 +6146,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" hidden="1">
       <c r="A185" s="4">
         <v>3</v>
       </c>
@@ -6168,7 +6169,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" hidden="1">
       <c r="A186" s="4">
         <v>10</v>
       </c>
@@ -6191,7 +6192,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" hidden="1">
       <c r="A187" s="4">
         <v>3.5</v>
       </c>
@@ -6214,7 +6215,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" hidden="1">
       <c r="A188" s="4">
         <v>10</v>
       </c>
@@ -6237,7 +6238,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" hidden="1">
       <c r="A189" s="4">
         <v>8</v>
       </c>
@@ -6260,7 +6261,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8">
       <c r="A190" s="4">
         <v>6.2</v>
       </c>
@@ -6283,7 +6284,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" hidden="1">
       <c r="A191" s="4">
         <v>2</v>
       </c>
@@ -6306,7 +6307,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" hidden="1">
       <c r="A192" s="4">
         <v>10</v>
       </c>
@@ -6329,7 +6330,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" hidden="1">
       <c r="A193" s="4">
         <v>22</v>
       </c>
@@ -6352,7 +6353,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" hidden="1">
       <c r="A194" s="4">
         <v>14</v>
       </c>
@@ -6375,7 +6376,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8">
       <c r="A195" s="4">
         <v>14</v>
       </c>
@@ -6398,7 +6399,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" hidden="1">
       <c r="A196" s="4">
         <v>4.7</v>
       </c>
@@ -6421,7 +6422,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" hidden="1">
       <c r="A197" s="4">
         <v>69.900000000000006</v>
       </c>
@@ -6444,7 +6445,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" hidden="1">
       <c r="A198" s="4">
         <v>8.4</v>
       </c>
@@ -6467,7 +6468,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" hidden="1">
       <c r="A199" s="4">
         <v>5</v>
       </c>
@@ -6490,7 +6491,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" hidden="1">
       <c r="A200" s="4">
         <v>4.5</v>
       </c>
@@ -6513,7 +6514,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" hidden="1">
       <c r="A201" s="4">
         <v>6</v>
       </c>
@@ -6536,7 +6537,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" hidden="1">
       <c r="A202" s="4">
         <v>5.46</v>
       </c>
@@ -6559,7 +6560,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" hidden="1">
       <c r="A203" s="4">
         <v>78.849999999999994</v>
       </c>
@@ -6582,7 +6583,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" hidden="1">
       <c r="A204" s="4">
         <v>10</v>
       </c>
@@ -6605,7 +6606,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" hidden="1">
       <c r="A205" s="4">
         <v>10</v>
       </c>
@@ -6628,7 +6629,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" hidden="1">
       <c r="A206" s="4">
         <v>26</v>
       </c>
@@ -6651,7 +6652,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" hidden="1">
       <c r="A207" s="4">
         <v>2</v>
       </c>
@@ -6674,7 +6675,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" hidden="1">
       <c r="A208" s="4">
         <v>2.5</v>
       </c>
@@ -6697,7 +6698,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" hidden="1">
       <c r="A209" s="4">
         <v>5.9</v>
       </c>
@@ -6720,7 +6721,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="210" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" hidden="1">
       <c r="A210" s="4">
         <v>8.6</v>
       </c>
@@ -6743,7 +6744,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" hidden="1">
       <c r="A211" s="4">
         <v>2.7</v>
       </c>
@@ -6766,7 +6767,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="212" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" hidden="1">
       <c r="A212" s="4">
         <v>4.8</v>
       </c>
@@ -6789,7 +6790,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="213" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" hidden="1">
       <c r="A213" s="4">
         <v>2.8</v>
       </c>
@@ -6812,7 +6813,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" hidden="1">
       <c r="A214" s="4">
         <v>2</v>
       </c>
@@ -6835,7 +6836,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="215" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" hidden="1">
       <c r="A215" s="4">
         <v>5</v>
       </c>
@@ -6858,7 +6859,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="216" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" hidden="1">
       <c r="A216" s="4">
         <v>2.5</v>
       </c>
@@ -6881,7 +6882,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:8">
       <c r="A217" s="4">
         <v>3.5</v>
       </c>
@@ -6904,7 +6905,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="218" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" hidden="1">
       <c r="A218" s="4">
         <v>1.8</v>
       </c>
@@ -6927,7 +6928,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="219" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" hidden="1">
       <c r="A219" s="4">
         <v>4</v>
       </c>
@@ -6950,7 +6951,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="220" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" hidden="1">
       <c r="A220" s="4">
         <v>6</v>
       </c>
@@ -6973,7 +6974,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="221" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" hidden="1">
       <c r="A221" s="4">
         <v>1.8</v>
       </c>
@@ -6996,7 +6997,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:8">
       <c r="A222" s="4">
         <v>5</v>
       </c>
@@ -7019,7 +7020,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="223" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" hidden="1">
       <c r="A223" s="4">
         <v>5</v>
       </c>
@@ -7042,7 +7043,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="224" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" hidden="1">
       <c r="A224" s="4">
         <v>4.7</v>
       </c>
@@ -7065,7 +7066,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" hidden="1">
       <c r="A225" s="4">
         <v>5</v>
       </c>
@@ -7088,7 +7089,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="226" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" hidden="1">
       <c r="A226" s="4">
         <v>10</v>
       </c>
@@ -7111,7 +7112,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" hidden="1">
       <c r="A227" s="4">
         <v>1.5</v>
       </c>
@@ -7134,7 +7135,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:8">
       <c r="A228" s="4">
         <v>129</v>
       </c>
@@ -7157,7 +7158,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" hidden="1">
       <c r="A229" s="4">
         <v>7</v>
       </c>
@@ -7180,7 +7181,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" hidden="1">
       <c r="A230" s="4">
         <v>2.8</v>
       </c>
@@ -7203,7 +7204,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="231" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" hidden="1">
       <c r="A231" s="4">
         <v>1</v>
       </c>
@@ -7226,7 +7227,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="232" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" hidden="1">
       <c r="A232" s="4">
         <v>4</v>
       </c>
@@ -7249,7 +7250,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="233" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" hidden="1">
       <c r="A233" s="4">
         <v>50</v>
       </c>
@@ -7272,7 +7273,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="234" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" hidden="1">
       <c r="A234" s="4">
         <v>7.2</v>
       </c>
@@ -7295,7 +7296,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" hidden="1">
       <c r="A235" s="4">
         <v>1</v>
       </c>
@@ -7318,7 +7319,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="236" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" hidden="1">
       <c r="A236" s="4">
         <v>7</v>
       </c>
@@ -7341,7 +7342,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="237" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" hidden="1">
       <c r="A237" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -7364,7 +7365,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:8">
       <c r="A238" s="4">
         <v>7</v>
       </c>
@@ -7387,7 +7388,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" hidden="1">
       <c r="A239" s="4">
         <v>15</v>
       </c>
@@ -7410,7 +7411,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="240" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" hidden="1">
       <c r="A240" s="4">
         <v>3</v>
       </c>
@@ -7433,7 +7434,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8">
       <c r="A241" s="4">
         <v>11.2</v>
       </c>
@@ -7456,7 +7457,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="242" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" hidden="1">
       <c r="A242" s="4">
         <v>2.1</v>
       </c>
@@ -7479,7 +7480,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="243" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" hidden="1">
       <c r="A243" s="4">
         <v>150</v>
       </c>
@@ -7502,7 +7503,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="244" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" hidden="1">
       <c r="A244" s="4">
         <v>12.7</v>
       </c>
@@ -7525,7 +7526,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="245" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" hidden="1">
       <c r="A245" s="4">
         <v>89.9</v>
       </c>
@@ -7548,7 +7549,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="246" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" hidden="1">
       <c r="A246" s="4">
         <v>4.4000000000000004</v>
       </c>
@@ -7571,7 +7572,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="247" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" hidden="1">
       <c r="A247" s="4">
         <v>4.2</v>
       </c>
@@ -7594,7 +7595,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="248" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" hidden="1">
       <c r="A248" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -7617,7 +7618,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="249" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" hidden="1">
       <c r="A249" s="4">
         <v>5</v>
       </c>
@@ -7640,7 +7641,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="250" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" hidden="1">
       <c r="A250" s="4">
         <v>5</v>
       </c>
@@ -7663,7 +7664,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="251" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" hidden="1">
       <c r="A251" s="4">
         <v>3.9</v>
       </c>
@@ -7686,7 +7687,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" hidden="1">
       <c r="A252" s="4">
         <v>0.5</v>
       </c>
@@ -7709,7 +7710,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="253" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" hidden="1">
       <c r="A253" s="4">
         <v>2.4</v>
       </c>
@@ -7732,7 +7733,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="254" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" hidden="1">
       <c r="A254" s="4">
         <v>2</v>
       </c>
@@ -7755,7 +7756,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="255" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" hidden="1">
       <c r="A255" s="4">
         <v>4.7</v>
       </c>
@@ -7778,7 +7779,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="256" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" hidden="1">
       <c r="A256" s="4">
         <v>5.3</v>
       </c>
@@ -7801,7 +7802,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="257" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" hidden="1">
       <c r="A257" s="4">
         <v>4.2</v>
       </c>
@@ -7824,7 +7825,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="258" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" hidden="1">
       <c r="A258" s="4">
         <v>5</v>
       </c>
@@ -7847,7 +7848,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="259" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" hidden="1">
       <c r="A259" s="4">
         <v>2.5</v>
       </c>
@@ -7870,7 +7871,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="260" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" hidden="1">
       <c r="A260" s="4">
         <v>3.3</v>
       </c>
@@ -7893,7 +7894,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="261" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" hidden="1">
       <c r="A261" s="4">
         <v>5.6</v>
       </c>
@@ -7916,7 +7917,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8">
       <c r="A262" s="4">
         <v>4</v>
       </c>
@@ -7939,7 +7940,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="263" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" hidden="1">
       <c r="A263" s="4">
         <v>10.199999999999999</v>
       </c>
@@ -7962,7 +7963,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="264" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" hidden="1">
       <c r="A264" s="4">
         <v>8</v>
       </c>
@@ -7985,7 +7986,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="265" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" hidden="1">
       <c r="A265" s="4">
         <v>2.1</v>
       </c>
@@ -8008,7 +8009,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" hidden="1">
       <c r="A266" s="4">
         <v>3.7</v>
       </c>
@@ -8031,7 +8032,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" hidden="1">
       <c r="A267" s="4">
         <v>7</v>
       </c>
@@ -8054,7 +8055,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:8">
       <c r="A268" s="4">
         <v>13.5</v>
       </c>
@@ -8077,7 +8078,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" hidden="1">
       <c r="A269" s="4">
         <v>5</v>
       </c>
@@ -8100,7 +8101,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:8">
       <c r="A270" s="4">
         <v>20</v>
       </c>
@@ -8123,7 +8124,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="271" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" hidden="1">
       <c r="A271" s="4">
         <v>6</v>
       </c>
@@ -8146,7 +8147,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="272" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" hidden="1">
       <c r="A272" s="4">
         <v>0.5</v>
       </c>
@@ -8169,7 +8170,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="273" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" hidden="1">
       <c r="A273" s="4">
         <v>5</v>
       </c>
@@ -8192,7 +8193,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="274" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" hidden="1">
       <c r="A274" s="4">
         <v>11</v>
       </c>
@@ -8215,7 +8216,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="275" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" hidden="1">
       <c r="A275" s="4">
         <v>8.8000000000000007</v>
       </c>
@@ -8238,7 +8239,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="276" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" hidden="1">
       <c r="A276" s="4">
         <v>0.5</v>
       </c>
@@ -8261,7 +8262,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8">
       <c r="A277" s="4">
         <v>5</v>
       </c>
@@ -8284,7 +8285,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="278" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" hidden="1">
       <c r="A278" s="4">
         <v>10</v>
       </c>
@@ -8307,7 +8308,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="279" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" hidden="1">
       <c r="A279" s="4">
         <v>15</v>
       </c>
@@ -8330,7 +8331,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8">
       <c r="A280" s="4">
         <v>10</v>
       </c>
@@ -8353,7 +8354,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" hidden="1">
       <c r="A281" s="4">
         <v>11.9</v>
       </c>
@@ -8376,7 +8377,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" hidden="1">
       <c r="A282" s="4">
         <v>7</v>
       </c>
@@ -8399,7 +8400,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" hidden="1">
       <c r="A283" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -8422,7 +8423,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="284" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" hidden="1">
       <c r="A284">
         <v>1.9</v>
       </c>
@@ -8445,7 +8446,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="285" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" hidden="1">
       <c r="A285">
         <v>119.9</v>
       </c>
@@ -8468,7 +8469,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="286" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" hidden="1">
       <c r="A286">
         <v>6.3</v>
       </c>
@@ -8491,7 +8492,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="287" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" hidden="1">
       <c r="A287">
         <v>3.5</v>
       </c>
@@ -8514,7 +8515,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="288" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" hidden="1">
       <c r="A288">
         <v>1.5</v>
       </c>
@@ -8537,7 +8538,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" hidden="1">
       <c r="A289">
         <v>1.9</v>
       </c>
@@ -8560,7 +8561,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" hidden="1">
       <c r="A290">
         <v>4.5</v>
       </c>
@@ -8583,7 +8584,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8" hidden="1">
       <c r="A291">
         <v>6.4</v>
       </c>
@@ -8606,7 +8607,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" hidden="1">
       <c r="A292">
         <v>1.9</v>
       </c>
@@ -8629,7 +8630,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8" hidden="1">
       <c r="A293">
         <v>10.6</v>
       </c>
@@ -8652,7 +8653,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:8" hidden="1">
       <c r="A294">
         <v>4.5</v>
       </c>
@@ -8675,7 +8676,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" hidden="1">
       <c r="A295">
         <v>22.2</v>
       </c>
@@ -8698,7 +8699,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8" hidden="1">
       <c r="A296" s="6">
         <v>25</v>
       </c>
@@ -8721,7 +8722,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:8">
       <c r="A297" s="6">
         <v>3.5</v>
       </c>
@@ -8744,7 +8745,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" hidden="1">
       <c r="A298">
         <v>4</v>
       </c>
@@ -8767,7 +8768,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" hidden="1">
       <c r="A299">
         <v>2.2000000000000002</v>
       </c>
@@ -8790,7 +8791,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" hidden="1">
       <c r="A300">
         <v>11.5</v>
       </c>
@@ -8813,7 +8814,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="301" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" hidden="1">
       <c r="A301">
         <v>6.3</v>
       </c>
@@ -8836,7 +8837,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="302" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" hidden="1">
       <c r="A302">
         <v>3.6</v>
       </c>
@@ -8859,7 +8860,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8">
       <c r="A303">
         <v>15</v>
       </c>
@@ -8882,7 +8883,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="304" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" hidden="1">
       <c r="A304">
         <v>2</v>
       </c>
@@ -8905,7 +8906,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="305" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8" hidden="1">
       <c r="A305">
         <v>4.5</v>
       </c>
@@ -8928,7 +8929,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="306" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" hidden="1">
       <c r="A306">
         <v>2.9</v>
       </c>
@@ -8951,7 +8952,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="307" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" hidden="1">
       <c r="A307">
         <v>3.9</v>
       </c>
@@ -8974,7 +8975,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="308" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8" hidden="1">
       <c r="A308">
         <v>1.7</v>
       </c>
@@ -8997,7 +8998,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="309" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:8" hidden="1">
       <c r="A309">
         <v>10</v>
       </c>
@@ -9020,7 +9021,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:8">
       <c r="A310">
         <v>7.5</v>
       </c>
@@ -9043,7 +9044,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="311" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:8" hidden="1">
       <c r="A311">
         <v>10.050000000000001</v>
       </c>
@@ -9066,7 +9067,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="312" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:8" hidden="1">
       <c r="A312">
         <v>5</v>
       </c>
@@ -9089,7 +9090,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:8">
       <c r="A313">
         <v>3</v>
       </c>
@@ -9112,7 +9113,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="314" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8" hidden="1">
       <c r="A314">
         <v>2</v>
       </c>
@@ -9135,7 +9136,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="315" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8" hidden="1">
       <c r="A315">
         <v>10.6</v>
       </c>
@@ -9158,7 +9159,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="316" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8" hidden="1">
       <c r="A316">
         <v>4</v>
       </c>
@@ -9181,7 +9182,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="317" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:8" hidden="1">
       <c r="A317">
         <v>2</v>
       </c>
@@ -9204,7 +9205,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="318" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:8" hidden="1">
       <c r="A318">
         <v>5.8</v>
       </c>
@@ -9227,7 +9228,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="319" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:8" hidden="1">
       <c r="A319">
         <v>5</v>
       </c>
@@ -9250,7 +9251,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="320" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:8" hidden="1">
       <c r="A320">
         <v>6.55</v>
       </c>
@@ -9273,7 +9274,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="321" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:8" hidden="1">
       <c r="A321">
         <v>2.8</v>
       </c>
@@ -9296,7 +9297,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="322" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8" hidden="1">
       <c r="A322">
         <v>3.8</v>
       </c>
@@ -9319,7 +9320,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="323" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" hidden="1">
       <c r="A323">
         <v>9</v>
       </c>
@@ -9342,7 +9343,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="324" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8" hidden="1">
       <c r="A324">
         <v>8</v>
       </c>
@@ -9365,7 +9366,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="325" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8" hidden="1">
       <c r="A325">
         <v>1.5</v>
       </c>
@@ -9388,7 +9389,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="326" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:8" hidden="1">
       <c r="A326">
         <v>5</v>
       </c>
@@ -9411,7 +9412,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="327" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" hidden="1">
       <c r="A327">
         <v>4.5999999999999996</v>
       </c>
@@ -9434,7 +9435,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="328" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:8" hidden="1">
       <c r="A328">
         <v>0.5</v>
       </c>
@@ -9457,7 +9458,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="329" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:8" hidden="1">
       <c r="A329">
         <v>2.95</v>
       </c>
@@ -9480,7 +9481,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="330" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:8" hidden="1">
       <c r="A330">
         <v>3.8</v>
       </c>
@@ -9503,7 +9504,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="331" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" hidden="1">
       <c r="A331">
         <v>10</v>
       </c>
@@ -9526,7 +9527,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="332" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:8" hidden="1">
       <c r="A332">
         <v>3.85</v>
       </c>
@@ -9549,7 +9550,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="333" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" hidden="1">
       <c r="A333">
         <v>1.2</v>
       </c>
@@ -9572,7 +9573,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="334" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:8" hidden="1">
       <c r="A334">
         <v>2</v>
       </c>
@@ -9595,7 +9596,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="335" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8" hidden="1">
       <c r="A335">
         <v>8.5</v>
       </c>
@@ -9618,7 +9619,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="336" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:8">
       <c r="A336">
         <v>4.9000000000000004</v>
       </c>
@@ -9641,7 +9642,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="337" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:8" hidden="1">
       <c r="A337">
         <v>10</v>
       </c>
@@ -9664,7 +9665,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="338" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:8" hidden="1">
       <c r="A338">
         <v>1.5</v>
       </c>
@@ -9684,7 +9685,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="339" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8" hidden="1">
       <c r="A339">
         <v>350</v>
       </c>
@@ -9707,7 +9708,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="340" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:8" hidden="1">
       <c r="A340">
         <v>4.4000000000000004</v>
       </c>
@@ -9730,7 +9731,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="341" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:8" hidden="1">
       <c r="A341">
         <v>3.2</v>
       </c>
@@ -9753,7 +9754,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="342" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8" hidden="1">
       <c r="A342">
         <v>3.8</v>
       </c>
@@ -9776,7 +9777,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="343" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:8" hidden="1">
       <c r="A343">
         <v>0.9</v>
       </c>
@@ -9799,7 +9800,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="344" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:8">
       <c r="A344">
         <v>6</v>
       </c>
@@ -9822,7 +9823,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="345" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8" hidden="1">
       <c r="A345">
         <v>3.8</v>
       </c>
@@ -9845,7 +9846,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="346" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:8" hidden="1">
       <c r="A346">
         <v>2</v>
       </c>
@@ -9868,7 +9869,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="347" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:8" hidden="1">
       <c r="A347">
         <v>5.5</v>
       </c>
@@ -9891,7 +9892,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="348" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:8" hidden="1">
       <c r="A348">
         <v>43.22</v>
       </c>
@@ -9914,7 +9915,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="349" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:8" hidden="1">
       <c r="A349">
         <v>2</v>
       </c>
@@ -9937,7 +9938,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="350" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:8" hidden="1">
       <c r="A350">
         <v>7</v>
       </c>
@@ -9960,7 +9961,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="351" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:8" hidden="1">
       <c r="A351">
         <v>1.61</v>
       </c>
@@ -9983,7 +9984,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="352" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:8" hidden="1">
       <c r="A352">
         <v>20</v>
       </c>
@@ -10006,7 +10007,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="353" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:12" hidden="1">
       <c r="A353">
         <v>14.84</v>
       </c>
@@ -10029,7 +10030,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="354" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:12" hidden="1">
       <c r="A354">
         <v>5.6</v>
       </c>
@@ -10052,7 +10053,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="355" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:12" hidden="1">
       <c r="A355">
         <v>6.8</v>
       </c>
@@ -10075,7 +10076,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="356" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:12" hidden="1">
       <c r="A356">
         <v>7.7</v>
       </c>
@@ -10098,7 +10099,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="357" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:12" hidden="1">
       <c r="A357">
         <v>29.4</v>
       </c>
@@ -10121,7 +10122,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="358" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:12" hidden="1">
       <c r="A358">
         <v>0.5</v>
       </c>
@@ -10144,7 +10145,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="359" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:12" hidden="1">
       <c r="A359">
         <v>2.2000000000000002</v>
       </c>
@@ -10167,7 +10168,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="360" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:12" hidden="1">
       <c r="A360">
         <v>3.5</v>
       </c>
@@ -10190,7 +10191,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="361" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:12" hidden="1">
       <c r="A361">
         <v>4.4000000000000004</v>
       </c>
@@ -10213,7 +10214,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="362" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:12" hidden="1">
       <c r="A362">
         <v>5.7</v>
       </c>
@@ -10236,7 +10237,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="363" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:12" hidden="1">
       <c r="A363">
         <v>7.74</v>
       </c>
@@ -10259,7 +10260,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="364" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:12" hidden="1">
       <c r="A364">
         <v>7</v>
       </c>
@@ -10282,7 +10283,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="365" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:12" hidden="1">
       <c r="A365">
         <v>3.8</v>
       </c>
@@ -10305,7 +10306,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="366" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:12" hidden="1">
       <c r="A366">
         <v>100</v>
       </c>
@@ -10328,7 +10329,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="367" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:12" hidden="1">
       <c r="A367" s="1">
         <v>5</v>
       </c>
@@ -10352,7 +10353,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="368" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:12" hidden="1">
       <c r="A368" s="6">
         <v>2</v>
       </c>
@@ -10379,7 +10380,7 @@
       <c r="K368" s="1"/>
       <c r="L368" s="1"/>
     </row>
-    <row r="369" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:8">
       <c r="A369">
         <v>7</v>
       </c>
@@ -10402,7 +10403,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="370" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:8" hidden="1">
       <c r="A370">
         <v>50</v>
       </c>
@@ -10425,7 +10426,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="371" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:8" hidden="1">
       <c r="A371">
         <v>10</v>
       </c>
@@ -10448,7 +10449,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="372" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:8">
       <c r="A372">
         <v>10.8</v>
       </c>
@@ -10471,7 +10472,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="373" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:8" hidden="1">
       <c r="A373">
         <v>10.5</v>
       </c>
@@ -10494,7 +10495,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="374" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:8" hidden="1">
       <c r="A374">
         <v>5.5</v>
       </c>
@@ -10517,7 +10518,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="375" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:8" hidden="1">
       <c r="A375">
         <v>5</v>
       </c>
@@ -10540,7 +10541,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="376" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:8" hidden="1">
       <c r="A376">
         <v>0.5</v>
       </c>
@@ -10563,7 +10564,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="377" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:8" hidden="1">
       <c r="A377">
         <v>10.5</v>
       </c>
@@ -10586,7 +10587,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="378" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:8" hidden="1">
       <c r="A378">
         <v>14</v>
       </c>
@@ -10609,7 +10610,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="379" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:8" hidden="1">
       <c r="A379">
         <v>2</v>
       </c>
@@ -10632,7 +10633,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="380" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:8" hidden="1">
       <c r="A380">
         <v>3.5</v>
       </c>
@@ -10655,7 +10656,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="381" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:8" hidden="1">
       <c r="A381">
         <v>3.5</v>
       </c>
@@ -10678,7 +10679,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="382" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:8" hidden="1">
       <c r="A382">
         <v>3.5</v>
       </c>
@@ -10701,7 +10702,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="383" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:8" hidden="1">
       <c r="A383">
         <v>2</v>
       </c>
@@ -10724,7 +10725,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="384" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:8" hidden="1">
       <c r="A384">
         <v>2</v>
       </c>
@@ -10747,7 +10748,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="385" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:8" hidden="1">
       <c r="A385">
         <v>2.5</v>
       </c>
@@ -10770,7 +10771,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="386" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:8" hidden="1">
       <c r="A386">
         <v>6.5</v>
       </c>
@@ -10793,7 +10794,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="387" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:8" hidden="1">
       <c r="A387">
         <v>3.78</v>
       </c>
@@ -10816,7 +10817,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="388" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:8" hidden="1">
       <c r="A388">
         <v>7</v>
       </c>
@@ -10839,7 +10840,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="389" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:8" hidden="1">
       <c r="A389">
         <v>2.5</v>
       </c>
@@ -10862,7 +10863,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="390" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:8" hidden="1">
       <c r="A390">
         <v>2</v>
       </c>
@@ -10885,7 +10886,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="391" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:8" hidden="1">
       <c r="A391">
         <v>1</v>
       </c>
@@ -10908,7 +10909,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="392" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:8" hidden="1">
       <c r="A392">
         <v>10.5</v>
       </c>
@@ -10931,7 +10932,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="393" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:8" hidden="1">
       <c r="A393">
         <v>1.5</v>
       </c>
@@ -10954,7 +10955,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="394" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:8" hidden="1">
       <c r="A394">
         <v>2.7</v>
       </c>
@@ -10977,7 +10978,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="395" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:8" hidden="1">
       <c r="A395">
         <v>2</v>
       </c>
@@ -11000,7 +11001,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="396" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:8" hidden="1">
       <c r="A396">
         <v>17.5</v>
       </c>
@@ -11023,7 +11024,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="397" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:8">
       <c r="A397">
         <v>43</v>
       </c>
@@ -11046,7 +11047,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="398" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:8" hidden="1">
       <c r="A398">
         <v>69.900000000000006</v>
       </c>
@@ -11069,7 +11070,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="399" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:8" hidden="1">
       <c r="A399">
         <v>16</v>
       </c>
@@ -11092,7 +11093,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="400" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:8" hidden="1">
       <c r="A400">
         <v>2.2000000000000002</v>
       </c>
@@ -11115,7 +11116,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="401" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:8" hidden="1">
       <c r="A401">
         <v>1.72</v>
       </c>
@@ -11138,7 +11139,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="402" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:8" hidden="1">
       <c r="A402">
         <v>6</v>
       </c>
@@ -11161,7 +11162,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="403" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:8" hidden="1">
       <c r="A403">
         <v>1.8</v>
       </c>
@@ -11184,7 +11185,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="404" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:8" hidden="1">
       <c r="A404">
         <v>4.5999999999999996</v>
       </c>
@@ -11207,7 +11208,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="405" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:8" hidden="1">
       <c r="A405">
         <v>27</v>
       </c>
@@ -11230,7 +11231,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="406" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:8" hidden="1">
       <c r="A406">
         <v>14</v>
       </c>
@@ -11253,7 +11254,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="407" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:8" hidden="1">
       <c r="A407">
         <v>2.5</v>
       </c>
@@ -11276,7 +11277,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="408" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:8" hidden="1">
       <c r="A408">
         <v>10</v>
       </c>
@@ -11299,7 +11300,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="409" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:8" hidden="1">
       <c r="A409">
         <v>11</v>
       </c>
@@ -11322,7 +11323,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="410" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:8" hidden="1">
       <c r="A410">
         <v>5.55</v>
       </c>
@@ -11345,7 +11346,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="411" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:8" hidden="1">
       <c r="A411">
         <v>3</v>
       </c>
@@ -11368,7 +11369,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="412" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:8" hidden="1">
       <c r="A412">
         <v>3.5</v>
       </c>
@@ -11391,7 +11392,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="413" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:8" hidden="1">
       <c r="A413">
         <v>3.8</v>
       </c>
@@ -11414,7 +11415,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="414" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:8" hidden="1">
       <c r="A414">
         <v>4</v>
       </c>
@@ -11437,7 +11438,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="415" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:8">
       <c r="A415">
         <v>8</v>
       </c>
@@ -11460,7 +11461,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="416" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:8" hidden="1">
       <c r="A416">
         <v>11.6</v>
       </c>
@@ -11483,7 +11484,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="417" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:8" hidden="1">
       <c r="A417">
         <v>1.6</v>
       </c>
@@ -11506,7 +11507,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="418" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:8" hidden="1">
       <c r="A418">
         <v>44.41</v>
       </c>
@@ -11529,7 +11530,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="419" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:8" hidden="1">
       <c r="A419">
         <v>4.8</v>
       </c>
@@ -11552,7 +11553,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="420" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:8" hidden="1">
       <c r="A420">
         <v>1.7</v>
       </c>
@@ -11575,7 +11576,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="421" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:8" hidden="1">
       <c r="A421">
         <v>2.85</v>
       </c>
@@ -11598,7 +11599,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="422" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:8" hidden="1">
       <c r="A422">
         <v>6.4</v>
       </c>
@@ -11621,7 +11622,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="423" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:8" hidden="1">
       <c r="A423">
         <v>3.5</v>
       </c>
@@ -11644,7 +11645,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="424" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:8" hidden="1">
       <c r="A424">
         <v>6.5</v>
       </c>
@@ -11667,7 +11668,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="425" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:8" hidden="1">
       <c r="A425">
         <v>1.2</v>
       </c>
@@ -11690,7 +11691,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="426" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:8" hidden="1">
       <c r="A426">
         <v>4.5999999999999996</v>
       </c>
@@ -11713,7 +11714,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="427" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:8" hidden="1">
       <c r="A427">
         <v>8</v>
       </c>
@@ -11736,7 +11737,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="428" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:8">
       <c r="A428">
         <v>3.5</v>
       </c>
@@ -11759,7 +11760,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="429" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:8" hidden="1">
       <c r="A429" s="1">
         <v>50</v>
       </c>
@@ -11783,7 +11784,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="430" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:8">
       <c r="A430">
         <v>10</v>
       </c>
@@ -11806,7 +11807,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="431" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:8" hidden="1">
       <c r="A431">
         <v>2.9</v>
       </c>
@@ -11829,7 +11830,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="432" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:8" hidden="1">
       <c r="A432">
         <v>15</v>
       </c>
@@ -11852,7 +11853,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="433" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:8">
       <c r="A433">
         <v>3.5</v>
       </c>
@@ -11875,7 +11876,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="434" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:8" hidden="1">
       <c r="A434">
         <v>9.25</v>
       </c>
@@ -11898,7 +11899,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="435" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:8" hidden="1">
       <c r="A435">
         <v>8</v>
       </c>
@@ -11921,7 +11922,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="436" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:8" hidden="1">
       <c r="A436">
         <v>4.0999999999999996</v>
       </c>
@@ -11944,7 +11945,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="437" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:8" hidden="1">
       <c r="A437">
         <v>4.9000000000000004</v>
       </c>
@@ -11967,7 +11968,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="438" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:8" hidden="1">
       <c r="A438">
         <v>2.8</v>
       </c>
@@ -11990,7 +11991,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="439" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:8">
       <c r="A439">
         <v>18.7</v>
       </c>
@@ -12013,7 +12014,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="440" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:8" hidden="1">
       <c r="A440">
         <v>20</v>
       </c>
@@ -12036,7 +12037,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="441" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:8" hidden="1">
       <c r="A441" s="1">
         <v>150</v>
       </c>
@@ -12060,7 +12061,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="442" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:8" hidden="1">
       <c r="A442" s="1">
         <v>10</v>
       </c>
@@ -12084,7 +12085,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="443" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:8" hidden="1">
       <c r="A443">
         <v>2.1</v>
       </c>
@@ -12107,7 +12108,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="444" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:8" hidden="1">
       <c r="A444">
         <v>5</v>
       </c>
@@ -12130,7 +12131,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="445" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:8" hidden="1">
       <c r="A445">
         <v>10</v>
       </c>
@@ -12153,7 +12154,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="446" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:8" hidden="1">
       <c r="A446">
         <v>59</v>
       </c>
@@ -12176,7 +12177,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="447" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:8" hidden="1">
       <c r="A447">
         <v>4</v>
       </c>
@@ -12199,7 +12200,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="448" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:8" hidden="1">
       <c r="A448">
         <v>4.17</v>
       </c>
@@ -12222,7 +12223,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="449" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:8" hidden="1">
       <c r="A449">
         <v>4.2</v>
       </c>
@@ -12245,7 +12246,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="450" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:8" hidden="1">
       <c r="A450">
         <v>4.4000000000000004</v>
       </c>
@@ -12268,7 +12269,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="451" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:8" hidden="1">
       <c r="A451">
         <v>30</v>
       </c>
@@ -12291,7 +12292,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="452" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:8" hidden="1">
       <c r="A452">
         <v>5</v>
       </c>
@@ -12314,7 +12315,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="453" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:8" hidden="1">
       <c r="A453">
         <v>15.7</v>
       </c>
@@ -12337,7 +12338,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="454" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:8" hidden="1">
       <c r="A454">
         <v>4</v>
       </c>
@@ -12360,7 +12361,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="455" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:8" hidden="1">
       <c r="A455">
         <v>8</v>
       </c>
@@ -12383,7 +12384,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="456" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:8">
       <c r="A456">
         <v>3.5</v>
       </c>
@@ -12406,7 +12407,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="457" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:8" hidden="1">
       <c r="A457">
         <v>4.2</v>
       </c>
@@ -12429,7 +12430,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="458" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:8" hidden="1">
       <c r="A458">
         <v>180</v>
       </c>
@@ -12452,7 +12453,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="459" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:8" hidden="1">
       <c r="A459">
         <v>2.2999999999999998</v>
       </c>
@@ -12475,7 +12476,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="460" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:8" hidden="1">
       <c r="A460">
         <v>11</v>
       </c>
@@ -12498,7 +12499,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="461" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:8" hidden="1">
       <c r="A461">
         <v>2</v>
       </c>
@@ -12521,7 +12522,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="462" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:8" hidden="1">
       <c r="A462">
         <v>3</v>
       </c>
@@ -12544,7 +12545,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="463" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:8" hidden="1">
       <c r="A463">
         <v>6.4</v>
       </c>
@@ -12567,7 +12568,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="464" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:8" hidden="1">
       <c r="A464">
         <v>3.2</v>
       </c>
@@ -12590,7 +12591,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="465" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:8" hidden="1">
       <c r="A465">
         <v>1</v>
       </c>
@@ -12613,7 +12614,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="466" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:8" hidden="1">
       <c r="A466">
         <v>4.2</v>
       </c>
@@ -12636,7 +12637,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="467" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:8" hidden="1">
       <c r="A467">
         <v>14</v>
       </c>
@@ -12659,7 +12660,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="468" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:8" hidden="1">
       <c r="A468">
         <v>2.9</v>
       </c>
@@ -12682,7 +12683,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="469" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:8" hidden="1">
       <c r="A469">
         <v>4</v>
       </c>
@@ -12705,7 +12706,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="470" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:8" hidden="1">
       <c r="A470">
         <v>1.8</v>
       </c>
@@ -12728,7 +12729,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="471" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:8" hidden="1">
       <c r="A471">
         <v>18</v>
       </c>
@@ -12751,7 +12752,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="472" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:8" hidden="1">
       <c r="A472">
         <v>2</v>
       </c>
@@ -12774,7 +12775,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="473" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:8" hidden="1">
       <c r="A473">
         <v>3</v>
       </c>
@@ -12797,7 +12798,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="474" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:8" hidden="1">
       <c r="A474">
         <v>10</v>
       </c>
@@ -12820,7 +12821,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="475" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:8" hidden="1">
       <c r="A475">
         <v>8.3000000000000007</v>
       </c>
@@ -12843,7 +12844,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="476" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:8" hidden="1">
       <c r="A476">
         <v>362</v>
       </c>
@@ -12866,7 +12867,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="477" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:8" hidden="1">
       <c r="A477">
         <v>4.2</v>
       </c>
@@ -12889,7 +12890,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="478" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:8" hidden="1">
       <c r="A478">
         <v>0.5</v>
       </c>
@@ -12912,7 +12913,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="479" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:8" hidden="1">
       <c r="A479">
         <v>1.7</v>
       </c>
@@ -12935,7 +12936,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="480" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:8" hidden="1">
       <c r="A480">
         <v>4.5999999999999996</v>
       </c>
@@ -12958,7 +12959,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="481" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:8" hidden="1">
       <c r="A481">
         <v>4.7</v>
       </c>
@@ -12981,7 +12982,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="482" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:8" hidden="1">
       <c r="A482">
         <v>1</v>
       </c>
@@ -13004,7 +13005,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="483" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:8" hidden="1">
       <c r="A483">
         <v>5.6</v>
       </c>
@@ -13027,7 +13028,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="484" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:8" hidden="1">
       <c r="A484">
         <v>33.799999999999997</v>
       </c>
@@ -13050,7 +13051,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="485" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:8">
       <c r="A485">
         <v>8</v>
       </c>
@@ -13073,7 +13074,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="486" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:8" hidden="1">
       <c r="A486">
         <v>5.2</v>
       </c>
@@ -13096,7 +13097,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="487" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:8" hidden="1">
       <c r="A487">
         <v>5.4</v>
       </c>
@@ -13119,7 +13120,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="488" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:8" hidden="1">
       <c r="A488">
         <v>40</v>
       </c>
@@ -13142,7 +13143,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="489" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:8" hidden="1">
       <c r="A489">
         <v>10.8</v>
       </c>
@@ -13165,7 +13166,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="490" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:8">
       <c r="A490">
         <v>15</v>
       </c>
@@ -13188,7 +13189,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="491" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:8">
       <c r="A491">
         <v>20</v>
       </c>
@@ -13211,7 +13212,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="492" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:8" hidden="1">
       <c r="A492">
         <v>3</v>
       </c>
@@ -13234,7 +13235,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="493" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:8" hidden="1">
       <c r="A493">
         <v>3.5</v>
       </c>
@@ -13257,7 +13258,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="494" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:8" hidden="1">
       <c r="A494">
         <v>2</v>
       </c>
@@ -13280,7 +13281,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="495" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:8" hidden="1">
       <c r="A495">
         <v>4.2</v>
       </c>
@@ -13303,7 +13304,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="496" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:8" hidden="1">
       <c r="A496">
         <v>5</v>
       </c>
@@ -13326,14 +13327,14 @@
         <v>250</v>
       </c>
     </row>
-    <row r="497" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="498" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="499" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="500" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="501" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="502" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="503" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="504" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:8" hidden="1"/>
+    <row r="498" spans="1:8" hidden="1"/>
+    <row r="499" spans="1:8" hidden="1"/>
+    <row r="500" spans="1:8" hidden="1"/>
+    <row r="501" spans="1:8" hidden="1"/>
+    <row r="502" spans="1:8" hidden="1"/>
+    <row r="503" spans="1:8" hidden="1"/>
+    <row r="504" spans="1:8" hidden="1">
       <c r="A504" s="1"/>
       <c r="B504" s="1"/>
       <c r="C504" s="1"/>
@@ -13343,7 +13344,7 @@
       <c r="G504" s="1"/>
       <c r="H504" s="1"/>
     </row>
-    <row r="505" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:8">
       <c r="A505">
         <v>2.2000000000000002</v>
       </c>
@@ -13366,7 +13367,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="506" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:8">
       <c r="A506">
         <v>4.5</v>
       </c>
@@ -13389,7 +13390,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="507" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:8">
       <c r="A507" s="1">
         <v>27.69</v>
       </c>
@@ -13413,7 +13414,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="508" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:8">
       <c r="A508">
         <v>70</v>
       </c>
@@ -13436,7 +13437,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="509" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:8">
       <c r="A509" s="1">
         <v>2.2999999999999998</v>
       </c>
@@ -13460,28 +13461,61 @@
         <v>250</v>
       </c>
     </row>
-    <row r="510" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:8">
       <c r="A510">
-        <v>3.6</v>
+        <v>3.2</v>
       </c>
       <c r="B510" t="s">
-        <v>223</v>
+        <v>344</v>
       </c>
       <c r="C510" s="2">
         <v>43383</v>
       </c>
       <c r="D510" t="s">
-        <v>319</v>
+        <v>495</v>
       </c>
       <c r="E510" t="s">
         <v>238</v>
       </c>
       <c r="F510">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H510" t="s">
         <v>250</v>
       </c>
+    </row>
+    <row r="511" spans="1:8">
+      <c r="A511">
+        <v>3.6</v>
+      </c>
+      <c r="B511" t="s">
+        <v>223</v>
+      </c>
+      <c r="C511" s="2">
+        <v>43383</v>
+      </c>
+      <c r="D511" t="s">
+        <v>319</v>
+      </c>
+      <c r="E511" t="s">
+        <v>238</v>
+      </c>
+      <c r="F511">
+        <v>4</v>
+      </c>
+      <c r="H511" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="514" spans="1:8">
+      <c r="A514" s="1"/>
+      <c r="B514" s="1"/>
+      <c r="C514" s="1"/>
+      <c r="D514" s="1"/>
+      <c r="E514" s="1"/>
+      <c r="F514" s="1"/>
+      <c r="G514" s="1"/>
+      <c r="H514" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ela na ksekatharizoyn oi malakies
</commit_message>
<xml_diff>
--- a/costs.xlsx
+++ b/costs.xlsx
@@ -1677,14 +1677,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Πίνακας1" displayName="Πίνακας1" ref="A1:H533" totalsRowShown="0">
-  <autoFilter ref="A1:H533">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="transport"/>
-        <filter val="travel-holidays"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H533"/>
   <tableColumns count="8">
     <tableColumn id="1" name="amount" totalsRowDxfId="7"/>
     <tableColumn id="11" name="type" totalsRowDxfId="6"/>
@@ -1988,13 +1981,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L527"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A517" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E527" sqref="E527"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.7109375" bestFit="1" customWidth="1"/>
@@ -2037,7 +2030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>489</v>
       </c>
@@ -2063,7 +2056,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>20</v>
       </c>
@@ -2087,7 +2080,7 @@
       </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>10</v>
       </c>
@@ -2110,7 +2103,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>100</v>
       </c>
@@ -2133,7 +2126,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>10</v>
       </c>
@@ -2156,7 +2149,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>50</v>
       </c>
@@ -2179,7 +2172,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>3.2</v>
       </c>
@@ -2202,7 +2195,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>1.3</v>
       </c>
@@ -2225,7 +2218,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1.2</v>
       </c>
@@ -2248,7 +2241,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>5</v>
       </c>
@@ -2271,7 +2264,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>4.5</v>
       </c>
@@ -2294,7 +2287,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>4</v>
       </c>
@@ -2317,7 +2310,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>10.6</v>
       </c>
@@ -2340,7 +2333,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>1.8</v>
       </c>
@@ -2386,7 +2379,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>18</v>
       </c>
@@ -2409,7 +2402,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>1.5</v>
       </c>
@@ -2432,7 +2425,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>7.8</v>
       </c>
@@ -2455,7 +2448,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>4.4400000000000004</v>
       </c>
@@ -2478,7 +2471,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>1.5</v>
       </c>
@@ -2501,7 +2494,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>8.84</v>
       </c>
@@ -2524,7 +2517,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>4</v>
       </c>
@@ -2547,7 +2540,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>10</v>
       </c>
@@ -2570,7 +2563,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>1.8</v>
       </c>
@@ -2593,7 +2586,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>11.8</v>
       </c>
@@ -2616,7 +2609,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>40</v>
       </c>
@@ -2639,7 +2632,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>2.9</v>
       </c>
@@ -2662,7 +2655,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>4.3</v>
       </c>
@@ -2685,7 +2678,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>3.35</v>
       </c>
@@ -2708,7 +2701,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>5.2</v>
       </c>
@@ -2731,7 +2724,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>15</v>
       </c>
@@ -2754,7 +2747,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>3.9</v>
       </c>
@@ -2777,7 +2770,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>63.45</v>
       </c>
@@ -2800,7 +2793,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>49.9</v>
       </c>
@@ -2820,7 +2813,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>140</v>
       </c>
@@ -2843,7 +2836,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>1.8</v>
       </c>
@@ -2866,7 +2859,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>13.02</v>
       </c>
@@ -2889,7 +2882,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>4.7</v>
       </c>
@@ -2912,7 +2905,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>15.96</v>
       </c>
@@ -2935,7 +2928,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>9.8000000000000007</v>
       </c>
@@ -2958,7 +2951,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>79.8</v>
       </c>
@@ -2981,7 +2974,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>11.9</v>
       </c>
@@ -3004,7 +2997,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>38.880000000000003</v>
       </c>
@@ -3027,7 +3020,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>7.75</v>
       </c>
@@ -3050,7 +3043,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>0.79</v>
       </c>
@@ -3096,7 +3089,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3119,7 +3112,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3142,7 +3135,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>1.8</v>
       </c>
@@ -3188,7 +3181,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>24</v>
       </c>
@@ -3234,7 +3227,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>3.5</v>
       </c>
@@ -3257,7 +3250,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>5.6</v>
       </c>
@@ -3281,7 +3274,7 @@
       </c>
       <c r="K55" s="4"/>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>1.5</v>
       </c>
@@ -3304,7 +3297,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>3</v>
       </c>
@@ -3350,7 +3343,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>8</v>
       </c>
@@ -3419,7 +3412,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3442,7 +3435,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>1.5</v>
       </c>
@@ -3465,7 +3458,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3557,7 +3550,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>3.5</v>
       </c>
@@ -3581,7 +3574,7 @@
       </c>
       <c r="K68" s="4"/>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>4.0999999999999996</v>
       </c>
@@ -3650,7 +3643,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>4.5</v>
       </c>
@@ -3673,7 +3666,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>10</v>
       </c>
@@ -3696,7 +3689,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>18.8</v>
       </c>
@@ -3719,7 +3712,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>1.8</v>
       </c>
@@ -3743,7 +3736,7 @@
       </c>
       <c r="K75" s="4"/>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>5.5</v>
       </c>
@@ -3766,7 +3759,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -3789,7 +3782,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>3</v>
       </c>
@@ -3812,7 +3805,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>2</v>
       </c>
@@ -3835,7 +3828,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>9.9</v>
       </c>
@@ -3858,7 +3851,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>6.5</v>
       </c>
@@ -3881,7 +3874,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>79.8</v>
       </c>
@@ -3904,7 +3897,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>10</v>
       </c>
@@ -3927,7 +3920,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>2.5</v>
       </c>
@@ -3950,7 +3943,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>5</v>
       </c>
@@ -3973,7 +3966,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>1.6</v>
       </c>
@@ -3996,7 +3989,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>5.5</v>
       </c>
@@ -4019,7 +4012,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>0.8</v>
       </c>
@@ -4042,7 +4035,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>17</v>
       </c>
@@ -4065,7 +4058,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>24.9</v>
       </c>
@@ -4088,7 +4081,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>1.8</v>
       </c>
@@ -4111,7 +4104,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>44.99</v>
       </c>
@@ -4157,7 +4150,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>5</v>
       </c>
@@ -4180,7 +4173,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>5</v>
       </c>
@@ -4203,13 +4196,13 @@
         <v>267</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
     </row>
-    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
     </row>
-    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -4232,7 +4225,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>3</v>
       </c>
@@ -4255,7 +4248,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>6</v>
       </c>
@@ -4278,7 +4271,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>3.5</v>
       </c>
@@ -4301,7 +4294,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>34.9</v>
       </c>
@@ -4324,7 +4317,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>12</v>
       </c>
@@ -4347,10 +4340,10 @@
         <v>241</v>
       </c>
     </row>
-    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
     </row>
-    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>5</v>
       </c>
@@ -4373,7 +4366,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>6.9</v>
       </c>
@@ -4396,7 +4389,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>6.04</v>
       </c>
@@ -4419,7 +4412,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>4.8</v>
       </c>
@@ -4442,7 +4435,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>9.6999999999999993</v>
       </c>
@@ -4465,7 +4458,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>5.5</v>
       </c>
@@ -4488,7 +4481,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>7</v>
       </c>
@@ -4511,7 +4504,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>1</v>
       </c>
@@ -4534,7 +4527,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>4</v>
       </c>
@@ -4557,7 +4550,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>4.0999999999999996</v>
       </c>
@@ -4580,7 +4573,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>2.3199999999999998</v>
       </c>
@@ -4603,7 +4596,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>8</v>
       </c>
@@ -4626,7 +4619,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>12.5</v>
       </c>
@@ -4649,7 +4642,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>0.7</v>
       </c>
@@ -4695,7 +4688,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>8</v>
       </c>
@@ -4718,7 +4711,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -4741,7 +4734,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>8</v>
       </c>
@@ -4764,7 +4757,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="123" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>4.5</v>
       </c>
@@ -4787,7 +4780,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="124" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>2.5</v>
       </c>
@@ -4833,7 +4826,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="126" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>2</v>
       </c>
@@ -4856,7 +4849,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="127" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>16</v>
       </c>
@@ -4879,7 +4872,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="128" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>6</v>
       </c>
@@ -4902,7 +4895,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>5</v>
       </c>
@@ -4925,7 +4918,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>6.52</v>
       </c>
@@ -4948,7 +4941,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>1.8</v>
       </c>
@@ -4971,7 +4964,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>1</v>
       </c>
@@ -5040,7 +5033,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>10</v>
       </c>
@@ -5063,7 +5056,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>2.97</v>
       </c>
@@ -5086,7 +5079,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>10</v>
       </c>
@@ -5109,7 +5102,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>1.6</v>
       </c>
@@ -5132,7 +5125,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>1.5</v>
       </c>
@@ -5155,7 +5148,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>1.8</v>
       </c>
@@ -5178,7 +5171,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>7.3</v>
       </c>
@@ -5201,7 +5194,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <v>4</v>
       </c>
@@ -5224,7 +5217,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>2.1</v>
       </c>
@@ -5247,7 +5240,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>4.2</v>
       </c>
@@ -5270,7 +5263,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <v>9</v>
       </c>
@@ -5293,7 +5286,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>1</v>
       </c>
@@ -5316,7 +5309,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>3.5</v>
       </c>
@@ -5339,7 +5332,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -5362,7 +5355,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>3</v>
       </c>
@@ -5385,7 +5378,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>2</v>
       </c>
@@ -5408,7 +5401,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
         <v>150</v>
       </c>
@@ -5431,7 +5424,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>7</v>
       </c>
@@ -5454,7 +5447,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
         <v>5</v>
       </c>
@@ -5477,7 +5470,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="4">
         <v>8</v>
       </c>
@@ -5523,7 +5516,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="4">
         <v>55</v>
       </c>
@@ -5546,7 +5539,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="4">
         <v>0.6</v>
       </c>
@@ -5569,7 +5562,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="4">
         <v>4</v>
       </c>
@@ -5592,7 +5585,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="4">
         <v>39.9</v>
       </c>
@@ -5615,7 +5608,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="4">
         <v>1.6</v>
       </c>
@@ -5638,7 +5631,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>80</v>
       </c>
@@ -5661,7 +5654,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="4">
         <v>6.2</v>
       </c>
@@ -5684,7 +5677,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="4">
         <v>15</v>
       </c>
@@ -5707,7 +5700,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="4">
         <v>4.3</v>
       </c>
@@ -5730,7 +5723,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="4">
         <v>9.6999999999999993</v>
       </c>
@@ -5753,7 +5746,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="4">
         <v>2.4500000000000002</v>
       </c>
@@ -5776,7 +5769,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="4">
         <v>1.96</v>
       </c>
@@ -5799,7 +5792,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="4">
         <v>11.5</v>
       </c>
@@ -5822,7 +5815,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="4">
         <v>2.7</v>
       </c>
@@ -5845,7 +5838,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="4">
         <v>2.7</v>
       </c>
@@ -5868,7 +5861,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="4">
         <v>7</v>
       </c>
@@ -5891,7 +5884,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
         <v>4.8</v>
       </c>
@@ -5914,7 +5907,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="4">
         <v>4.4000000000000004</v>
       </c>
@@ -5937,7 +5930,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
         <v>3.8</v>
       </c>
@@ -5960,7 +5953,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="4">
         <v>1.5</v>
       </c>
@@ -5983,7 +5976,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
         <v>11.5</v>
       </c>
@@ -6006,7 +5999,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
         <v>4.4000000000000004</v>
       </c>
@@ -6029,7 +6022,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
         <v>6.5</v>
       </c>
@@ -6052,7 +6045,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="4">
         <v>6.5</v>
       </c>
@@ -6075,7 +6068,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="4">
         <v>5</v>
       </c>
@@ -6098,7 +6091,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="4">
         <v>6</v>
       </c>
@@ -6144,7 +6137,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="4">
         <v>3.2</v>
       </c>
@@ -6167,7 +6160,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="4">
         <v>10</v>
       </c>
@@ -6190,7 +6183,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="4">
         <v>3</v>
       </c>
@@ -6213,7 +6206,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="4">
         <v>10</v>
       </c>
@@ -6236,7 +6229,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="4">
         <v>3.5</v>
       </c>
@@ -6259,7 +6252,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="4">
         <v>10</v>
       </c>
@@ -6282,7 +6275,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="4">
         <v>8</v>
       </c>
@@ -6328,7 +6321,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="4">
         <v>2</v>
       </c>
@@ -6351,7 +6344,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="4">
         <v>10</v>
       </c>
@@ -6374,7 +6367,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="4">
         <v>22</v>
       </c>
@@ -6397,7 +6390,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="4">
         <v>14</v>
       </c>
@@ -6443,7 +6436,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="4">
         <v>4.7</v>
       </c>
@@ -6466,7 +6459,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="4">
         <v>69.900000000000006</v>
       </c>
@@ -6489,7 +6482,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="4">
         <v>8.4</v>
       </c>
@@ -6512,7 +6505,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="4">
         <v>5</v>
       </c>
@@ -6535,7 +6528,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="4">
         <v>4.5</v>
       </c>
@@ -6558,7 +6551,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
         <v>6</v>
       </c>
@@ -6581,7 +6574,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="4">
         <v>5.46</v>
       </c>
@@ -6604,7 +6597,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="4">
         <v>78.849999999999994</v>
       </c>
@@ -6627,7 +6620,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="4">
         <v>10</v>
       </c>
@@ -6650,7 +6643,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="4">
         <v>10</v>
       </c>
@@ -6673,7 +6666,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="4">
         <v>26</v>
       </c>
@@ -6696,7 +6689,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="4">
         <v>2</v>
       </c>
@@ -6719,7 +6712,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="4">
         <v>2.5</v>
       </c>
@@ -6742,7 +6735,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="4">
         <v>5.9</v>
       </c>
@@ -6765,7 +6758,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="210" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="4">
         <v>8.6</v>
       </c>
@@ -6788,7 +6781,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="4">
         <v>2.7</v>
       </c>
@@ -6811,7 +6804,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="212" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="4">
         <v>4.8</v>
       </c>
@@ -6834,7 +6827,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="213" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="4">
         <v>2.8</v>
       </c>
@@ -6857,7 +6850,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="4">
         <v>2</v>
       </c>
@@ -6880,7 +6873,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="215" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="4">
         <v>5</v>
       </c>
@@ -6903,7 +6896,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="216" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="4">
         <v>2.5</v>
       </c>
@@ -6949,7 +6942,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="218" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="4">
         <v>1.8</v>
       </c>
@@ -6972,7 +6965,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="219" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="4">
         <v>4</v>
       </c>
@@ -6995,7 +6988,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="220" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="4">
         <v>6</v>
       </c>
@@ -7018,7 +7011,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="221" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="4">
         <v>1.8</v>
       </c>
@@ -7064,7 +7057,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="223" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="4">
         <v>5</v>
       </c>
@@ -7087,7 +7080,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="224" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="4">
         <v>4.7</v>
       </c>
@@ -7110,7 +7103,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="4">
         <v>5</v>
       </c>
@@ -7133,7 +7126,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="226" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="4">
         <v>10</v>
       </c>
@@ -7156,7 +7149,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="4">
         <v>1.5</v>
       </c>
@@ -7202,7 +7195,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="4">
         <v>7</v>
       </c>
@@ -7225,7 +7218,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="230" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="4">
         <v>2.8</v>
       </c>
@@ -7248,7 +7241,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="231" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" s="4">
         <v>1</v>
       </c>
@@ -7271,7 +7264,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="232" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="4">
         <v>4</v>
       </c>
@@ -7294,7 +7287,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="233" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="4">
         <v>50</v>
       </c>
@@ -7317,7 +7310,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="234" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" s="4">
         <v>7.2</v>
       </c>
@@ -7340,7 +7333,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" s="4">
         <v>1</v>
       </c>
@@ -7363,7 +7356,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="236" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="4">
         <v>7</v>
       </c>
@@ -7386,7 +7379,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="237" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="4">
         <v>1.1000000000000001</v>
       </c>
@@ -7432,7 +7425,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" s="4">
         <v>15</v>
       </c>
@@ -7455,7 +7448,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="240" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="4">
         <v>3</v>
       </c>
@@ -7501,7 +7494,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="242" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="4">
         <v>2.1</v>
       </c>
@@ -7524,7 +7517,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="243" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="4">
         <v>150</v>
       </c>
@@ -7547,7 +7540,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="244" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" s="4">
         <v>12.7</v>
       </c>
@@ -7570,7 +7563,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="245" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A245" s="4">
         <v>89.9</v>
       </c>
@@ -7593,7 +7586,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="246" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="4">
         <v>4.4000000000000004</v>
       </c>
@@ -7616,7 +7609,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="247" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A247" s="4">
         <v>4.2</v>
       </c>
@@ -7639,7 +7632,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="248" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="4">
         <v>2.2000000000000002</v>
       </c>
@@ -7662,7 +7655,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="249" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="4">
         <v>5</v>
       </c>
@@ -7685,7 +7678,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="250" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="4">
         <v>5</v>
       </c>
@@ -7708,7 +7701,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="251" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="4">
         <v>3.9</v>
       </c>
@@ -7731,7 +7724,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A252" s="4">
         <v>0.5</v>
       </c>
@@ -7754,7 +7747,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="253" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A253" s="4">
         <v>2.4</v>
       </c>
@@ -7777,7 +7770,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="254" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A254" s="4">
         <v>2</v>
       </c>
@@ -7800,7 +7793,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="255" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A255" s="4">
         <v>4.7</v>
       </c>
@@ -7823,7 +7816,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="256" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A256" s="4">
         <v>5.3</v>
       </c>
@@ -7846,7 +7839,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="257" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" s="4">
         <v>4.2</v>
       </c>
@@ -7869,7 +7862,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="258" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" s="4">
         <v>5</v>
       </c>
@@ -7892,7 +7885,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="259" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" s="4">
         <v>2.5</v>
       </c>
@@ -7915,7 +7908,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="260" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" s="4">
         <v>3.3</v>
       </c>
@@ -7938,7 +7931,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="261" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" s="4">
         <v>5.6</v>
       </c>
@@ -7984,7 +7977,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="263" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" s="4">
         <v>10.199999999999999</v>
       </c>
@@ -8007,7 +8000,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="264" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264" s="4">
         <v>8</v>
       </c>
@@ -8030,7 +8023,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="265" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265" s="4">
         <v>2.1</v>
       </c>
@@ -8053,7 +8046,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="266" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A266" s="4">
         <v>3.7</v>
       </c>
@@ -8076,7 +8069,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="267" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A267" s="4">
         <v>7</v>
       </c>
@@ -8122,7 +8115,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="269" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269" s="4">
         <v>5</v>
       </c>
@@ -8168,7 +8161,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="271" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A271" s="4">
         <v>6</v>
       </c>
@@ -8191,7 +8184,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="272" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A272" s="4">
         <v>0.5</v>
       </c>
@@ -8214,7 +8207,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="273" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" s="4">
         <v>5</v>
       </c>
@@ -8237,7 +8230,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="274" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" s="4">
         <v>11</v>
       </c>
@@ -8260,7 +8253,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="275" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="4">
         <v>8.8000000000000007</v>
       </c>
@@ -8283,7 +8276,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="276" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="4">
         <v>0.5</v>
       </c>
@@ -8329,7 +8322,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="278" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="4">
         <v>10</v>
       </c>
@@ -8352,7 +8345,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="279" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" s="4">
         <v>15</v>
       </c>
@@ -8398,7 +8391,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="281" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281" s="4">
         <v>11.9</v>
       </c>
@@ -8421,7 +8414,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="282" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A282" s="4">
         <v>7</v>
       </c>
@@ -8444,7 +8437,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="283" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283" s="4">
         <v>5.0999999999999996</v>
       </c>
@@ -8467,7 +8460,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="284" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>1.9</v>
       </c>
@@ -8490,7 +8483,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="285" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>119.9</v>
       </c>
@@ -8513,7 +8506,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="286" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>6.3</v>
       </c>
@@ -8536,7 +8529,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="287" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>3.5</v>
       </c>
@@ -8559,7 +8552,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="288" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>1.5</v>
       </c>
@@ -8582,7 +8575,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="289" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>1.9</v>
       </c>
@@ -8605,7 +8598,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="290" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>4.5</v>
       </c>
@@ -8628,7 +8621,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="291" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>6.4</v>
       </c>
@@ -8651,7 +8644,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="292" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>1.9</v>
       </c>
@@ -8674,7 +8667,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="293" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>10.6</v>
       </c>
@@ -8697,7 +8690,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="294" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>4.5</v>
       </c>
@@ -8720,7 +8713,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="295" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>22.2</v>
       </c>
@@ -8743,7 +8736,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="296" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A296" s="6">
         <v>25</v>
       </c>
@@ -8789,7 +8782,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="298" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>4</v>
       </c>
@@ -8812,7 +8805,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="299" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>2.2000000000000002</v>
       </c>
@@ -8835,7 +8828,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="300" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>11.5</v>
       </c>
@@ -8858,7 +8851,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="301" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>6.3</v>
       </c>
@@ -8881,7 +8874,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="302" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>3.6</v>
       </c>
@@ -8927,7 +8920,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="304" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>2</v>
       </c>
@@ -8950,7 +8943,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="305" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>4.5</v>
       </c>
@@ -8973,7 +8966,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="306" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>2.9</v>
       </c>
@@ -8996,7 +8989,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="307" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>3.9</v>
       </c>
@@ -9019,7 +9012,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="308" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>1.7</v>
       </c>
@@ -9042,7 +9035,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="309" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>10</v>
       </c>
@@ -9088,7 +9081,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="311" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>10.050000000000001</v>
       </c>
@@ -9111,7 +9104,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="312" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>5</v>
       </c>
@@ -9157,7 +9150,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="314" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>2</v>
       </c>
@@ -9180,7 +9173,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="315" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>10.6</v>
       </c>
@@ -9203,7 +9196,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="316" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>4</v>
       </c>
@@ -9226,7 +9219,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="317" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>2</v>
       </c>
@@ -9249,7 +9242,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="318" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>5.8</v>
       </c>
@@ -9272,7 +9265,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="319" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>5</v>
       </c>
@@ -9295,7 +9288,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="320" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>6.55</v>
       </c>
@@ -9318,7 +9311,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="321" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>2.8</v>
       </c>
@@ -9341,7 +9334,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="322" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>3.8</v>
       </c>
@@ -9364,7 +9357,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="323" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>9</v>
       </c>
@@ -9387,7 +9380,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="324" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>8</v>
       </c>
@@ -9410,7 +9403,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="325" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>1.5</v>
       </c>
@@ -9433,7 +9426,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="326" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>5</v>
       </c>
@@ -9456,7 +9449,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="327" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>4.5999999999999996</v>
       </c>
@@ -9479,7 +9472,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="328" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>0.5</v>
       </c>
@@ -9502,7 +9495,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="329" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>2.95</v>
       </c>
@@ -9525,7 +9518,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="330" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>3.8</v>
       </c>
@@ -9548,7 +9541,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="331" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>10</v>
       </c>
@@ -9571,7 +9564,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="332" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>3.85</v>
       </c>
@@ -9594,7 +9587,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="333" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>1.2</v>
       </c>
@@ -9617,7 +9610,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="334" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>2</v>
       </c>
@@ -9640,7 +9633,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="335" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>8.5</v>
       </c>
@@ -9686,7 +9679,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="337" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>10</v>
       </c>
@@ -9709,7 +9702,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="338" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>1.5</v>
       </c>
@@ -9729,7 +9722,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="339" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>350</v>
       </c>
@@ -9752,7 +9745,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="340" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>4.4000000000000004</v>
       </c>
@@ -9775,7 +9768,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="341" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>3.2</v>
       </c>
@@ -9798,7 +9791,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="342" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>3.8</v>
       </c>
@@ -9821,7 +9814,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="343" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>0.9</v>
       </c>
@@ -9867,7 +9860,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="345" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>3.8</v>
       </c>
@@ -9890,7 +9883,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="346" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>2</v>
       </c>
@@ -9913,7 +9906,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="347" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>5.5</v>
       </c>
@@ -9936,7 +9929,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="348" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>43.22</v>
       </c>
@@ -9959,7 +9952,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="349" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>2</v>
       </c>
@@ -9982,7 +9975,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="350" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>7</v>
       </c>
@@ -10005,7 +9998,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="351" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>1.61</v>
       </c>
@@ -10028,7 +10021,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="352" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>20</v>
       </c>
@@ -10051,7 +10044,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="353" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>14.84</v>
       </c>
@@ -10074,7 +10067,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="354" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>5.6</v>
       </c>
@@ -10097,7 +10090,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="355" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>6.8</v>
       </c>
@@ -10120,7 +10113,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="356" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>7.7</v>
       </c>
@@ -10143,7 +10136,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="357" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>29.4</v>
       </c>
@@ -10166,7 +10159,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="358" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>0.5</v>
       </c>
@@ -10189,7 +10182,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="359" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>2.2000000000000002</v>
       </c>
@@ -10212,7 +10205,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="360" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>3.5</v>
       </c>
@@ -10235,7 +10228,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="361" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>4.4000000000000004</v>
       </c>
@@ -10258,7 +10251,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="362" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>5.7</v>
       </c>
@@ -10281,7 +10274,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="363" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>7.74</v>
       </c>
@@ -10304,7 +10297,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="364" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>7</v>
       </c>
@@ -10327,7 +10320,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="365" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>3.8</v>
       </c>
@@ -10350,7 +10343,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="366" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>100</v>
       </c>
@@ -10373,7 +10366,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="367" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A367" s="1">
         <v>5</v>
       </c>
@@ -10397,7 +10390,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="368" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A368" s="6">
         <v>2</v>
       </c>
@@ -10447,7 +10440,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="370" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>50</v>
       </c>
@@ -10470,7 +10463,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="371" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>10</v>
       </c>
@@ -10516,7 +10509,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="373" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>10.5</v>
       </c>
@@ -10539,7 +10532,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="374" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>5.5</v>
       </c>
@@ -10562,7 +10555,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="375" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>5</v>
       </c>
@@ -10585,7 +10578,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="376" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>0.5</v>
       </c>
@@ -10608,7 +10601,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="377" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>10.5</v>
       </c>
@@ -10631,7 +10624,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="378" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>14</v>
       </c>
@@ -10654,7 +10647,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="379" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>2</v>
       </c>
@@ -10677,7 +10670,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="380" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>3.5</v>
       </c>
@@ -10700,7 +10693,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="381" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>3.5</v>
       </c>
@@ -10723,7 +10716,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="382" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>3.5</v>
       </c>
@@ -10746,7 +10739,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="383" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>2</v>
       </c>
@@ -10769,7 +10762,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="384" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>2</v>
       </c>
@@ -10792,7 +10785,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="385" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>2.5</v>
       </c>
@@ -10815,7 +10808,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="386" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>6.5</v>
       </c>
@@ -10838,7 +10831,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="387" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>3.78</v>
       </c>
@@ -10861,7 +10854,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="388" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>7</v>
       </c>
@@ -10884,7 +10877,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="389" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>2.5</v>
       </c>
@@ -10907,7 +10900,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="390" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>2</v>
       </c>
@@ -10930,7 +10923,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="391" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>1</v>
       </c>
@@ -10953,7 +10946,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="392" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>10.5</v>
       </c>
@@ -10976,7 +10969,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="393" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>1.5</v>
       </c>
@@ -10999,7 +10992,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="394" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>2.7</v>
       </c>
@@ -11022,7 +11015,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="395" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>2</v>
       </c>
@@ -11045,7 +11038,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="396" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>17.5</v>
       </c>
@@ -11091,7 +11084,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="398" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>69.900000000000006</v>
       </c>
@@ -11114,7 +11107,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="399" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>16</v>
       </c>
@@ -11137,7 +11130,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="400" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>2.2000000000000002</v>
       </c>
@@ -11160,7 +11153,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="401" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>1.72</v>
       </c>
@@ -11183,7 +11176,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="402" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>6</v>
       </c>
@@ -11206,7 +11199,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="403" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>1.8</v>
       </c>
@@ -11229,7 +11222,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="404" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>4.5999999999999996</v>
       </c>
@@ -11252,7 +11245,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="405" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A405">
         <v>27</v>
       </c>
@@ -11275,7 +11268,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="406" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>14</v>
       </c>
@@ -11298,7 +11291,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="407" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>2.5</v>
       </c>
@@ -11321,7 +11314,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="408" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>10</v>
       </c>
@@ -11344,7 +11337,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="409" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>11</v>
       </c>
@@ -11367,7 +11360,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="410" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>5.55</v>
       </c>
@@ -11390,7 +11383,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="411" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>3</v>
       </c>
@@ -11413,7 +11406,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="412" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>3.5</v>
       </c>
@@ -11436,7 +11429,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="413" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>3.8</v>
       </c>
@@ -11459,7 +11452,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="414" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>4</v>
       </c>
@@ -11505,7 +11498,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="416" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A416">
         <v>11.6</v>
       </c>
@@ -11528,7 +11521,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="417" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>1.6</v>
       </c>
@@ -11551,7 +11544,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="418" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A418">
         <v>44.41</v>
       </c>
@@ -11574,7 +11567,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="419" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A419">
         <v>4.8</v>
       </c>
@@ -11597,7 +11590,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="420" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A420">
         <v>1.7</v>
       </c>
@@ -11620,7 +11613,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="421" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A421">
         <v>2.85</v>
       </c>
@@ -11643,7 +11636,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="422" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A422">
         <v>6.4</v>
       </c>
@@ -11666,7 +11659,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="423" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A423">
         <v>3.5</v>
       </c>
@@ -11689,7 +11682,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="424" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A424">
         <v>6.5</v>
       </c>
@@ -11712,7 +11705,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="425" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A425">
         <v>1.2</v>
       </c>
@@ -11735,7 +11728,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="426" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A426">
         <v>4.5999999999999996</v>
       </c>
@@ -11758,7 +11751,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="427" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A427">
         <v>8</v>
       </c>
@@ -11804,7 +11797,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="429" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A429" s="1">
         <v>50</v>
       </c>
@@ -11851,7 +11844,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="431" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A431">
         <v>2.9</v>
       </c>
@@ -11874,7 +11867,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="432" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A432">
         <v>15</v>
       </c>
@@ -11920,7 +11913,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="434" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>9.25</v>
       </c>
@@ -11943,7 +11936,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="435" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>8</v>
       </c>
@@ -11966,7 +11959,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="436" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>4.0999999999999996</v>
       </c>
@@ -11989,7 +11982,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="437" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>4.9000000000000004</v>
       </c>
@@ -12012,7 +12005,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="438" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>2.8</v>
       </c>
@@ -12058,7 +12051,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="440" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>20</v>
       </c>
@@ -12081,7 +12074,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="441" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A441" s="1">
         <v>150</v>
       </c>
@@ -12105,7 +12098,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="442" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A442" s="1">
         <v>10</v>
       </c>
@@ -12129,7 +12122,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="443" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>2.1</v>
       </c>
@@ -12152,7 +12145,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="444" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A444">
         <v>5</v>
       </c>
@@ -12175,7 +12168,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="445" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A445">
         <v>10</v>
       </c>
@@ -12198,7 +12191,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="446" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>59</v>
       </c>
@@ -12221,7 +12214,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="447" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A447">
         <v>4</v>
       </c>
@@ -12244,7 +12237,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="448" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A448">
         <v>4.17</v>
       </c>
@@ -12267,7 +12260,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="449" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A449">
         <v>4.2</v>
       </c>
@@ -12290,7 +12283,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="450" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A450">
         <v>4.4000000000000004</v>
       </c>
@@ -12313,7 +12306,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="451" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A451">
         <v>30</v>
       </c>
@@ -12336,7 +12329,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="452" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A452">
         <v>5</v>
       </c>
@@ -12359,7 +12352,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="453" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A453">
         <v>15.7</v>
       </c>
@@ -12382,7 +12375,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="454" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A454">
         <v>4</v>
       </c>
@@ -12405,7 +12398,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="455" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A455">
         <v>8</v>
       </c>
@@ -12451,7 +12444,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="457" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A457">
         <v>4.2</v>
       </c>
@@ -12474,7 +12467,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="458" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A458">
         <v>180</v>
       </c>
@@ -12497,7 +12490,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="459" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A459">
         <v>2.2999999999999998</v>
       </c>
@@ -12520,7 +12513,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="460" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A460">
         <v>11</v>
       </c>
@@ -12543,7 +12536,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="461" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A461">
         <v>2</v>
       </c>
@@ -12566,7 +12559,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="462" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A462">
         <v>3</v>
       </c>
@@ -12589,7 +12582,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="463" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A463">
         <v>6.4</v>
       </c>
@@ -12612,7 +12605,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="464" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A464">
         <v>3.2</v>
       </c>
@@ -12635,7 +12628,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="465" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A465">
         <v>1</v>
       </c>
@@ -12658,7 +12651,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="466" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A466">
         <v>4.2</v>
       </c>
@@ -12681,7 +12674,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="467" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A467">
         <v>14</v>
       </c>
@@ -12704,7 +12697,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="468" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A468">
         <v>2.9</v>
       </c>
@@ -12727,7 +12720,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="469" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A469">
         <v>4</v>
       </c>
@@ -12750,7 +12743,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="470" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A470">
         <v>1.8</v>
       </c>
@@ -12773,7 +12766,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="471" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A471">
         <v>18</v>
       </c>
@@ -12796,7 +12789,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="472" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A472">
         <v>2</v>
       </c>
@@ -12819,7 +12812,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="473" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A473">
         <v>3</v>
       </c>
@@ -12842,7 +12835,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="474" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A474">
         <v>10</v>
       </c>
@@ -12865,7 +12858,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="475" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A475">
         <v>8.3000000000000007</v>
       </c>
@@ -12888,7 +12881,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="476" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A476">
         <v>362</v>
       </c>
@@ -12911,7 +12904,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="477" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A477">
         <v>4.2</v>
       </c>
@@ -12934,7 +12927,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="478" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A478">
         <v>0.5</v>
       </c>
@@ -12957,7 +12950,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="479" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A479">
         <v>1.7</v>
       </c>
@@ -12980,7 +12973,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="480" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A480">
         <v>4.5999999999999996</v>
       </c>
@@ -13003,7 +12996,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="481" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A481">
         <v>4.7</v>
       </c>
@@ -13026,7 +13019,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="482" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A482">
         <v>1</v>
       </c>
@@ -13049,7 +13042,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="483" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A483">
         <v>5.6</v>
       </c>
@@ -13072,7 +13065,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="484" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A484">
         <v>33.799999999999997</v>
       </c>
@@ -13118,7 +13111,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="486" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A486">
         <v>5.2</v>
       </c>
@@ -13141,7 +13134,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="487" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A487">
         <v>5.4</v>
       </c>
@@ -13164,7 +13157,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="488" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A488">
         <v>40</v>
       </c>
@@ -13187,7 +13180,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="489" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A489">
         <v>10.8</v>
       </c>
@@ -13256,7 +13249,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="492" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A492">
         <v>3</v>
       </c>
@@ -13279,7 +13272,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="493" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A493">
         <v>3.5</v>
       </c>
@@ -13302,7 +13295,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="494" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A494">
         <v>2</v>
       </c>
@@ -13325,7 +13318,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="495" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A495">
         <v>4.2</v>
       </c>
@@ -13348,7 +13341,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="496" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A496">
         <v>5</v>
       </c>
@@ -13371,14 +13364,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="497" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="498" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="499" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="500" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="501" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="502" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="503" spans="1:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="504" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A504" s="1"/>
       <c r="B504" s="1"/>
       <c r="C504" s="1"/>

</xml_diff>